<commit_message>
MOSIP-17570 Added subject in email template
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6836" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6860" uniqueCount="592">
   <si>
     <t>lang_code</t>
   </si>
@@ -1797,6 +1797,12 @@
   </si>
   <si>
     <t>Template for Supervisor Reject SMS</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL_SUBJECT</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email Subject</t>
   </si>
 </sst>
 </file>
@@ -2177,10 +2183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1709"/>
+  <dimension ref="A1:D1715"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1689" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1709" sqref="K1709"/>
+    <sheetView tabSelected="1" topLeftCell="A1693" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1709" sqref="I1709"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26116,6 +26122,90 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1710" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1710" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1710" t="s">
+        <v>590</v>
+      </c>
+      <c r="C1710" t="s">
+        <v>591</v>
+      </c>
+      <c r="D1710" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1711" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1711" t="s">
+        <v>590</v>
+      </c>
+      <c r="C1711" t="s">
+        <v>591</v>
+      </c>
+      <c r="D1711" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1712" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1712" t="s">
+        <v>590</v>
+      </c>
+      <c r="C1712" t="s">
+        <v>591</v>
+      </c>
+      <c r="D1712" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1713" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1713" t="s">
+        <v>590</v>
+      </c>
+      <c r="C1713" t="s">
+        <v>591</v>
+      </c>
+      <c r="D1713" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1714" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1714" t="s">
+        <v>590</v>
+      </c>
+      <c r="C1714" t="s">
+        <v>591</v>
+      </c>
+      <c r="D1714" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1715" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1715" t="s">
+        <v>590</v>
+      </c>
+      <c r="C1715" t="s">
+        <v>591</v>
+      </c>
+      <c r="D1715" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D400"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
MOSIP-17570 added new supervisor rejected templates for SMS and EMAIL
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP-Team\mosip-data\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337574ED-1CFC-4A0F-8051-07E976BC82F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6860" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6932" uniqueCount="628">
   <si>
     <t>lang_code</t>
   </si>
@@ -1894,12 +1893,30 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_SMS</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject SMS</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL_SUBJECT</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email Subject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -2013,7 +2030,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2291,18 +2308,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1715"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1733"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1700" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1716" sqref="C1716"/>
+    <sheetView tabSelected="1" topLeftCell="A1711" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1718" sqref="H1718"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1"/>
+    <col min="4" max="4" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -26315,8 +26332,260 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1716" spans="1:4">
+      <c r="A1716" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1716" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1716" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:4">
+      <c r="A1717" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1717" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1717" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:4">
+      <c r="A1718" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1718" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1718" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1718" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:4">
+      <c r="A1719" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1719" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1719" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1719" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:4">
+      <c r="A1720" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1720" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1720" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:4">
+      <c r="A1721" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1721" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1721" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1721" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:4">
+      <c r="A1722" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1722" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1722" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1722" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:4">
+      <c r="A1723" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1723" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1723" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1723" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:4">
+      <c r="A1724" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1724" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1724" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1724" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:4">
+      <c r="A1725" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1725" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1725" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1725" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:4">
+      <c r="A1726" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1726" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1726" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:4">
+      <c r="A1727" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1727" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1727" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:4">
+      <c r="A1728" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1728" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:4">
+      <c r="A1729" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1729" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:4">
+      <c r="A1730" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1730" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:4">
+      <c r="A1731" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1731" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:4">
+      <c r="A1732" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1732" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1732" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:4">
+      <c r="A1733" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1733" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1733" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D400"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
MOSIP-17570 added supervisor rejected email and sms templates
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP-Team\mosip-data\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0B56CD-AB7B-4BD9-A295-CFCA527DC959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6900" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6972" uniqueCount="648">
   <si>
     <t>lang_code</t>
   </si>
@@ -1954,12 +1953,30 @@
   </si>
   <si>
     <t>Failure sms to download my VID card</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_SMS</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject SMS</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL_SUBJECT</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email Subject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -2073,7 +2090,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2351,11 +2368,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1725"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1712" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1716" sqref="C1716"/>
+    <sheetView tabSelected="1" topLeftCell="A1724" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1730" sqref="F1730"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -26515,8 +26532,260 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1726" spans="1:4">
+      <c r="A1726" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1726" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1726" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:4">
+      <c r="A1727" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1727" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1727" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:4">
+      <c r="A1728" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1728" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:4">
+      <c r="A1729" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1729" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:4">
+      <c r="A1730" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1730" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:4">
+      <c r="A1731" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1731" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:4">
+      <c r="A1732" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1732" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1732" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:4">
+      <c r="A1733" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1733" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1733" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:4">
+      <c r="A1734" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1734" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1734" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1734" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:4">
+      <c r="A1735" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1735" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1735" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:4">
+      <c r="A1736" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1736" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1736" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1736" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:4">
+      <c r="A1737" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1737" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1737" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:4">
+      <c r="A1738" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1738" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1738" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1738" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:4">
+      <c r="A1739" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1739" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1739" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1739" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:4">
+      <c r="A1740" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1740" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1740" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:4">
+      <c r="A1741" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1741" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1741" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:4">
+      <c r="A1742" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1742" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1742" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1742" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:4">
+      <c r="A1743" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1743" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1743" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1743" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D400"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Move develop template.xlsx and template_type.xlsx to 1.2.0.1
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP-Team\mosip-data\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ABF47C-ED22-434A-9978-DA641204EF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6812" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6972" uniqueCount="648">
   <si>
     <t>lang_code</t>
   </si>
@@ -1822,13 +1821,163 @@
   </si>
   <si>
     <t>vid-card-download-negative-purpose</t>
+  </si>
+  <si>
+    <t>mosip.idp.otp.template.property</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>mosip.idp.biometrics.template.property</t>
+  </si>
+  <si>
+    <t>Biometrics</t>
+  </si>
+  <si>
+    <t>mosip.idp.unknown.authentication.template.property</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>mosip.full.name.template.property</t>
+  </si>
+  <si>
+    <t>mosip.date.of.birth.template.property</t>
+  </si>
+  <si>
+    <t>mosip.uin.template.property</t>
+  </si>
+  <si>
+    <t>mosip.perpetual.vid.template.property</t>
+  </si>
+  <si>
+    <t>mosip.phone.template.property</t>
+  </si>
+  <si>
+    <t>mosip.email.template.property</t>
+  </si>
+  <si>
+    <t>mosip.address.template.property</t>
+  </si>
+  <si>
+    <t>mosip.gender.template.property</t>
+  </si>
+  <si>
+    <t>mosip.defualt.template.property</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Date Of Birth</t>
+  </si>
+  <si>
+    <t>UIN</t>
+  </si>
+  <si>
+    <t>Perpetual VID</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Defualt</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>vid-card-type</t>
+  </si>
+  <si>
+    <t>Vid Card Type</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>Request received email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success-email-subject</t>
+  </si>
+  <si>
+    <t>Success email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure-email-subject</t>
+  </si>
+  <si>
+    <t>Failure email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received-email-content</t>
+  </si>
+  <si>
+    <t>Request received email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success-email-content</t>
+  </si>
+  <si>
+    <t>Success email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure-email-content</t>
+  </si>
+  <si>
+    <t>Failure email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received_SMS</t>
+  </si>
+  <si>
+    <t>Request received sms to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success_SMS</t>
+  </si>
+  <si>
+    <t>Success sms to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure_SMS</t>
+  </si>
+  <si>
+    <t>Failure sms to download my VID card</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_SMS</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject SMS</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL_SUBJECT</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email Subject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1851,6 +2000,12 @@
     <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -1890,7 +2045,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1901,6 +2056,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1932,7 +2090,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2210,18 +2368,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1703"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1688" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1703" sqref="B1703"/>
+    <sheetView tabSelected="1" topLeftCell="A1724" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1730" sqref="F1730"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1"/>
+    <col min="4" max="4" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -26066,8 +26224,568 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1704" spans="1:4">
+      <c r="A1704" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1704" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1704" t="s">
+        <v>599</v>
+      </c>
+      <c r="D1704" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:4">
+      <c r="A1705" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1705" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="C1705" t="s">
+        <v>601</v>
+      </c>
+      <c r="D1705" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:4">
+      <c r="A1706" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1706" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1706" t="s">
+        <v>603</v>
+      </c>
+      <c r="D1706" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:4">
+      <c r="A1707" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1707" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1707" t="s">
+        <v>613</v>
+      </c>
+      <c r="D1707" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:4">
+      <c r="A1708" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1708" t="s">
+        <v>605</v>
+      </c>
+      <c r="C1708" t="s">
+        <v>614</v>
+      </c>
+      <c r="D1708" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:4">
+      <c r="A1709" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1709" t="s">
+        <v>606</v>
+      </c>
+      <c r="C1709" t="s">
+        <v>615</v>
+      </c>
+      <c r="D1709" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:4">
+      <c r="A1710" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1710" t="s">
+        <v>607</v>
+      </c>
+      <c r="C1710" t="s">
+        <v>616</v>
+      </c>
+      <c r="D1710" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:4">
+      <c r="A1711" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1711" t="s">
+        <v>608</v>
+      </c>
+      <c r="C1711" t="s">
+        <v>617</v>
+      </c>
+      <c r="D1711" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:4">
+      <c r="A1712" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1712" t="s">
+        <v>609</v>
+      </c>
+      <c r="C1712" t="s">
+        <v>621</v>
+      </c>
+      <c r="D1712" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:4">
+      <c r="A1713" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1713" t="s">
+        <v>610</v>
+      </c>
+      <c r="C1713" t="s">
+        <v>618</v>
+      </c>
+      <c r="D1713" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:4">
+      <c r="A1714" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1714" t="s">
+        <v>611</v>
+      </c>
+      <c r="C1714" t="s">
+        <v>619</v>
+      </c>
+      <c r="D1714" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:4">
+      <c r="A1715" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1715" t="s">
+        <v>612</v>
+      </c>
+      <c r="C1715" t="s">
+        <v>620</v>
+      </c>
+      <c r="D1715" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:4">
+      <c r="A1716" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1716" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1716" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:4">
+      <c r="A1717" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1717" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1717" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:4">
+      <c r="A1718" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1718" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1718" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1718" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:4">
+      <c r="A1719" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1719" t="s">
+        <v>628</v>
+      </c>
+      <c r="C1719" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1719" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:4">
+      <c r="A1720" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>630</v>
+      </c>
+      <c r="C1720" t="s">
+        <v>631</v>
+      </c>
+      <c r="D1720" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:4">
+      <c r="A1721" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1721" t="s">
+        <v>632</v>
+      </c>
+      <c r="C1721" t="s">
+        <v>633</v>
+      </c>
+      <c r="D1721" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:4">
+      <c r="A1722" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1722" t="s">
+        <v>634</v>
+      </c>
+      <c r="C1722" t="s">
+        <v>635</v>
+      </c>
+      <c r="D1722" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:4">
+      <c r="A1723" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1723" t="s">
+        <v>636</v>
+      </c>
+      <c r="C1723" t="s">
+        <v>637</v>
+      </c>
+      <c r="D1723" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:4">
+      <c r="A1724" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1724" t="s">
+        <v>638</v>
+      </c>
+      <c r="C1724" t="s">
+        <v>639</v>
+      </c>
+      <c r="D1724" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:4">
+      <c r="A1725" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1725" t="s">
+        <v>640</v>
+      </c>
+      <c r="C1725" t="s">
+        <v>641</v>
+      </c>
+      <c r="D1725" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:4">
+      <c r="A1726" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1726" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1726" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:4">
+      <c r="A1727" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1727" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1727" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:4">
+      <c r="A1728" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1728" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:4">
+      <c r="A1729" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1729" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:4">
+      <c r="A1730" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1730" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:4">
+      <c r="A1731" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1731" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:4">
+      <c r="A1732" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1732" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1732" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:4">
+      <c r="A1733" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1733" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1733" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:4">
+      <c r="A1734" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1734" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1734" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1734" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:4">
+      <c r="A1735" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1735" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1735" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:4">
+      <c r="A1736" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1736" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1736" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1736" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:4">
+      <c r="A1737" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1737" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1737" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:4">
+      <c r="A1738" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1738" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1738" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1738" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:4">
+      <c r="A1739" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1739" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1739" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1739" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:4">
+      <c r="A1740" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1740" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1740" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:4">
+      <c r="A1741" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1741" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1741" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:4">
+      <c r="A1742" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1742" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1742" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1742" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:4">
+      <c r="A1743" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1743" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1743" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1743" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D400"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[DSD-2063] merging develop to 1.2.0.1
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP-Team\mosip-data\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8ABF47C-ED22-434A-9978-DA641204EF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6812" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6972" uniqueCount="648">
   <si>
     <t>lang_code</t>
   </si>
@@ -1822,13 +1821,163 @@
   </si>
   <si>
     <t>vid-card-download-negative-purpose</t>
+  </si>
+  <si>
+    <t>mosip.idp.otp.template.property</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>mosip.idp.biometrics.template.property</t>
+  </si>
+  <si>
+    <t>Biometrics</t>
+  </si>
+  <si>
+    <t>mosip.idp.unknown.authentication.template.property</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>mosip.full.name.template.property</t>
+  </si>
+  <si>
+    <t>mosip.date.of.birth.template.property</t>
+  </si>
+  <si>
+    <t>mosip.uin.template.property</t>
+  </si>
+  <si>
+    <t>mosip.perpetual.vid.template.property</t>
+  </si>
+  <si>
+    <t>mosip.phone.template.property</t>
+  </si>
+  <si>
+    <t>mosip.email.template.property</t>
+  </si>
+  <si>
+    <t>mosip.address.template.property</t>
+  </si>
+  <si>
+    <t>mosip.gender.template.property</t>
+  </si>
+  <si>
+    <t>mosip.defualt.template.property</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Date Of Birth</t>
+  </si>
+  <si>
+    <t>UIN</t>
+  </si>
+  <si>
+    <t>Perpetual VID</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Defualt</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>vid-card-type</t>
+  </si>
+  <si>
+    <t>Vid Card Type</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received-email-subject</t>
+  </si>
+  <si>
+    <t>Request received email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success-email-subject</t>
+  </si>
+  <si>
+    <t>Success email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure-email-subject</t>
+  </si>
+  <si>
+    <t>Failure email subject to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received-email-content</t>
+  </si>
+  <si>
+    <t>Request received email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success-email-content</t>
+  </si>
+  <si>
+    <t>Success email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure-email-content</t>
+  </si>
+  <si>
+    <t>Failure email to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-request-received_SMS</t>
+  </si>
+  <si>
+    <t>Request received sms to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-success_SMS</t>
+  </si>
+  <si>
+    <t>Success sms to download my VID card</t>
+  </si>
+  <si>
+    <t>vid-card-download-failure_SMS</t>
+  </si>
+  <si>
+    <t>Failure sms to download my VID card</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_SMS</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject SMS</t>
+  </si>
+  <si>
+    <t>RPR_SUP_REJECT_EMAIL_SUBJECT</t>
+  </si>
+  <si>
+    <t>Template for Supervisor Reject Email Subject</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1851,6 +2000,12 @@
     <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -1890,7 +2045,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1901,6 +2056,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1932,7 +2090,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2210,18 +2368,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1703"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1743"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1688" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1703" sqref="B1703"/>
+    <sheetView tabSelected="1" topLeftCell="A1724" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1730" sqref="F1730"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" style="1"/>
+    <col min="4" max="4" width="8.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -26066,8 +26224,568 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1704" spans="1:4">
+      <c r="A1704" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1704" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1704" t="s">
+        <v>599</v>
+      </c>
+      <c r="D1704" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:4">
+      <c r="A1705" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1705" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="C1705" t="s">
+        <v>601</v>
+      </c>
+      <c r="D1705" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:4">
+      <c r="A1706" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1706" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1706" t="s">
+        <v>603</v>
+      </c>
+      <c r="D1706" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:4">
+      <c r="A1707" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1707" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1707" t="s">
+        <v>613</v>
+      </c>
+      <c r="D1707" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:4">
+      <c r="A1708" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1708" t="s">
+        <v>605</v>
+      </c>
+      <c r="C1708" t="s">
+        <v>614</v>
+      </c>
+      <c r="D1708" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:4">
+      <c r="A1709" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1709" t="s">
+        <v>606</v>
+      </c>
+      <c r="C1709" t="s">
+        <v>615</v>
+      </c>
+      <c r="D1709" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:4">
+      <c r="A1710" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1710" t="s">
+        <v>607</v>
+      </c>
+      <c r="C1710" t="s">
+        <v>616</v>
+      </c>
+      <c r="D1710" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:4">
+      <c r="A1711" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1711" t="s">
+        <v>608</v>
+      </c>
+      <c r="C1711" t="s">
+        <v>617</v>
+      </c>
+      <c r="D1711" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:4">
+      <c r="A1712" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1712" t="s">
+        <v>609</v>
+      </c>
+      <c r="C1712" t="s">
+        <v>621</v>
+      </c>
+      <c r="D1712" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:4">
+      <c r="A1713" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1713" t="s">
+        <v>610</v>
+      </c>
+      <c r="C1713" t="s">
+        <v>618</v>
+      </c>
+      <c r="D1713" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:4">
+      <c r="A1714" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1714" t="s">
+        <v>611</v>
+      </c>
+      <c r="C1714" t="s">
+        <v>619</v>
+      </c>
+      <c r="D1714" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:4">
+      <c r="A1715" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1715" t="s">
+        <v>612</v>
+      </c>
+      <c r="C1715" t="s">
+        <v>620</v>
+      </c>
+      <c r="D1715" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:4">
+      <c r="A1716" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>622</v>
+      </c>
+      <c r="C1716" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1716" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:4">
+      <c r="A1717" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>624</v>
+      </c>
+      <c r="C1717" t="s">
+        <v>625</v>
+      </c>
+      <c r="D1717" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:4">
+      <c r="A1718" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1718" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1718" t="s">
+        <v>627</v>
+      </c>
+      <c r="D1718" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:4">
+      <c r="A1719" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1719" t="s">
+        <v>628</v>
+      </c>
+      <c r="C1719" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1719" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:4">
+      <c r="A1720" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>630</v>
+      </c>
+      <c r="C1720" t="s">
+        <v>631</v>
+      </c>
+      <c r="D1720" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:4">
+      <c r="A1721" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1721" t="s">
+        <v>632</v>
+      </c>
+      <c r="C1721" t="s">
+        <v>633</v>
+      </c>
+      <c r="D1721" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:4">
+      <c r="A1722" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1722" t="s">
+        <v>634</v>
+      </c>
+      <c r="C1722" t="s">
+        <v>635</v>
+      </c>
+      <c r="D1722" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:4">
+      <c r="A1723" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1723" t="s">
+        <v>636</v>
+      </c>
+      <c r="C1723" t="s">
+        <v>637</v>
+      </c>
+      <c r="D1723" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:4">
+      <c r="A1724" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1724" t="s">
+        <v>638</v>
+      </c>
+      <c r="C1724" t="s">
+        <v>639</v>
+      </c>
+      <c r="D1724" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:4">
+      <c r="A1725" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1725" t="s">
+        <v>640</v>
+      </c>
+      <c r="C1725" t="s">
+        <v>641</v>
+      </c>
+      <c r="D1725" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:4">
+      <c r="A1726" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1726" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1726" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:4">
+      <c r="A1727" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1727" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1727" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:4">
+      <c r="A1728" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1728" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1728" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:4">
+      <c r="A1729" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1729" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1729" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:4">
+      <c r="A1730" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1730" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1730" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:4">
+      <c r="A1731" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1731" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1731" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:4">
+      <c r="A1732" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1732" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1732" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:4">
+      <c r="A1733" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1733" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1733" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:4">
+      <c r="A1734" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1734" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1734" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1734" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:4">
+      <c r="A1735" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1735" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1735" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:4">
+      <c r="A1736" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1736" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1736" t="s">
+        <v>643</v>
+      </c>
+      <c r="D1736" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:4">
+      <c r="A1737" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>644</v>
+      </c>
+      <c r="C1737" t="s">
+        <v>645</v>
+      </c>
+      <c r="D1737" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:4">
+      <c r="A1738" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1738" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1738" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1738" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:4">
+      <c r="A1739" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1739" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1739" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1739" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:4">
+      <c r="A1740" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1740" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1740" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:4">
+      <c r="A1741" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1741" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1741" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:4">
+      <c r="A1742" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1742" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1742" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1742" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:4">
+      <c r="A1743" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1743" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1743" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1743" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D400"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected template for resident service.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP-Team\mosip-data\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87778D35-F03C-4626-B422-D54C36170F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$400</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6972" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6992" uniqueCount="658">
   <si>
     <t>lang_code</t>
   </si>
@@ -1971,12 +1972,42 @@
   </si>
   <si>
     <t>Template for Supervisor Reject Email Subject</t>
+  </si>
+  <si>
+    <t>mosip.province.template.property</t>
+  </si>
+  <si>
+    <t>mosip.city.template.property</t>
+  </si>
+  <si>
+    <t>mosip.zone.template.property</t>
+  </si>
+  <si>
+    <t>mosip.postal.code.template.property</t>
+  </si>
+  <si>
+    <t>mosip.region.template.property</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -2090,7 +2121,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2368,11 +2399,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1743"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1748"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1724" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1730" sqref="F1730"/>
+    <sheetView tabSelected="1" topLeftCell="A1705" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1718" sqref="C1718"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -26369,10 +26400,10 @@
         <v>4</v>
       </c>
       <c r="B1714" t="s">
-        <v>611</v>
+        <v>648</v>
       </c>
       <c r="C1714" t="s">
-        <v>619</v>
+        <v>653</v>
       </c>
       <c r="D1714" s="1" t="s">
         <v>7</v>
@@ -26383,10 +26414,10 @@
         <v>4</v>
       </c>
       <c r="B1715" t="s">
-        <v>612</v>
+        <v>649</v>
       </c>
       <c r="C1715" t="s">
-        <v>620</v>
+        <v>654</v>
       </c>
       <c r="D1715" s="1" t="s">
         <v>7</v>
@@ -26397,10 +26428,10 @@
         <v>4</v>
       </c>
       <c r="B1716" t="s">
-        <v>622</v>
+        <v>650</v>
       </c>
       <c r="C1716" t="s">
-        <v>623</v>
+        <v>655</v>
       </c>
       <c r="D1716" s="1" t="s">
         <v>7</v>
@@ -26411,10 +26442,10 @@
         <v>4</v>
       </c>
       <c r="B1717" t="s">
-        <v>624</v>
+        <v>651</v>
       </c>
       <c r="C1717" t="s">
-        <v>625</v>
+        <v>657</v>
       </c>
       <c r="D1717" s="1" t="s">
         <v>7</v>
@@ -26425,10 +26456,10 @@
         <v>4</v>
       </c>
       <c r="B1718" t="s">
-        <v>626</v>
+        <v>652</v>
       </c>
       <c r="C1718" t="s">
-        <v>627</v>
+        <v>656</v>
       </c>
       <c r="D1718" s="1" t="s">
         <v>7</v>
@@ -26439,10 +26470,10 @@
         <v>4</v>
       </c>
       <c r="B1719" t="s">
-        <v>628</v>
+        <v>611</v>
       </c>
       <c r="C1719" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="D1719" s="1" t="s">
         <v>7</v>
@@ -26453,10 +26484,10 @@
         <v>4</v>
       </c>
       <c r="B1720" t="s">
-        <v>630</v>
+        <v>612</v>
       </c>
       <c r="C1720" t="s">
-        <v>631</v>
+        <v>620</v>
       </c>
       <c r="D1720" s="1" t="s">
         <v>7</v>
@@ -26467,10 +26498,10 @@
         <v>4</v>
       </c>
       <c r="B1721" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
       <c r="C1721" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="D1721" s="1" t="s">
         <v>7</v>
@@ -26481,10 +26512,10 @@
         <v>4</v>
       </c>
       <c r="B1722" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="C1722" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="D1722" s="1" t="s">
         <v>7</v>
@@ -26495,10 +26526,10 @@
         <v>4</v>
       </c>
       <c r="B1723" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
       <c r="C1723" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
       <c r="D1723" s="1" t="s">
         <v>7</v>
@@ -26509,10 +26540,10 @@
         <v>4</v>
       </c>
       <c r="B1724" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="C1724" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="D1724" s="1" t="s">
         <v>7</v>
@@ -26523,10 +26554,10 @@
         <v>4</v>
       </c>
       <c r="B1725" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="C1725" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="D1725" s="1" t="s">
         <v>7</v>
@@ -26537,10 +26568,10 @@
         <v>4</v>
       </c>
       <c r="B1726" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="C1726" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="D1726" s="1" t="s">
         <v>7</v>
@@ -26551,10 +26582,10 @@
         <v>4</v>
       </c>
       <c r="B1727" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="C1727" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="D1727" s="1" t="s">
         <v>7</v>
@@ -26562,13 +26593,13 @@
     </row>
     <row r="1728" spans="1:4">
       <c r="A1728" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="B1728" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="C1728" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="D1728" s="1" t="s">
         <v>7</v>
@@ -26576,13 +26607,13 @@
     </row>
     <row r="1729" spans="1:4">
       <c r="A1729" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="B1729" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="C1729" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="D1729" s="1" t="s">
         <v>7</v>
@@ -26590,13 +26621,13 @@
     </row>
     <row r="1730" spans="1:4">
       <c r="A1730" t="s">
-        <v>294</v>
+        <v>4</v>
       </c>
       <c r="B1730" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C1730" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D1730" s="1" t="s">
         <v>7</v>
@@ -26604,13 +26635,13 @@
     </row>
     <row r="1731" spans="1:4">
       <c r="A1731" t="s">
-        <v>294</v>
+        <v>4</v>
       </c>
       <c r="B1731" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1731" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1731" s="1" t="s">
         <v>7</v>
@@ -26618,13 +26649,13 @@
     </row>
     <row r="1732" spans="1:4">
       <c r="A1732" t="s">
-        <v>302</v>
+        <v>4</v>
       </c>
       <c r="B1732" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1732" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1732" s="1" t="s">
         <v>7</v>
@@ -26632,13 +26663,13 @@
     </row>
     <row r="1733" spans="1:4">
       <c r="A1733" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B1733" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1733" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1733" s="1" t="s">
         <v>7</v>
@@ -26646,13 +26677,13 @@
     </row>
     <row r="1734" spans="1:4">
       <c r="A1734" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B1734" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1734" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1734" s="1" t="s">
         <v>7</v>
@@ -26660,13 +26691,13 @@
     </row>
     <row r="1735" spans="1:4">
       <c r="A1735" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B1735" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1735" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1735" s="1" t="s">
         <v>7</v>
@@ -26674,13 +26705,13 @@
     </row>
     <row r="1736" spans="1:4">
       <c r="A1736" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B1736" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1736" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1736" s="1" t="s">
         <v>7</v>
@@ -26688,13 +26719,13 @@
     </row>
     <row r="1737" spans="1:4">
       <c r="A1737" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B1737" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1737" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1737" s="1" t="s">
         <v>7</v>
@@ -26702,13 +26733,13 @@
     </row>
     <row r="1738" spans="1:4">
       <c r="A1738" t="s">
-        <v>4</v>
+        <v>302</v>
       </c>
       <c r="B1738" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1738" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1738" s="1" t="s">
         <v>7</v>
@@ -26716,13 +26747,13 @@
     </row>
     <row r="1739" spans="1:4">
       <c r="A1739" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="B1739" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C1739" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D1739" s="1" t="s">
         <v>7</v>
@@ -26730,13 +26761,13 @@
     </row>
     <row r="1740" spans="1:4">
       <c r="A1740" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B1740" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1740" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1740" s="1" t="s">
         <v>7</v>
@@ -26744,13 +26775,13 @@
     </row>
     <row r="1741" spans="1:4">
       <c r="A1741" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B1741" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C1741" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D1741" s="1" t="s">
         <v>7</v>
@@ -26758,13 +26789,13 @@
     </row>
     <row r="1742" spans="1:4">
       <c r="A1742" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B1742" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1742" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1742" s="1" t="s">
         <v>7</v>
@@ -26772,7 +26803,7 @@
     </row>
     <row r="1743" spans="1:4">
       <c r="A1743" t="s">
-        <v>303</v>
+        <v>4</v>
       </c>
       <c r="B1743" t="s">
         <v>646</v>
@@ -26784,8 +26815,78 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1744" spans="1:4">
+      <c r="A1744" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1744" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1744" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1744" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:4">
+      <c r="A1745" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1745" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1745" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1745" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:4">
+      <c r="A1746" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1746" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1746" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1746" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:4">
+      <c r="A1747" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1747" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1747" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1747" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:4">
+      <c r="A1748" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1748" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1748" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1748" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D400"/>
+  <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added templates for address lines
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1F5D6F-AEEF-4B2A-A358-D97623743B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E622F0E-CE90-40B5-AE3C-0DC534EC9E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7000" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7012" uniqueCount="668">
   <si>
     <t>lang_code</t>
   </si>
@@ -2014,6 +2014,24 @@
   </si>
   <si>
     <t>Photo</t>
+  </si>
+  <si>
+    <t>mosip.address.line1.template.property</t>
+  </si>
+  <si>
+    <t>mosip.address.line2.template.property</t>
+  </si>
+  <si>
+    <t>mosip.address.line3.template.property</t>
+  </si>
+  <si>
+    <t>Address line1</t>
+  </si>
+  <si>
+    <t>Address line2</t>
+  </si>
+  <si>
+    <t>Address line3</t>
   </si>
 </sst>
 </file>
@@ -2412,10 +2430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1750"/>
+  <dimension ref="A1:D1753"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1716" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1720" sqref="C1720"/>
+    <sheetView tabSelected="1" topLeftCell="A1710" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1716" sqref="C1716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -26412,10 +26430,10 @@
         <v>4</v>
       </c>
       <c r="B1714" t="s">
-        <v>648</v>
+        <v>662</v>
       </c>
       <c r="C1714" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
       <c r="D1714" s="1" t="s">
         <v>7</v>
@@ -26426,10 +26444,10 @@
         <v>4</v>
       </c>
       <c r="B1715" t="s">
-        <v>649</v>
+        <v>663</v>
       </c>
       <c r="C1715" t="s">
-        <v>654</v>
+        <v>666</v>
       </c>
       <c r="D1715" s="1" t="s">
         <v>7</v>
@@ -26440,10 +26458,10 @@
         <v>4</v>
       </c>
       <c r="B1716" t="s">
-        <v>650</v>
+        <v>664</v>
       </c>
       <c r="C1716" t="s">
-        <v>655</v>
+        <v>667</v>
       </c>
       <c r="D1716" s="1" t="s">
         <v>7</v>
@@ -26454,10 +26472,10 @@
         <v>4</v>
       </c>
       <c r="B1717" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="C1717" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="D1717" s="1" t="s">
         <v>7</v>
@@ -26468,10 +26486,10 @@
         <v>4</v>
       </c>
       <c r="B1718" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="C1718" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D1718" s="1" t="s">
         <v>7</v>
@@ -26482,10 +26500,10 @@
         <v>4</v>
       </c>
       <c r="B1719" t="s">
-        <v>611</v>
+        <v>650</v>
       </c>
       <c r="C1719" t="s">
-        <v>619</v>
+        <v>655</v>
       </c>
       <c r="D1719" s="1" t="s">
         <v>7</v>
@@ -26496,10 +26514,10 @@
         <v>4</v>
       </c>
       <c r="B1720" t="s">
-        <v>660</v>
+        <v>651</v>
       </c>
       <c r="C1720" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="D1720" s="1" t="s">
         <v>7</v>
@@ -26510,10 +26528,10 @@
         <v>4</v>
       </c>
       <c r="B1721" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="C1721" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D1721" s="1" t="s">
         <v>7</v>
@@ -26524,10 +26542,10 @@
         <v>4</v>
       </c>
       <c r="B1722" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C1722" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D1722" s="1" t="s">
         <v>7</v>
@@ -26538,10 +26556,10 @@
         <v>4</v>
       </c>
       <c r="B1723" t="s">
-        <v>622</v>
+        <v>660</v>
       </c>
       <c r="C1723" t="s">
-        <v>623</v>
+        <v>661</v>
       </c>
       <c r="D1723" s="1" t="s">
         <v>7</v>
@@ -26552,10 +26570,10 @@
         <v>4</v>
       </c>
       <c r="B1724" t="s">
-        <v>624</v>
+        <v>658</v>
       </c>
       <c r="C1724" t="s">
-        <v>625</v>
+        <v>659</v>
       </c>
       <c r="D1724" s="1" t="s">
         <v>7</v>
@@ -26566,10 +26584,10 @@
         <v>4</v>
       </c>
       <c r="B1725" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="C1725" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="D1725" s="1" t="s">
         <v>7</v>
@@ -26580,10 +26598,10 @@
         <v>4</v>
       </c>
       <c r="B1726" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="C1726" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="D1726" s="1" t="s">
         <v>7</v>
@@ -26594,10 +26612,10 @@
         <v>4</v>
       </c>
       <c r="B1727" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="C1727" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="D1727" s="1" t="s">
         <v>7</v>
@@ -26608,10 +26626,10 @@
         <v>4</v>
       </c>
       <c r="B1728" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="C1728" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="D1728" s="1" t="s">
         <v>7</v>
@@ -26622,10 +26640,10 @@
         <v>4</v>
       </c>
       <c r="B1729" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C1729" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="D1729" s="1" t="s">
         <v>7</v>
@@ -26636,10 +26654,10 @@
         <v>4</v>
       </c>
       <c r="B1730" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="C1730" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="D1730" s="1" t="s">
         <v>7</v>
@@ -26650,10 +26668,10 @@
         <v>4</v>
       </c>
       <c r="B1731" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="C1731" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D1731" s="1" t="s">
         <v>7</v>
@@ -26664,10 +26682,10 @@
         <v>4</v>
       </c>
       <c r="B1732" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="C1732" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="D1732" s="1" t="s">
         <v>7</v>
@@ -26678,10 +26696,10 @@
         <v>4</v>
       </c>
       <c r="B1733" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="C1733" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="D1733" s="1" t="s">
         <v>7</v>
@@ -26692,10 +26710,10 @@
         <v>4</v>
       </c>
       <c r="B1734" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="C1734" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="D1734" s="1" t="s">
         <v>7</v>
@@ -26703,13 +26721,13 @@
     </row>
     <row r="1735" spans="1:4">
       <c r="A1735" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="B1735" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C1735" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D1735" s="1" t="s">
         <v>7</v>
@@ -26717,13 +26735,13 @@
     </row>
     <row r="1736" spans="1:4">
       <c r="A1736" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="B1736" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1736" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1736" s="1" t="s">
         <v>7</v>
@@ -26731,13 +26749,13 @@
     </row>
     <row r="1737" spans="1:4">
       <c r="A1737" t="s">
-        <v>294</v>
+        <v>4</v>
       </c>
       <c r="B1737" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1737" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1737" s="1" t="s">
         <v>7</v>
@@ -26745,13 +26763,13 @@
     </row>
     <row r="1738" spans="1:4">
       <c r="A1738" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B1738" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1738" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1738" s="1" t="s">
         <v>7</v>
@@ -26759,13 +26777,13 @@
     </row>
     <row r="1739" spans="1:4">
       <c r="A1739" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="B1739" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1739" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1739" s="1" t="s">
         <v>7</v>
@@ -26773,13 +26791,13 @@
     </row>
     <row r="1740" spans="1:4">
       <c r="A1740" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B1740" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1740" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1740" s="1" t="s">
         <v>7</v>
@@ -26787,13 +26805,13 @@
     </row>
     <row r="1741" spans="1:4">
       <c r="A1741" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="B1741" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1741" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1741" s="1" t="s">
         <v>7</v>
@@ -26801,13 +26819,13 @@
     </row>
     <row r="1742" spans="1:4">
       <c r="A1742" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B1742" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1742" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1742" s="1" t="s">
         <v>7</v>
@@ -26815,13 +26833,13 @@
     </row>
     <row r="1743" spans="1:4">
       <c r="A1743" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B1743" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="C1743" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="D1743" s="1" t="s">
         <v>7</v>
@@ -26829,13 +26847,13 @@
     </row>
     <row r="1744" spans="1:4">
       <c r="A1744" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B1744" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C1744" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1744" s="1" t="s">
         <v>7</v>
@@ -26843,13 +26861,13 @@
     </row>
     <row r="1745" spans="1:4">
       <c r="A1745" t="s">
-        <v>4</v>
+        <v>301</v>
       </c>
       <c r="B1745" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1745" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1745" s="1" t="s">
         <v>7</v>
@@ -26857,13 +26875,13 @@
     </row>
     <row r="1746" spans="1:4">
       <c r="A1746" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B1746" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="C1746" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D1746" s="1" t="s">
         <v>7</v>
@@ -26871,13 +26889,13 @@
     </row>
     <row r="1747" spans="1:4">
       <c r="A1747" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="B1747" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1747" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1747" s="1" t="s">
         <v>7</v>
@@ -26885,7 +26903,7 @@
     </row>
     <row r="1748" spans="1:4">
       <c r="A1748" t="s">
-        <v>302</v>
+        <v>4</v>
       </c>
       <c r="B1748" t="s">
         <v>646</v>
@@ -26899,7 +26917,7 @@
     </row>
     <row r="1749" spans="1:4">
       <c r="A1749" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B1749" t="s">
         <v>646</v>
@@ -26913,7 +26931,7 @@
     </row>
     <row r="1750" spans="1:4">
       <c r="A1750" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B1750" t="s">
         <v>646</v>
@@ -26922,6 +26940,48 @@
         <v>647</v>
       </c>
       <c r="D1750" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:4">
+      <c r="A1751" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1751" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1751" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1751" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:4">
+      <c r="A1752" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1752" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1752" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1752" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:4">
+      <c r="A1753" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1753" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1753" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1753" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new templates for auth-lock-unlock attribute
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\mosipProject\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E622F0E-CE90-40B5-AE3C-0DC534EC9E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9494A80A-3FC8-490A-AFFC-9AF3F37FB991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7012" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7044" uniqueCount="684">
   <si>
     <t>lang_code</t>
   </si>
@@ -2032,6 +2032,54 @@
   </si>
   <si>
     <t>Address line3</t>
+  </si>
+  <si>
+    <t>mosip.otp-email.template.property</t>
+  </si>
+  <si>
+    <t>mosip.otp-phone.template.property</t>
+  </si>
+  <si>
+    <t>mosip.demo.template.property</t>
+  </si>
+  <si>
+    <t>mosip.bio-finger.template.property</t>
+  </si>
+  <si>
+    <t>mosip.bio-iris.template.property</t>
+  </si>
+  <si>
+    <t>mosip.bio-face.template.property</t>
+  </si>
+  <si>
+    <t>Email otp</t>
+  </si>
+  <si>
+    <t>Phone otp</t>
+  </si>
+  <si>
+    <t>Demographic</t>
+  </si>
+  <si>
+    <t>Finger bio</t>
+  </si>
+  <si>
+    <t>Iris bio</t>
+  </si>
+  <si>
+    <t>Face bio</t>
+  </si>
+  <si>
+    <t>mosip.locked.template.property</t>
+  </si>
+  <si>
+    <t>mosip.unlocked.template.property</t>
+  </si>
+  <si>
+    <t>Unlocked status</t>
+  </si>
+  <si>
+    <t>Locked status</t>
   </si>
 </sst>
 </file>
@@ -2430,10 +2478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1753"/>
+  <dimension ref="A1:D1761"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1710" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1716" sqref="C1716"/>
+    <sheetView tabSelected="1" topLeftCell="A1752" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1763" sqref="C1763"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -26985,6 +27033,118 @@
         <v>7</v>
       </c>
     </row>
+    <row r="1754" spans="1:4">
+      <c r="A1754" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1754" t="s">
+        <v>668</v>
+      </c>
+      <c r="C1754" t="s">
+        <v>674</v>
+      </c>
+      <c r="D1754" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:4">
+      <c r="A1755" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1755" t="s">
+        <v>669</v>
+      </c>
+      <c r="C1755" t="s">
+        <v>675</v>
+      </c>
+      <c r="D1755" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:4">
+      <c r="A1756" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1756" t="s">
+        <v>670</v>
+      </c>
+      <c r="C1756" t="s">
+        <v>676</v>
+      </c>
+      <c r="D1756" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:4">
+      <c r="A1757" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1757" t="s">
+        <v>671</v>
+      </c>
+      <c r="C1757" t="s">
+        <v>677</v>
+      </c>
+      <c r="D1757" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:4">
+      <c r="A1758" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1758" t="s">
+        <v>672</v>
+      </c>
+      <c r="C1758" t="s">
+        <v>678</v>
+      </c>
+      <c r="D1758" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:4">
+      <c r="A1759" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1759" t="s">
+        <v>673</v>
+      </c>
+      <c r="C1759" t="s">
+        <v>679</v>
+      </c>
+      <c r="D1759" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:4">
+      <c r="A1760" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1760" t="s">
+        <v>681</v>
+      </c>
+      <c r="C1760" t="s">
+        <v>682</v>
+      </c>
+      <c r="D1760" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:4">
+      <c r="A1761" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1761" t="s">
+        <v>680</v>
+      </c>
+      <c r="C1761" t="s">
+        <v>683</v>
+      </c>
+      <c r="D1761" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D400" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
added templates for event status
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E92173D-F462-49D4-A0E1-04E09237AA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E8D824-C08A-4C44-9480-149ED5502CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8904" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8988" uniqueCount="691">
   <si>
     <t>lang_code</t>
   </si>
@@ -2078,6 +2078,24 @@
   </si>
   <si>
     <t>spa</t>
+  </si>
+  <si>
+    <t>mosip.event.status.success.template</t>
+  </si>
+  <si>
+    <t>mosip.event.status.failed.template</t>
+  </si>
+  <si>
+    <t>mosip.event.status.inprogress.template</t>
+  </si>
+  <si>
+    <t>Success event status</t>
+  </si>
+  <si>
+    <t>Failed event status</t>
+  </si>
+  <si>
+    <t>In progress event status</t>
   </si>
 </sst>
 </file>
@@ -2497,10 +2515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2226"/>
+  <dimension ref="A1:D2247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2218" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2227" sqref="A2227"/>
+    <sheetView tabSelected="1" topLeftCell="A2235" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2248" sqref="A2248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -33674,6 +33692,300 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2227" spans="1:4">
+      <c r="A2227" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2227" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2227" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2227" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:4">
+      <c r="A2228" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2228" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2228" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2228" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2229" spans="1:4">
+      <c r="A2229" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2229" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2229" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2229" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2230" spans="1:4">
+      <c r="A2230" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2230" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2230" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2230" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:4">
+      <c r="A2231" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2231" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2231" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2231" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2232" spans="1:4">
+      <c r="A2232" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2232" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2232" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2232" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2233" spans="1:4">
+      <c r="A2233" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2233" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2233" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2233" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:4">
+      <c r="A2234" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2234" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2234" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2234" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:4">
+      <c r="A2235" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2235" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2235" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2235" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2236" spans="1:4">
+      <c r="A2236" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2236" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2236" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2236" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2237" spans="1:4">
+      <c r="A2237" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2237" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2237" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2237" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:4">
+      <c r="A2238" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2238" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2238" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2238" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:4">
+      <c r="A2239" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2239" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2239" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2239" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2240" spans="1:4">
+      <c r="A2240" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2240" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2240" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2240" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2241" spans="1:4">
+      <c r="A2241" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2241" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2241" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2241" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2242" spans="1:4">
+      <c r="A2242" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2242" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2242" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2242" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2243" spans="1:4">
+      <c r="A2243" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2243" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2243" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2243" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2244" spans="1:4">
+      <c r="A2244" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2244" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2244" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2244" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2245" spans="1:4">
+      <c r="A2245" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2245" t="s">
+        <v>685</v>
+      </c>
+      <c r="C2245" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2245" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2246" spans="1:4">
+      <c r="A2246" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2246" t="s">
+        <v>686</v>
+      </c>
+      <c r="C2246" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2246" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2247" spans="1:4">
+      <c r="A2247" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2247" t="s">
+        <v>687</v>
+      </c>
+      <c r="C2247" t="s">
+        <v>690</v>
+      </c>
+      <c r="D2247" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added templates for auth types
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E8D824-C08A-4C44-9480-149ED5502CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AB5609-948E-4530-9863-17363723231D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8988" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9772" uniqueCount="747">
   <si>
     <t>lang_code</t>
   </si>
@@ -2096,6 +2096,174 @@
   </si>
   <si>
     <t>In progress event status</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.OTP-REQUEST.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.OTP-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.DEMO-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.FINGERPRINT-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.IRIS-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.FACE-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.STATIC-PIN-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.STATIC-PIN-STORAGE.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.EKYC-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.KYC-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.KYC-EXCHANGE.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.IDENTITY-KEY-BINDING.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.TOKEN-REQUEST.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.TOKEN-AUTH.Y</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.OTP-REQUEST.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.OTP-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.DEMO-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.FINGERPRINT-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.IRIS-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.FACE-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.STATIC-PIN-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.STATIC-PIN-STORAGE.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.EKYC-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.KYC-AUTH.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.KYC-EXCHANGE.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.IDENTITY-KEY-BINDING.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.TOKEN-REQUEST.N</t>
+  </si>
+  <si>
+    <t>mosip.ida.auth-request.TOKEN-AUTH.N</t>
+  </si>
+  <si>
+    <t>OTP Request Success</t>
+  </si>
+  <si>
+    <t>OTP Authentication Success</t>
+  </si>
+  <si>
+    <t>Demo Authentication Success</t>
+  </si>
+  <si>
+    <t>Finger Authentication Success</t>
+  </si>
+  <si>
+    <t>Iris  Authentication Success</t>
+  </si>
+  <si>
+    <t>Face Authentication Success</t>
+  </si>
+  <si>
+    <t>Pin Authentication Success</t>
+  </si>
+  <si>
+    <t>Static Pin Store Request Success</t>
+  </si>
+  <si>
+    <t>EKYC Authentication Request Success</t>
+  </si>
+  <si>
+    <t>KYC Authentication Request Success</t>
+  </si>
+  <si>
+    <t>KYC Exchange Request Success</t>
+  </si>
+  <si>
+    <t>Identity Key Binding Request Success</t>
+  </si>
+  <si>
+    <t>Token Request Success</t>
+  </si>
+  <si>
+    <t>Token based Authentication Success</t>
+  </si>
+  <si>
+    <t>OTP Request Failed</t>
+  </si>
+  <si>
+    <t>OTP Authentication Failed</t>
+  </si>
+  <si>
+    <t>Demo Authentication Failed</t>
+  </si>
+  <si>
+    <t>Finger Authentication Failed</t>
+  </si>
+  <si>
+    <t>Iris  Authentication Failed</t>
+  </si>
+  <si>
+    <t>Face Authentication Failed</t>
+  </si>
+  <si>
+    <t>Pin Authentication Failed</t>
+  </si>
+  <si>
+    <t>Static Pin Store Request Failed</t>
+  </si>
+  <si>
+    <t>EKYC Authentication Request Failed</t>
+  </si>
+  <si>
+    <t>KYC Authentication Request Failed</t>
+  </si>
+  <si>
+    <t>KYC Exchange Request Failed</t>
+  </si>
+  <si>
+    <t>Identity Key Binding Request Failed</t>
+  </si>
+  <si>
+    <t>Token Request Failed</t>
+  </si>
+  <si>
+    <t>Token based Authentication Failed</t>
   </si>
 </sst>
 </file>
@@ -2515,10 +2683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2247"/>
+  <dimension ref="A1:D2443"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2235" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2248" sqref="A2248"/>
+    <sheetView tabSelected="1" topLeftCell="A2430" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2444" sqref="A2444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -33986,6 +34154,2750 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2248" spans="1:4">
+      <c r="A2248" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2248" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2248" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2248" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:4">
+      <c r="A2249" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2249" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2249" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2249" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2250" spans="1:4">
+      <c r="A2250" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2250" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2250" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2250" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:4">
+      <c r="A2251" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2251" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2251" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2251" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:4">
+      <c r="A2252" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2252" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2252" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2252" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2253" spans="1:4">
+      <c r="A2253" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2253" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2253" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2253" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:4">
+      <c r="A2254" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2254" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2254" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2254" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2255" spans="1:4">
+      <c r="A2255" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2255" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2255" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2255" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:4">
+      <c r="A2256" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2256" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2256" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2256" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:4">
+      <c r="A2257" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2257" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2257" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2257" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2258" spans="1:4">
+      <c r="A2258" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2258" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2258" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2258" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:4">
+      <c r="A2259" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2259" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2259" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2259" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:4">
+      <c r="A2260" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2260" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2260" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2260" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:4">
+      <c r="A2261" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2261" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2261" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2261" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:4">
+      <c r="A2262" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2262" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2262" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2262" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:4">
+      <c r="A2263" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2263" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2263" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2263" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:4">
+      <c r="A2264" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2264" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2264" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2264" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:4">
+      <c r="A2265" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2265" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2265" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2265" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:4">
+      <c r="A2266" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2266" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2266" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2266" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:4">
+      <c r="A2267" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2267" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2267" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2267" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:4">
+      <c r="A2268" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2268" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2268" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2268" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:4">
+      <c r="A2269" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2269" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2269" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2269" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:4">
+      <c r="A2270" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2270" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2270" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2270" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:4">
+      <c r="A2271" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2271" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2271" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2271" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:4">
+      <c r="A2272" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2272" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2272" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2272" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2273" spans="1:4">
+      <c r="A2273" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2273" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2273" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2273" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:4">
+      <c r="A2274" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2274" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2274" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2274" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:4">
+      <c r="A2275" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2275" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2275" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2275" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:4">
+      <c r="A2276" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2276" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2276" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2276" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2277" spans="1:4">
+      <c r="A2277" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2277" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2277" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2277" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:4">
+      <c r="A2278" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2278" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2278" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2278" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:4">
+      <c r="A2279" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2279" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2279" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2279" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:4">
+      <c r="A2280" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2280" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2280" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2280" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:4">
+      <c r="A2281" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2281" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2281" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2281" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:4">
+      <c r="A2282" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2282" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2282" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2282" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2283" spans="1:4">
+      <c r="A2283" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2283" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2283" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2283" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:4">
+      <c r="A2284" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2284" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2284" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2284" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:4">
+      <c r="A2285" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2285" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2285" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2285" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:4">
+      <c r="A2286" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2286" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2286" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2286" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:4">
+      <c r="A2287" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2287" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2287" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2287" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:4">
+      <c r="A2288" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2288" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2288" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2288" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:4">
+      <c r="A2289" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2289" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2289" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2289" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:4">
+      <c r="A2290" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2290" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2290" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2290" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:4">
+      <c r="A2291" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2291" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2291" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2291" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:4">
+      <c r="A2292" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2292" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2292" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2292" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2293" spans="1:4">
+      <c r="A2293" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2293" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2293" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2293" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:4">
+      <c r="A2294" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2294" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2294" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2294" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:4">
+      <c r="A2295" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2295" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2295" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2295" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:4">
+      <c r="A2296" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2296" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2296" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2296" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:4">
+      <c r="A2297" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2297" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2297" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2297" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:4">
+      <c r="A2298" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2298" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2298" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2298" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:4">
+      <c r="A2299" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2299" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2299" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2299" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:4">
+      <c r="A2300" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2300" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2300" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2300" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:4">
+      <c r="A2301" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2301" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2301" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2301" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:4">
+      <c r="A2302" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2302" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2302" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2302" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:4">
+      <c r="A2303" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2303" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2303" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2303" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:4">
+      <c r="A2304" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2304" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2304" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2304" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:4">
+      <c r="A2305" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2305" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2305" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2305" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:4">
+      <c r="A2306" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2306" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2306" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2306" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:4">
+      <c r="A2307" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2307" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2307" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2307" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:4">
+      <c r="A2308" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2308" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2308" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2308" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:4">
+      <c r="A2309" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2309" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2309" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2309" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:4">
+      <c r="A2310" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2310" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2310" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2310" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:4">
+      <c r="A2311" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2311" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2311" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2311" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:4">
+      <c r="A2312" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2312" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2312" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2312" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2313" spans="1:4">
+      <c r="A2313" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2313" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2313" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2313" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:4">
+      <c r="A2314" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2314" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2314" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2314" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:4">
+      <c r="A2315" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2315" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2315" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2315" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:4">
+      <c r="A2316" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2316" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2316" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2316" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:4">
+      <c r="A2317" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2317" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2317" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2317" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:4">
+      <c r="A2318" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2318" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2318" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2318" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:4">
+      <c r="A2319" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2319" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2319" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2319" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:4">
+      <c r="A2320" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2320" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2320" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2320" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:4">
+      <c r="A2321" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2321" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2321" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2321" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2322" spans="1:4">
+      <c r="A2322" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2322" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2322" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2322" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2323" spans="1:4">
+      <c r="A2323" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2323" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2323" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2323" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:4">
+      <c r="A2324" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2324" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2324" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2324" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2325" spans="1:4">
+      <c r="A2325" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2325" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2325" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2325" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:4">
+      <c r="A2326" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2326" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2326" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2326" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2327" spans="1:4">
+      <c r="A2327" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2327" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2327" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2327" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2328" spans="1:4">
+      <c r="A2328" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2328" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2328" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2328" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2329" spans="1:4">
+      <c r="A2329" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2329" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2329" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2329" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:4">
+      <c r="A2330" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2330" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2330" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2330" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:4">
+      <c r="A2331" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2331" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2331" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2331" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:4">
+      <c r="A2332" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2332" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2332" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2332" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2333" spans="1:4">
+      <c r="A2333" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2333" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2333" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2333" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:4">
+      <c r="A2334" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2334" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2334" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2334" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:4">
+      <c r="A2335" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2335" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2335" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2335" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:4">
+      <c r="A2336" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2336" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2336" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2336" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:4">
+      <c r="A2337" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2337" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2337" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2337" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:4">
+      <c r="A2338" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2338" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2338" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2338" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:4">
+      <c r="A2339" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2339" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2339" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2339" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:4">
+      <c r="A2340" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2340" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2340" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2340" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:4">
+      <c r="A2341" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2341" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2341" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2341" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:4">
+      <c r="A2342" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2342" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2342" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2342" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:4">
+      <c r="A2343" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2343" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2343" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2343" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:4">
+      <c r="A2344" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2344" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2344" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2344" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:4">
+      <c r="A2345" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2345" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2345" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2345" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:4">
+      <c r="A2346" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2346" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2346" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2346" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:4">
+      <c r="A2347" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2347" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2347" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2347" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:4">
+      <c r="A2348" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2348" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2348" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2348" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:4">
+      <c r="A2349" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2349" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2349" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2349" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:4">
+      <c r="A2350" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2350" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2350" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2350" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:4">
+      <c r="A2351" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2351" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2351" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2351" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2352" spans="1:4">
+      <c r="A2352" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2352" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2352" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2352" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2353" spans="1:4">
+      <c r="A2353" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2353" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2353" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2353" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2354" spans="1:4">
+      <c r="A2354" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2354" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2354" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2354" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2355" spans="1:4">
+      <c r="A2355" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2355" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2355" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2355" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2356" spans="1:4">
+      <c r="A2356" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2356" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2356" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2356" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2357" spans="1:4">
+      <c r="A2357" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2357" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2357" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2357" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:4">
+      <c r="A2358" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2358" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2358" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2358" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2359" spans="1:4">
+      <c r="A2359" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2359" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2359" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2359" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2360" spans="1:4">
+      <c r="A2360" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2360" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2360" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2360" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:4">
+      <c r="A2361" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2361" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2361" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2361" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:4">
+      <c r="A2362" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2362" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2362" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2362" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:4">
+      <c r="A2363" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2363" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2363" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2363" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:4">
+      <c r="A2364" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2364" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2364" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2364" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:4">
+      <c r="A2365" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2365" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2365" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2365" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:4">
+      <c r="A2366" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2366" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2366" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2366" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:4">
+      <c r="A2367" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2367" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2367" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2367" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:4">
+      <c r="A2368" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2368" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2368" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2368" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:4">
+      <c r="A2369" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2369" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2369" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2369" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:4">
+      <c r="A2370" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2370" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2370" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2370" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:4">
+      <c r="A2371" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2371" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2371" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2371" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:4">
+      <c r="A2372" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2372" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2372" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2372" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:4">
+      <c r="A2373" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2373" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2373" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2373" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:4">
+      <c r="A2374" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2374" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2374" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2374" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:4">
+      <c r="A2375" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2375" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2375" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2375" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:4">
+      <c r="A2376" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2376" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2376" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2376" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:4">
+      <c r="A2377" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2377" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2377" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2377" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:4">
+      <c r="A2378" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2378" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2378" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2378" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:4">
+      <c r="A2379" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2379" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2379" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2379" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:4">
+      <c r="A2380" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2380" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2380" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2380" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:4">
+      <c r="A2381" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2381" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2381" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2381" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:4">
+      <c r="A2382" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2382" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2382" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2382" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:4">
+      <c r="A2383" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2383" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2383" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2383" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:4">
+      <c r="A2384" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2384" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2384" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2384" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:4">
+      <c r="A2385" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2385" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2385" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2385" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:4">
+      <c r="A2386" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2386" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2386" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2386" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:4">
+      <c r="A2387" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2387" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2387" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2387" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:4">
+      <c r="A2388" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2388" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2388" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2388" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:4">
+      <c r="A2389" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2389" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2389" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2389" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:4">
+      <c r="A2390" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2390" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2390" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2390" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:4">
+      <c r="A2391" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2391" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2391" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2391" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:4">
+      <c r="A2392" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2392" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2392" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2392" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:4">
+      <c r="A2393" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2393" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2393" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2393" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:4">
+      <c r="A2394" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2394" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2394" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2394" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:4">
+      <c r="A2395" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2395" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2395" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2395" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:4">
+      <c r="A2396" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2396" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2396" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2396" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:4">
+      <c r="A2397" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2397" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2397" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2397" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:4">
+      <c r="A2398" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2398" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2398" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2398" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:4">
+      <c r="A2399" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2399" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2399" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2399" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:4">
+      <c r="A2400" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2400" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2400" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2400" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:4">
+      <c r="A2401" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2401" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2401" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2401" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:4">
+      <c r="A2402" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2402" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2402" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2402" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:4">
+      <c r="A2403" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2403" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2403" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2403" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:4">
+      <c r="A2404" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2404" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2404" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2404" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:4">
+      <c r="A2405" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2405" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2405" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2405" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:4">
+      <c r="A2406" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2406" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2406" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2406" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:4">
+      <c r="A2407" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2407" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2407" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2407" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:4">
+      <c r="A2408" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2408" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2408" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2408" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:4">
+      <c r="A2409" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2409" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2409" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2409" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:4">
+      <c r="A2410" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2410" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2410" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2410" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:4">
+      <c r="A2411" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2411" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2411" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2411" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:4">
+      <c r="A2412" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2412" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2412" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2412" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:4">
+      <c r="A2413" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2413" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2413" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2413" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:4">
+      <c r="A2414" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2414" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2414" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2414" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:4">
+      <c r="A2415" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2415" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2415" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2415" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:4">
+      <c r="A2416" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2416" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2416" t="s">
+        <v>719</v>
+      </c>
+      <c r="D2416" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:4">
+      <c r="A2417" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2417" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2417" t="s">
+        <v>720</v>
+      </c>
+      <c r="D2417" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:4">
+      <c r="A2418" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2418" t="s">
+        <v>693</v>
+      </c>
+      <c r="C2418" t="s">
+        <v>721</v>
+      </c>
+      <c r="D2418" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:4">
+      <c r="A2419" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2419" t="s">
+        <v>694</v>
+      </c>
+      <c r="C2419" t="s">
+        <v>722</v>
+      </c>
+      <c r="D2419" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:4">
+      <c r="A2420" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2420" t="s">
+        <v>695</v>
+      </c>
+      <c r="C2420" t="s">
+        <v>723</v>
+      </c>
+      <c r="D2420" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:4">
+      <c r="A2421" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2421" t="s">
+        <v>696</v>
+      </c>
+      <c r="C2421" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2421" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:4">
+      <c r="A2422" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2422" t="s">
+        <v>697</v>
+      </c>
+      <c r="C2422" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2422" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:4">
+      <c r="A2423" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2423" t="s">
+        <v>698</v>
+      </c>
+      <c r="C2423" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2423" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:4">
+      <c r="A2424" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2424" t="s">
+        <v>699</v>
+      </c>
+      <c r="C2424" t="s">
+        <v>727</v>
+      </c>
+      <c r="D2424" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:4">
+      <c r="A2425" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2425" t="s">
+        <v>700</v>
+      </c>
+      <c r="C2425" t="s">
+        <v>728</v>
+      </c>
+      <c r="D2425" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:4">
+      <c r="A2426" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2426" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2426" t="s">
+        <v>729</v>
+      </c>
+      <c r="D2426" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:4">
+      <c r="A2427" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2427" t="s">
+        <v>702</v>
+      </c>
+      <c r="C2427" t="s">
+        <v>730</v>
+      </c>
+      <c r="D2427" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:4">
+      <c r="A2428" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2428" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2428" t="s">
+        <v>731</v>
+      </c>
+      <c r="D2428" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:4">
+      <c r="A2429" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2429" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2429" t="s">
+        <v>732</v>
+      </c>
+      <c r="D2429" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:4">
+      <c r="A2430" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2430" t="s">
+        <v>705</v>
+      </c>
+      <c r="C2430" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2430" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:4">
+      <c r="A2431" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2431" t="s">
+        <v>706</v>
+      </c>
+      <c r="C2431" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2431" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:4">
+      <c r="A2432" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2432" t="s">
+        <v>707</v>
+      </c>
+      <c r="C2432" t="s">
+        <v>735</v>
+      </c>
+      <c r="D2432" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:4">
+      <c r="A2433" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2433" t="s">
+        <v>708</v>
+      </c>
+      <c r="C2433" t="s">
+        <v>736</v>
+      </c>
+      <c r="D2433" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:4">
+      <c r="A2434" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2434" t="s">
+        <v>709</v>
+      </c>
+      <c r="C2434" t="s">
+        <v>737</v>
+      </c>
+      <c r="D2434" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:4">
+      <c r="A2435" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2435" t="s">
+        <v>710</v>
+      </c>
+      <c r="C2435" t="s">
+        <v>738</v>
+      </c>
+      <c r="D2435" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:4">
+      <c r="A2436" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2436" t="s">
+        <v>711</v>
+      </c>
+      <c r="C2436" t="s">
+        <v>739</v>
+      </c>
+      <c r="D2436" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:4">
+      <c r="A2437" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2437" t="s">
+        <v>712</v>
+      </c>
+      <c r="C2437" t="s">
+        <v>740</v>
+      </c>
+      <c r="D2437" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:4">
+      <c r="A2438" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2438" t="s">
+        <v>713</v>
+      </c>
+      <c r="C2438" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2438" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:4">
+      <c r="A2439" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2439" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2439" t="s">
+        <v>742</v>
+      </c>
+      <c r="D2439" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:4">
+      <c r="A2440" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2440" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2440" t="s">
+        <v>743</v>
+      </c>
+      <c r="D2440" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:4">
+      <c r="A2441" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2441" t="s">
+        <v>716</v>
+      </c>
+      <c r="C2441" t="s">
+        <v>744</v>
+      </c>
+      <c r="D2441" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:4">
+      <c r="A2442" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2442" t="s">
+        <v>717</v>
+      </c>
+      <c r="C2442" t="s">
+        <v>745</v>
+      </c>
+      <c r="D2442" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:4">
+      <c r="A2443" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2443" t="s">
+        <v>718</v>
+      </c>
+      <c r="C2443" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2443" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added templates for event types
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB47532A-C573-4679-B035-A1344A948F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9686E3A6-2E78-4136-89FD-57B1FCDF1DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10388" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10780" uniqueCount="818">
   <si>
     <t>lang_code</t>
   </si>
@@ -2393,6 +2393,90 @@
   </si>
   <si>
     <t>mosip.auth-type-code.UNKNOWN</t>
+  </si>
+  <si>
+    <t>Authentication Request event type</t>
+  </si>
+  <si>
+    <t>Share Credential With Partner event type</t>
+  </si>
+  <si>
+    <t>Download Personalized Card event type</t>
+  </si>
+  <si>
+    <t>Order a Physical Card event type</t>
+  </si>
+  <si>
+    <t>Get UIN Card event type</t>
+  </si>
+  <si>
+    <t>Book An Appointment event type</t>
+  </si>
+  <si>
+    <t>Update UIN Data event type</t>
+  </si>
+  <si>
+    <t>Generate VID event type</t>
+  </si>
+  <si>
+    <t>Revoke VID event type</t>
+  </si>
+  <si>
+    <t>Secure My ID event type</t>
+  </si>
+  <si>
+    <t>Download VID Card event type</t>
+  </si>
+  <si>
+    <t>Send OTP event type</t>
+  </si>
+  <si>
+    <t>Verify My Phone/Email event type</t>
+  </si>
+  <si>
+    <t>Default event type</t>
+  </si>
+  <si>
+    <t>mosip.event.type.AUTHENTICATION_REQUEST</t>
+  </si>
+  <si>
+    <t>mosip.event.type.SHARE_CRED_WITH_PARTNER</t>
+  </si>
+  <si>
+    <t>mosip.event.type.DOWNLOAD_PERSONALIZED_CARD</t>
+  </si>
+  <si>
+    <t>mosip.event.type.ORDER_PHYSICAL_CARD</t>
+  </si>
+  <si>
+    <t>mosip.event.type.GET_MY_ID</t>
+  </si>
+  <si>
+    <t>mosip.event.type.BOOK_AN_APPOINTMENT</t>
+  </si>
+  <si>
+    <t>mosip.event.type.UPDATE_MY_UIN</t>
+  </si>
+  <si>
+    <t>mosip.event.type.GENERATE_VID</t>
+  </si>
+  <si>
+    <t>mosip.event.type.REVOKE_VID</t>
+  </si>
+  <si>
+    <t>mosip.event.type.AUTH_TYPE_LOCK_UNLOCK</t>
+  </si>
+  <si>
+    <t>mosip.event.type.VID_CARD_DOWNLOAD</t>
+  </si>
+  <si>
+    <t>mosip.event.type.SEND_OTP</t>
+  </si>
+  <si>
+    <t>mosip.event.type.VALIDATE_OTP</t>
+  </si>
+  <si>
+    <t>mosip.event.type.DEFAULT</t>
   </si>
 </sst>
 </file>
@@ -2812,10 +2896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2597"/>
+  <dimension ref="A1:D2695"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2589" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2598" sqref="A2598"/>
+    <sheetView tabSelected="1" topLeftCell="A2687" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2696" sqref="A2696"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -39183,6 +39267,1378 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2598" spans="1:4">
+      <c r="A2598" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2598" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2598" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2598" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:4">
+      <c r="A2599" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2599" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2599" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2599" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:4">
+      <c r="A2600" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2600" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2600" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2600" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:4">
+      <c r="A2601" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2601" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2601" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2601" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:4">
+      <c r="A2602" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2602" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2602" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2602" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:4">
+      <c r="A2603" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2603" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2603" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2603" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:4">
+      <c r="A2604" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2604" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2604" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2604" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:4">
+      <c r="A2605" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2605" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2605" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2605" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:4">
+      <c r="A2606" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2606" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2606" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2606" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:4">
+      <c r="A2607" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2607" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2607" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2607" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:4">
+      <c r="A2608" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2608" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2608" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2608" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:4">
+      <c r="A2609" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2609" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2609" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2609" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2610" spans="1:4">
+      <c r="A2610" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2610" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2610" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2610" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2611" spans="1:4">
+      <c r="A2611" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2611" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2611" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2611" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2612" spans="1:4">
+      <c r="A2612" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2612" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2612" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2612" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2613" spans="1:4">
+      <c r="A2613" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2613" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2613" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2613" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2614" spans="1:4">
+      <c r="A2614" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2614" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2614" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2614" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2615" spans="1:4">
+      <c r="A2615" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2615" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2615" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2615" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2616" spans="1:4">
+      <c r="A2616" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2616" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2616" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2616" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2617" spans="1:4">
+      <c r="A2617" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2617" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2617" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2617" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2618" spans="1:4">
+      <c r="A2618" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2618" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2618" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2618" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2619" spans="1:4">
+      <c r="A2619" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2619" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2619" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2619" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2620" spans="1:4">
+      <c r="A2620" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2620" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2620" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2620" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2621" spans="1:4">
+      <c r="A2621" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2621" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2621" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2621" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2622" spans="1:4">
+      <c r="A2622" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2622" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2622" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2622" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2623" spans="1:4">
+      <c r="A2623" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2623" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2623" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2623" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2624" spans="1:4">
+      <c r="A2624" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2624" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2624" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2624" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2625" spans="1:4">
+      <c r="A2625" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2625" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2625" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2625" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2626" spans="1:4">
+      <c r="A2626" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2626" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2626" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2626" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2627" spans="1:4">
+      <c r="A2627" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2627" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2627" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2627" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2628" spans="1:4">
+      <c r="A2628" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2628" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2628" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2628" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2629" spans="1:4">
+      <c r="A2629" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2629" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2629" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2629" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2630" spans="1:4">
+      <c r="A2630" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2630" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2630" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2630" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2631" spans="1:4">
+      <c r="A2631" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2631" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2631" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2631" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2632" spans="1:4">
+      <c r="A2632" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2632" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2632" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2632" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2633" spans="1:4">
+      <c r="A2633" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2633" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2633" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2633" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2634" spans="1:4">
+      <c r="A2634" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2634" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2634" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2634" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2635" spans="1:4">
+      <c r="A2635" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2635" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2635" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2635" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2636" spans="1:4">
+      <c r="A2636" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2636" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2636" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2636" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2637" spans="1:4">
+      <c r="A2637" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2637" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2637" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2637" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2638" spans="1:4">
+      <c r="A2638" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2638" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2638" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2638" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2639" spans="1:4">
+      <c r="A2639" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2639" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2639" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2639" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2640" spans="1:4">
+      <c r="A2640" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2640" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2640" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2640" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2641" spans="1:4">
+      <c r="A2641" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2641" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2641" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2641" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:4">
+      <c r="A2642" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2642" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2642" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2642" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:4">
+      <c r="A2643" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2643" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2643" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2643" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:4">
+      <c r="A2644" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2644" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2644" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2644" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:4">
+      <c r="A2645" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2645" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2645" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2645" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:4">
+      <c r="A2646" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2646" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2646" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2646" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:4">
+      <c r="A2647" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2647" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2647" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2647" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:4">
+      <c r="A2648" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2648" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2648" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2648" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:4">
+      <c r="A2649" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2649" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2649" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2649" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:4">
+      <c r="A2650" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2650" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2650" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2650" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:4">
+      <c r="A2651" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2651" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2651" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2651" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:4">
+      <c r="A2652" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2652" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2652" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2652" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:4">
+      <c r="A2653" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2653" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2653" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2653" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:4">
+      <c r="A2654" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2654" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2654" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2654" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:4">
+      <c r="A2655" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2655" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2655" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2655" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:4">
+      <c r="A2656" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2656" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2656" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2656" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:4">
+      <c r="A2657" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2657" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2657" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2657" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:4">
+      <c r="A2658" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2658" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2658" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2658" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:4">
+      <c r="A2659" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2659" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2659" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2659" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:4">
+      <c r="A2660" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2660" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2660" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2660" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:4">
+      <c r="A2661" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2661" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2661" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2661" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:4">
+      <c r="A2662" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2662" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2662" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2662" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:4">
+      <c r="A2663" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2663" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2663" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2663" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:4">
+      <c r="A2664" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2664" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2664" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2664" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:4">
+      <c r="A2665" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2665" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2665" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2665" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:4">
+      <c r="A2666" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2666" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2666" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2666" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:4">
+      <c r="A2667" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2667" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2667" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2667" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:4">
+      <c r="A2668" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2668" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2668" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2668" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:4">
+      <c r="A2669" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2669" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2669" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2669" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:4">
+      <c r="A2670" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2670" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2670" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2670" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:4">
+      <c r="A2671" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2671" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2671" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2671" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:4">
+      <c r="A2672" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2672" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2672" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2672" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:4">
+      <c r="A2673" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2673" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2673" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2673" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:4">
+      <c r="A2674" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2674" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2674" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2674" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:4">
+      <c r="A2675" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2675" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2675" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2675" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:4">
+      <c r="A2676" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2676" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2676" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2676" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:4">
+      <c r="A2677" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2677" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2677" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2677" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:4">
+      <c r="A2678" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2678" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2678" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2678" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:4">
+      <c r="A2679" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2679" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2679" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2679" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:4">
+      <c r="A2680" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2680" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2680" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2680" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:4">
+      <c r="A2681" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2681" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2681" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2681" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:4">
+      <c r="A2682" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2682" t="s">
+        <v>804</v>
+      </c>
+      <c r="C2682" t="s">
+        <v>790</v>
+      </c>
+      <c r="D2682" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:4">
+      <c r="A2683" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2683" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2683" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2683" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:4">
+      <c r="A2684" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2684" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2684" t="s">
+        <v>792</v>
+      </c>
+      <c r="D2684" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:4">
+      <c r="A2685" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2685" t="s">
+        <v>807</v>
+      </c>
+      <c r="C2685" t="s">
+        <v>793</v>
+      </c>
+      <c r="D2685" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:4">
+      <c r="A2686" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2686" t="s">
+        <v>808</v>
+      </c>
+      <c r="C2686" t="s">
+        <v>794</v>
+      </c>
+      <c r="D2686" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:4">
+      <c r="A2687" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2687" t="s">
+        <v>809</v>
+      </c>
+      <c r="C2687" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2687" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:4">
+      <c r="A2688" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2688" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2688" t="s">
+        <v>796</v>
+      </c>
+      <c r="D2688" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:4">
+      <c r="A2689" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2689" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2689" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2689" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:4">
+      <c r="A2690" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2690" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2690" t="s">
+        <v>798</v>
+      </c>
+      <c r="D2690" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:4">
+      <c r="A2691" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2691" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2691" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2691" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:4">
+      <c r="A2692" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2692" t="s">
+        <v>814</v>
+      </c>
+      <c r="C2692" t="s">
+        <v>800</v>
+      </c>
+      <c r="D2692" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:4">
+      <c r="A2693" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2693" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2693" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2693" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:4">
+      <c r="A2694" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2694" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2694" t="s">
+        <v>802</v>
+      </c>
+      <c r="D2694" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:4">
+      <c r="A2695" t="s">
+        <v>684</v>
+      </c>
+      <c r="B2695" t="s">
+        <v>817</v>
+      </c>
+      <c r="C2695" t="s">
+        <v>803</v>
+      </c>
+      <c r="D2695" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added templates for generate revoke msg
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1074108\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5B0F94-DE08-4F06-9012-ECBBD5913697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35702D44-441F-4065-9FC9-1FCAC9389F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9548" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9604" uniqueCount="735">
   <si>
     <t>lang_code</t>
   </si>
@@ -2216,6 +2216,18 @@
   </si>
   <si>
     <t>Unknown attribute</t>
+  </si>
+  <si>
+    <t>mosip.generated.template.property</t>
+  </si>
+  <si>
+    <t>mosip.revoked.template.property</t>
+  </si>
+  <si>
+    <t>Generated</t>
+  </si>
+  <si>
+    <t>Revoked</t>
   </si>
 </sst>
 </file>
@@ -2622,10 +2634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2387"/>
+  <dimension ref="A1:D2401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2380" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2388" sqref="A2388"/>
+    <sheetView tabSelected="1" topLeftCell="A2386" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2402" sqref="A2402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -36053,6 +36065,202 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2388" spans="1:4">
+      <c r="A2388" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2388" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2388" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2388" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:4">
+      <c r="A2389" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2389" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2389" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2389" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:4">
+      <c r="A2390" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2390" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2390" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2390" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:4">
+      <c r="A2391" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2391" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2391" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2391" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:4">
+      <c r="A2392" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2392" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2392" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2392" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:4">
+      <c r="A2393" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2393" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2393" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2393" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:4">
+      <c r="A2394" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2394" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2394" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2394" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:4">
+      <c r="A2395" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2395" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2395" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2395" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:4">
+      <c r="A2396" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2396" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2396" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2396" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:4">
+      <c r="A2397" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2397" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2397" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2397" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:4">
+      <c r="A2398" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2398" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2398" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2398" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:4">
+      <c r="A2399" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2399" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2399" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2399" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:4">
+      <c r="A2400" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2400" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="C2400" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="D2400" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:4">
+      <c r="A2401" t="s">
+        <v>314</v>
+      </c>
+      <c r="B2401" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2401" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="D2401" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
DSD-3609 Removed duplicate code for template type code RPR_SUP_REJECT_EMAIL_SUBJECT.
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A72B4D-BA1A-4992-9B77-3DB127B7494C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D67A2A-6DCA-4473-9B8D-71040041915D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12312" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1773</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1767</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7092" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7068" uniqueCount="684">
   <si>
     <t>lang_code</t>
   </si>
@@ -2478,17 +2478,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1773"/>
+  <dimension ref="A1:D1767"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A1753" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1762" sqref="E1762"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="37.5546875" customWidth="1"/>
+    <col min="2" max="2" width="37.54296875" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="1"/>
+    <col min="4" max="4" width="8.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -27150,10 +27150,10 @@
         <v>4</v>
       </c>
       <c r="B1762" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1762" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1762" s="1" t="s">
         <v>7</v>
@@ -27164,10 +27164,10 @@
         <v>293</v>
       </c>
       <c r="B1763" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1763" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1763" s="1" t="s">
         <v>7</v>
@@ -27178,10 +27178,10 @@
         <v>294</v>
       </c>
       <c r="B1764" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1764" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1764" s="1" t="s">
         <v>7</v>
@@ -27192,10 +27192,10 @@
         <v>302</v>
       </c>
       <c r="B1765" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1765" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1765" s="1" t="s">
         <v>7</v>
@@ -27206,10 +27206,10 @@
         <v>301</v>
       </c>
       <c r="B1766" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1766" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1766" s="1" t="s">
         <v>7</v>
@@ -27220,101 +27220,17 @@
         <v>303</v>
       </c>
       <c r="B1767" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C1767" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D1767" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="1768" spans="1:4">
-      <c r="A1768" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1768" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1768" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1768" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1769" spans="1:4">
-      <c r="A1769" t="s">
-        <v>293</v>
-      </c>
-      <c r="B1769" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1769" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1769" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1770" spans="1:4">
-      <c r="A1770" t="s">
-        <v>294</v>
-      </c>
-      <c r="B1770" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1770" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1770" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1771" spans="1:4">
-      <c r="A1771" t="s">
-        <v>302</v>
-      </c>
-      <c r="B1771" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1771" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1771" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1772" spans="1:4">
-      <c r="A1772" t="s">
-        <v>301</v>
-      </c>
-      <c r="B1772" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1772" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1772" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1773" spans="1:4">
-      <c r="A1773" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1773" t="s">
-        <v>644</v>
-      </c>
-      <c r="C1773" t="s">
-        <v>645</v>
-      </c>
-      <c r="D1773" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D1773" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D1767" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
MOSIP-40766: Added all new templates for email notifications
Signed-off-by: Swetha K <swetha.k@technoforte.co.in>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FBD232-C82B-47AC-B317-F76556C5A17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2569C69-C9F3-4645-BAB1-9AE72E65D57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14964" uniqueCount="1399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15108" uniqueCount="1431">
   <si>
     <t>lang_code</t>
   </si>
@@ -5837,6 +5837,102 @@
   </si>
   <si>
     <t>Authentication positive summary</t>
+  </si>
+  <si>
+    <t>ROOT_CERT_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>INTERMEDIATE_CERT_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>PARTNER_CERT_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>WEEKLY_SUMMARY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>ROOT_CERT_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>INTERMEDIATE_CERT_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>PARTNER_CERT_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>WEEKLY_SUMMARY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Template for root certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle d'expiration du certificat racine</t>
+  </si>
+  <si>
+    <t>نموذج لانتهاء صلاحية شهادة الجذر</t>
+  </si>
+  <si>
+    <t>Template for intermediate certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle d'expiration de certificat intermédiaire</t>
+  </si>
+  <si>
+    <t>نموذج انتهاء صلاحية الشهادة المتوسطة</t>
+  </si>
+  <si>
+    <t>Template for partner certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle d'expiration du certificat de partenaire</t>
+  </si>
+  <si>
+    <t>نموذج انتهاء صلاحية شهادة الشريك</t>
+  </si>
+  <si>
+    <t>Template for weekly summary notifications</t>
+  </si>
+  <si>
+    <t>Modèle pour les notifications récapitulatives hebdomadaires</t>
+  </si>
+  <si>
+    <t>نموذج لإشعارات الملخص الأسبوعية</t>
+  </si>
+  <si>
+    <t>Subject template for root certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du certificat racine</t>
+  </si>
+  <si>
+    <t>نموذج موضوعي لانتهاء صلاحية شهادة الجذر</t>
+  </si>
+  <si>
+    <t>Subject template for intermediate certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du certificat intermédiaire</t>
+  </si>
+  <si>
+    <t>نموذج موضوعي لانتهاء صلاحية الشهادة المتوسطة</t>
+  </si>
+  <si>
+    <t>Subject template for partner certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du certificat du partenaire</t>
+  </si>
+  <si>
+    <t>نموذج موضوعي لانتهاء صلاحية شهادة الشريك</t>
+  </si>
+  <si>
+    <t>Subject template for weekly summary notifications</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour les notifications récapitulatives hebdomadaires</t>
+  </si>
+  <si>
+    <t>قالب موضوعي لإشعارات الملخص الأسبوعي</t>
   </si>
 </sst>
 </file>
@@ -6305,17 +6401,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2494"/>
+  <dimension ref="A1:F2518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2478" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2493" sqref="B2493"/>
+    <sheetView tabSelected="1" topLeftCell="A2510" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2518" sqref="D2518"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" customWidth="1"/>
-    <col min="2" max="2" width="40.453125" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="27" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6879,7 +6975,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28.5">
+    <row r="29" spans="1:6" ht="29.25">
       <c r="A29" t="s">
         <v>291</v>
       </c>
@@ -6919,7 +7015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" ht="29.25">
       <c r="A31" t="s">
         <v>291</v>
       </c>
@@ -6959,7 +7055,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.5">
+    <row r="33" spans="1:6" ht="29.25">
       <c r="A33" t="s">
         <v>291</v>
       </c>
@@ -7359,7 +7455,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.5">
+    <row r="53" spans="1:6" ht="29.25">
       <c r="A53" t="s">
         <v>291</v>
       </c>
@@ -7379,7 +7475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="28.5">
+    <row r="54" spans="1:6" ht="29.25">
       <c r="A54" t="s">
         <v>291</v>
       </c>
@@ -7419,7 +7515,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="28.5">
+    <row r="56" spans="1:6" ht="29.25">
       <c r="A56" t="s">
         <v>291</v>
       </c>
@@ -7439,7 +7535,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="29">
+    <row r="57" spans="1:6" ht="30">
       <c r="A57" t="s">
         <v>291</v>
       </c>
@@ -7479,7 +7575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="28.5">
+    <row r="59" spans="1:6" ht="29.25">
       <c r="A59" t="s">
         <v>291</v>
       </c>
@@ -7499,7 +7595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="28.5">
+    <row r="60" spans="1:6" ht="29.25">
       <c r="A60" t="s">
         <v>291</v>
       </c>
@@ -7799,7 +7895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" ht="29.25">
       <c r="A75" t="s">
         <v>291</v>
       </c>
@@ -7819,7 +7915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="28.5">
+    <row r="76" spans="1:6" ht="29.25">
       <c r="A76" t="s">
         <v>291</v>
       </c>
@@ -7839,7 +7935,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="28.5">
+    <row r="77" spans="1:6" ht="29.25">
       <c r="A77" t="s">
         <v>291</v>
       </c>
@@ -7939,7 +8035,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="28.5">
+    <row r="82" spans="1:6" ht="29.25">
       <c r="A82" t="s">
         <v>291</v>
       </c>
@@ -8119,7 +8215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="28.5">
+    <row r="91" spans="1:6" ht="29.25">
       <c r="A91" t="s">
         <v>291</v>
       </c>
@@ -8239,7 +8335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="29">
+    <row r="97" spans="1:6" ht="30">
       <c r="A97" t="s">
         <v>291</v>
       </c>
@@ -8479,7 +8575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="28.5">
+    <row r="109" spans="1:6" ht="29.25">
       <c r="A109" t="s">
         <v>291</v>
       </c>
@@ -8539,7 +8635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="28.5">
+    <row r="112" spans="1:6" ht="29.25">
       <c r="A112" t="s">
         <v>291</v>
       </c>
@@ -8719,7 +8815,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" ht="30">
       <c r="A121" t="s">
         <v>291</v>
       </c>
@@ -9199,7 +9295,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="29">
+    <row r="145" spans="1:6" ht="30">
       <c r="A145" t="s">
         <v>291</v>
       </c>
@@ -9259,7 +9355,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="28.5">
+    <row r="148" spans="1:6" ht="29.25">
       <c r="A148" t="s">
         <v>291</v>
       </c>
@@ -9319,7 +9415,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="29">
+    <row r="151" spans="1:6" ht="30">
       <c r="A151" t="s">
         <v>291</v>
       </c>
@@ -9379,7 +9475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="28.5">
+    <row r="154" spans="1:6" ht="29.25">
       <c r="A154" t="s">
         <v>291</v>
       </c>
@@ -9439,7 +9535,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="28.5">
+    <row r="157" spans="1:6" ht="29.25">
       <c r="A157" t="s">
         <v>291</v>
       </c>
@@ -9499,7 +9595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="28.5">
+    <row r="160" spans="1:6" ht="29.25">
       <c r="A160" t="s">
         <v>291</v>
       </c>
@@ -9559,7 +9655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="29">
+    <row r="163" spans="1:6" ht="30">
       <c r="A163" t="s">
         <v>291</v>
       </c>
@@ -9619,7 +9715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="28.5">
+    <row r="166" spans="1:6" ht="29.25">
       <c r="A166" t="s">
         <v>291</v>
       </c>
@@ -9679,7 +9775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="29">
+    <row r="169" spans="1:6" ht="30">
       <c r="A169" t="s">
         <v>291</v>
       </c>
@@ -9739,7 +9835,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="42.5">
+    <row r="172" spans="1:6" ht="43.5">
       <c r="A172" t="s">
         <v>291</v>
       </c>
@@ -9799,7 +9895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="29">
+    <row r="175" spans="1:6" ht="30">
       <c r="A175" t="s">
         <v>291</v>
       </c>
@@ -9859,7 +9955,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="28.5">
+    <row r="178" spans="1:6" ht="29.25">
       <c r="A178" t="s">
         <v>291</v>
       </c>
@@ -9919,7 +10015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="29">
+    <row r="181" spans="1:6" ht="30">
       <c r="A181" t="s">
         <v>291</v>
       </c>
@@ -9979,7 +10075,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="28.5">
+    <row r="184" spans="1:6" ht="29.25">
       <c r="A184" t="s">
         <v>291</v>
       </c>
@@ -10039,7 +10135,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="43">
+    <row r="187" spans="1:6" ht="44.25">
       <c r="A187" t="s">
         <v>291</v>
       </c>
@@ -10099,7 +10195,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="28.5">
+    <row r="190" spans="1:6" ht="29.25">
       <c r="A190" t="s">
         <v>291</v>
       </c>
@@ -10159,7 +10255,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="28.5">
+    <row r="193" spans="1:6" ht="29.25">
       <c r="A193" t="s">
         <v>291</v>
       </c>
@@ -10219,7 +10315,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="28.5">
+    <row r="196" spans="1:6" ht="29.25">
       <c r="A196" t="s">
         <v>291</v>
       </c>
@@ -10279,7 +10375,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="42.5">
+    <row r="199" spans="1:6" ht="43.5">
       <c r="A199" t="s">
         <v>291</v>
       </c>
@@ -10339,7 +10435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="42.5">
+    <row r="202" spans="1:6" ht="43.5">
       <c r="A202" t="s">
         <v>291</v>
       </c>
@@ -10399,7 +10495,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="28.5">
+    <row r="205" spans="1:6" ht="29.25">
       <c r="A205" t="s">
         <v>291</v>
       </c>
@@ -10459,7 +10555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="42.5">
+    <row r="208" spans="1:6" ht="43.5">
       <c r="A208" t="s">
         <v>291</v>
       </c>
@@ -10999,7 +11095,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="28.5">
+    <row r="235" spans="1:6" ht="29.25">
       <c r="A235" t="s">
         <v>291</v>
       </c>
@@ -11059,7 +11155,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="28.5">
+    <row r="238" spans="1:6" ht="29.25">
       <c r="A238" t="s">
         <v>291</v>
       </c>
@@ -11119,7 +11215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="28.5">
+    <row r="241" spans="1:6" ht="29.25">
       <c r="A241" t="s">
         <v>291</v>
       </c>
@@ -11179,7 +11275,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="244" spans="1:6">
+    <row r="244" spans="1:6" ht="29.25">
       <c r="A244" t="s">
         <v>291</v>
       </c>
@@ -11479,7 +11575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="28.5">
+    <row r="259" spans="1:6" ht="29.25">
       <c r="A259" t="s">
         <v>291</v>
       </c>
@@ -11559,7 +11655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="29">
+    <row r="263" spans="1:6" ht="30">
       <c r="A263" t="s">
         <v>297</v>
       </c>
@@ -11579,7 +11675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="29">
+    <row r="264" spans="1:6" ht="30">
       <c r="A264" t="s">
         <v>297</v>
       </c>
@@ -11599,7 +11695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="265" spans="1:6" ht="29">
+    <row r="265" spans="1:6" ht="30">
       <c r="A265" t="s">
         <v>297</v>
       </c>
@@ -11619,7 +11715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="266" spans="1:6" ht="29">
+    <row r="266" spans="1:6" ht="30">
       <c r="A266" t="s">
         <v>297</v>
       </c>
@@ -11639,7 +11735,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="267" spans="1:6" ht="29">
+    <row r="267" spans="1:6" ht="30">
       <c r="A267" t="s">
         <v>297</v>
       </c>
@@ -11659,7 +11755,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="268" spans="1:6" ht="29">
+    <row r="268" spans="1:6" ht="30">
       <c r="A268" t="s">
         <v>297</v>
       </c>
@@ -11679,7 +11775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="269" spans="1:6" ht="29">
+    <row r="269" spans="1:6" ht="30">
       <c r="A269" t="s">
         <v>297</v>
       </c>
@@ -11699,7 +11795,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="270" spans="1:6" ht="29">
+    <row r="270" spans="1:6" ht="30">
       <c r="A270" t="s">
         <v>297</v>
       </c>
@@ -11719,7 +11815,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="271" spans="1:6" ht="29">
+    <row r="271" spans="1:6" ht="30">
       <c r="A271" t="s">
         <v>297</v>
       </c>
@@ -11739,7 +11835,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="272" spans="1:6" ht="29">
+    <row r="272" spans="1:6" ht="45">
       <c r="A272" t="s">
         <v>297</v>
       </c>
@@ -11759,7 +11855,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="273" spans="1:6" ht="29">
+    <row r="273" spans="1:6" ht="45">
       <c r="A273" t="s">
         <v>297</v>
       </c>
@@ -11779,7 +11875,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="274" spans="1:6" ht="43.5">
+    <row r="274" spans="1:6" ht="45">
       <c r="A274" t="s">
         <v>297</v>
       </c>
@@ -11799,7 +11895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="275" spans="1:6" ht="43.5">
+    <row r="275" spans="1:6" ht="45">
       <c r="A275" t="s">
         <v>297</v>
       </c>
@@ -11819,7 +11915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="276" spans="1:6" ht="29">
+    <row r="276" spans="1:6" ht="30">
       <c r="A276" t="s">
         <v>297</v>
       </c>
@@ -11839,7 +11935,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="277" spans="1:6" ht="29">
+    <row r="277" spans="1:6" ht="30">
       <c r="A277" t="s">
         <v>297</v>
       </c>
@@ -11859,7 +11955,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="278" spans="1:6" ht="29">
+    <row r="278" spans="1:6" ht="30">
       <c r="A278" t="s">
         <v>297</v>
       </c>
@@ -11899,7 +11995,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="280" spans="1:6" ht="43.5">
+    <row r="280" spans="1:6" ht="60">
       <c r="A280" t="s">
         <v>297</v>
       </c>
@@ -11919,7 +12015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="281" spans="1:6" ht="43.5">
+    <row r="281" spans="1:6" ht="60">
       <c r="A281" t="s">
         <v>297</v>
       </c>
@@ -11939,7 +12035,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="282" spans="1:6" ht="43.5">
+    <row r="282" spans="1:6" ht="45">
       <c r="A282" t="s">
         <v>297</v>
       </c>
@@ -11959,7 +12055,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="283" spans="1:6" ht="29">
+    <row r="283" spans="1:6" ht="30">
       <c r="A283" t="s">
         <v>297</v>
       </c>
@@ -11979,7 +12075,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="284" spans="1:6" ht="29">
+    <row r="284" spans="1:6" ht="30">
       <c r="A284" t="s">
         <v>297</v>
       </c>
@@ -11999,7 +12095,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="285" spans="1:6" ht="29">
+    <row r="285" spans="1:6" ht="30">
       <c r="A285" t="s">
         <v>297</v>
       </c>
@@ -12019,7 +12115,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="286" spans="1:6" ht="29">
+    <row r="286" spans="1:6" ht="30">
       <c r="A286" t="s">
         <v>297</v>
       </c>
@@ -12059,7 +12155,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="288" spans="1:6" ht="29">
+    <row r="288" spans="1:6" ht="30">
       <c r="A288" t="s">
         <v>297</v>
       </c>
@@ -12079,7 +12175,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="289" spans="1:6" ht="29">
+    <row r="289" spans="1:6" ht="30">
       <c r="A289" t="s">
         <v>297</v>
       </c>
@@ -12099,7 +12195,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="15">
+    <row r="290" spans="1:6">
       <c r="A290" s="5" t="s">
         <v>297</v>
       </c>
@@ -12119,7 +12215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="291" spans="1:6" ht="29">
+    <row r="291" spans="1:6" ht="45">
       <c r="A291" t="s">
         <v>297</v>
       </c>
@@ -12139,7 +12235,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="29">
+    <row r="292" spans="1:6" ht="30">
       <c r="A292" t="s">
         <v>297</v>
       </c>
@@ -12159,7 +12255,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="293" spans="1:6" ht="29">
+    <row r="293" spans="1:6" ht="45">
       <c r="A293" t="s">
         <v>297</v>
       </c>
@@ -12179,7 +12275,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="294" spans="1:6" ht="43.5">
+    <row r="294" spans="1:6" ht="45">
       <c r="A294" t="s">
         <v>297</v>
       </c>
@@ -12239,7 +12335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="297" spans="1:6" ht="29">
+    <row r="297" spans="1:6" ht="30">
       <c r="A297" t="s">
         <v>297</v>
       </c>
@@ -12259,7 +12355,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="298" spans="1:6" ht="29">
+    <row r="298" spans="1:6" ht="30">
       <c r="A298" t="s">
         <v>297</v>
       </c>
@@ -12279,7 +12375,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="299" spans="1:6" ht="29">
+    <row r="299" spans="1:6" ht="30">
       <c r="A299" t="s">
         <v>297</v>
       </c>
@@ -12299,7 +12395,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="29">
+    <row r="300" spans="1:6" ht="30">
       <c r="A300" t="s">
         <v>297</v>
       </c>
@@ -12319,7 +12415,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="29">
+    <row r="301" spans="1:6" ht="30">
       <c r="A301" t="s">
         <v>297</v>
       </c>
@@ -12339,7 +12435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="302" spans="1:6" ht="29">
+    <row r="302" spans="1:6" ht="30">
       <c r="A302" t="s">
         <v>297</v>
       </c>
@@ -12459,7 +12555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="29">
+    <row r="308" spans="1:6" ht="45">
       <c r="A308" t="s">
         <v>297</v>
       </c>
@@ -12479,7 +12575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="29">
+    <row r="309" spans="1:6" ht="30">
       <c r="A309" t="s">
         <v>297</v>
       </c>
@@ -12499,7 +12595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="310" spans="1:6" ht="29">
+    <row r="310" spans="1:6" ht="30">
       <c r="A310" t="s">
         <v>297</v>
       </c>
@@ -12519,7 +12615,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="311" spans="1:6" ht="43.5">
+    <row r="311" spans="1:6" ht="45">
       <c r="A311" t="s">
         <v>297</v>
       </c>
@@ -12539,7 +12635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="312" spans="1:6" ht="43.5">
+    <row r="312" spans="1:6" ht="45">
       <c r="A312" t="s">
         <v>297</v>
       </c>
@@ -12559,7 +12655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="313" spans="1:6" ht="43.5">
+    <row r="313" spans="1:6" ht="60">
       <c r="A313" t="s">
         <v>297</v>
       </c>
@@ -12579,7 +12675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="43.5">
+    <row r="314" spans="1:6" ht="60">
       <c r="A314" t="s">
         <v>297</v>
       </c>
@@ -12599,7 +12695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="315" spans="1:6" ht="43.5">
+    <row r="315" spans="1:6" ht="45">
       <c r="A315" t="s">
         <v>297</v>
       </c>
@@ -12619,7 +12715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="316" spans="1:6" ht="43.5">
+    <row r="316" spans="1:6" ht="45">
       <c r="A316" t="s">
         <v>297</v>
       </c>
@@ -12639,7 +12735,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="317" spans="1:6" ht="43.5">
+    <row r="317" spans="1:6" ht="60">
       <c r="A317" t="s">
         <v>297</v>
       </c>
@@ -12659,7 +12755,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="318" spans="1:6" ht="43.5">
+    <row r="318" spans="1:6" ht="45">
       <c r="A318" t="s">
         <v>297</v>
       </c>
@@ -12679,7 +12775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="319" spans="1:6" ht="43.5">
+    <row r="319" spans="1:6" ht="60">
       <c r="A319" t="s">
         <v>297</v>
       </c>
@@ -12719,7 +12815,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="321" spans="1:6" ht="43.5">
+    <row r="321" spans="1:6" ht="60">
       <c r="A321" t="s">
         <v>297</v>
       </c>
@@ -12739,7 +12835,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="322" spans="1:6" ht="43.5">
+    <row r="322" spans="1:6" ht="60">
       <c r="A322" t="s">
         <v>297</v>
       </c>
@@ -12759,7 +12855,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="323" spans="1:6" ht="43.5">
+    <row r="323" spans="1:6" ht="60">
       <c r="A323" t="s">
         <v>297</v>
       </c>
@@ -12779,7 +12875,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="324" spans="1:6" ht="43.5">
+    <row r="324" spans="1:6" ht="45">
       <c r="A324" t="s">
         <v>297</v>
       </c>
@@ -12799,7 +12895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="325" spans="1:6" ht="43.5">
+    <row r="325" spans="1:6" ht="45">
       <c r="A325" t="s">
         <v>297</v>
       </c>
@@ -12819,7 +12915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="326" spans="1:6" ht="43.5">
+    <row r="326" spans="1:6" ht="60">
       <c r="A326" t="s">
         <v>297</v>
       </c>
@@ -12839,7 +12935,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="43.5">
+    <row r="327" spans="1:6" ht="45">
       <c r="A327" t="s">
         <v>297</v>
       </c>
@@ -12859,7 +12955,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="43.5">
+    <row r="328" spans="1:6" ht="60">
       <c r="A328" t="s">
         <v>297</v>
       </c>
@@ -12879,7 +12975,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="329" spans="1:6" ht="43.5">
+    <row r="329" spans="1:6" ht="60">
       <c r="A329" t="s">
         <v>297</v>
       </c>
@@ -12899,7 +12995,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="330" spans="1:6" ht="43.5">
+    <row r="330" spans="1:6" ht="60">
       <c r="A330" t="s">
         <v>297</v>
       </c>
@@ -12919,7 +13015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="331" spans="1:6" ht="43.5">
+    <row r="331" spans="1:6" ht="45">
       <c r="A331" t="s">
         <v>297</v>
       </c>
@@ -12939,7 +13035,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="332" spans="1:6" ht="29">
+    <row r="332" spans="1:6" ht="30">
       <c r="A332" t="s">
         <v>297</v>
       </c>
@@ -12959,7 +13055,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="333" spans="1:6" ht="29">
+    <row r="333" spans="1:6" ht="45">
       <c r="A333" t="s">
         <v>297</v>
       </c>
@@ -12979,7 +13075,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="334" spans="1:6" ht="29">
+    <row r="334" spans="1:6" ht="30">
       <c r="A334" t="s">
         <v>297</v>
       </c>
@@ -12999,7 +13095,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="335" spans="1:6" ht="29">
+    <row r="335" spans="1:6" ht="30">
       <c r="A335" t="s">
         <v>297</v>
       </c>
@@ -13019,7 +13115,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="336" spans="1:6" ht="29">
+    <row r="336" spans="1:6" ht="30">
       <c r="A336" t="s">
         <v>297</v>
       </c>
@@ -13039,7 +13135,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="337" spans="1:6" ht="29">
+    <row r="337" spans="1:6" ht="30">
       <c r="A337" t="s">
         <v>297</v>
       </c>
@@ -13239,7 +13335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="347" spans="1:6" ht="29">
+    <row r="347" spans="1:6" ht="30">
       <c r="A347" t="s">
         <v>297</v>
       </c>
@@ -13339,7 +13435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="352" spans="1:6" ht="29">
+    <row r="352" spans="1:6" ht="30">
       <c r="A352" t="s">
         <v>298</v>
       </c>
@@ -13359,7 +13455,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="353" spans="1:6" ht="29">
+    <row r="353" spans="1:6" ht="30">
       <c r="A353" t="s">
         <v>298</v>
       </c>
@@ -13379,7 +13475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="354" spans="1:6" ht="29">
+    <row r="354" spans="1:6" ht="30">
       <c r="A354" t="s">
         <v>298</v>
       </c>
@@ -13399,7 +13495,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="355" spans="1:6" ht="29">
+    <row r="355" spans="1:6" ht="30">
       <c r="A355" t="s">
         <v>298</v>
       </c>
@@ -13419,7 +13515,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="356" spans="1:6" ht="29">
+    <row r="356" spans="1:6" ht="30">
       <c r="A356" t="s">
         <v>298</v>
       </c>
@@ -13459,7 +13555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="358" spans="1:6" ht="29">
+    <row r="358" spans="1:6" ht="30">
       <c r="A358" t="s">
         <v>298</v>
       </c>
@@ -13479,7 +13575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="359" spans="1:6" ht="29">
+    <row r="359" spans="1:6" ht="30">
       <c r="A359" t="s">
         <v>298</v>
       </c>
@@ -13499,7 +13595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="360" spans="1:6" ht="29">
+    <row r="360" spans="1:6" ht="30">
       <c r="A360" t="s">
         <v>298</v>
       </c>
@@ -13519,7 +13615,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="361" spans="1:6" ht="29">
+    <row r="361" spans="1:6" ht="30">
       <c r="A361" t="s">
         <v>298</v>
       </c>
@@ -13539,7 +13635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="362" spans="1:6" ht="29">
+    <row r="362" spans="1:6" ht="30">
       <c r="A362" t="s">
         <v>298</v>
       </c>
@@ -13559,7 +13655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="363" spans="1:6" ht="29">
+    <row r="363" spans="1:6" ht="30">
       <c r="A363" t="s">
         <v>298</v>
       </c>
@@ -13579,7 +13675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="364" spans="1:6" ht="29">
+    <row r="364" spans="1:6" ht="30">
       <c r="A364" t="s">
         <v>298</v>
       </c>
@@ -13599,7 +13695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="365" spans="1:6" ht="29">
+    <row r="365" spans="1:6" ht="30">
       <c r="A365" t="s">
         <v>298</v>
       </c>
@@ -13619,7 +13715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="366" spans="1:6" ht="29">
+    <row r="366" spans="1:6" ht="30">
       <c r="A366" t="s">
         <v>298</v>
       </c>
@@ -13639,7 +13735,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="367" spans="1:6" ht="29">
+    <row r="367" spans="1:6" ht="30">
       <c r="A367" t="s">
         <v>298</v>
       </c>
@@ -13659,7 +13755,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="368" spans="1:6" ht="29">
+    <row r="368" spans="1:6" ht="30">
       <c r="A368" t="s">
         <v>298</v>
       </c>
@@ -13679,7 +13775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="369" spans="1:6" ht="29">
+    <row r="369" spans="1:6" ht="30">
       <c r="A369" t="s">
         <v>298</v>
       </c>
@@ -13699,7 +13795,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="370" spans="1:6" ht="29">
+    <row r="370" spans="1:6" ht="30">
       <c r="A370" t="s">
         <v>298</v>
       </c>
@@ -13719,7 +13815,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="371" spans="1:6" ht="29">
+    <row r="371" spans="1:6" ht="30">
       <c r="A371" t="s">
         <v>298</v>
       </c>
@@ -13739,7 +13835,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="372" spans="1:6">
+    <row r="372" spans="1:6" ht="30">
       <c r="A372" t="s">
         <v>298</v>
       </c>
@@ -13759,7 +13855,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="29">
+    <row r="373" spans="1:6" ht="30">
       <c r="A373" t="s">
         <v>298</v>
       </c>
@@ -13779,7 +13875,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="374" spans="1:6" ht="29">
+    <row r="374" spans="1:6" ht="30">
       <c r="A374" t="s">
         <v>298</v>
       </c>
@@ -13799,7 +13895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="375" spans="1:6" ht="29">
+    <row r="375" spans="1:6" ht="30">
       <c r="A375" t="s">
         <v>298</v>
       </c>
@@ -13819,7 +13915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="376" spans="1:6" ht="29">
+    <row r="376" spans="1:6" ht="30">
       <c r="A376" t="s">
         <v>298</v>
       </c>
@@ -13839,7 +13935,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="377" spans="1:6" ht="29">
+    <row r="377" spans="1:6" ht="30">
       <c r="A377" t="s">
         <v>298</v>
       </c>
@@ -13859,7 +13955,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="378" spans="1:6" ht="29">
+    <row r="378" spans="1:6" ht="30">
       <c r="A378" t="s">
         <v>298</v>
       </c>
@@ -13899,7 +13995,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="380" spans="1:6" ht="29">
+    <row r="380" spans="1:6" ht="30">
       <c r="A380" t="s">
         <v>298</v>
       </c>
@@ -13919,7 +14015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="381" spans="1:6" ht="29">
+    <row r="381" spans="1:6" ht="30">
       <c r="A381" t="s">
         <v>298</v>
       </c>
@@ -13939,7 +14035,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="382" spans="1:6" ht="29">
+    <row r="382" spans="1:6" ht="30">
       <c r="A382" t="s">
         <v>298</v>
       </c>
@@ -13959,7 +14055,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="383" spans="1:6" ht="29">
+    <row r="383" spans="1:6" ht="30">
       <c r="A383" t="s">
         <v>298</v>
       </c>
@@ -14039,7 +14135,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="387" spans="1:6" ht="29">
+    <row r="387" spans="1:6" ht="30">
       <c r="A387" t="s">
         <v>298</v>
       </c>
@@ -14059,7 +14155,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="388" spans="1:6" ht="29">
+    <row r="388" spans="1:6" ht="30">
       <c r="A388" t="s">
         <v>298</v>
       </c>
@@ -14079,7 +14175,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="389" spans="1:6">
+    <row r="389" spans="1:6" ht="30">
       <c r="A389" t="s">
         <v>298</v>
       </c>
@@ -14099,7 +14195,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="390" spans="1:6">
+    <row r="390" spans="1:6" ht="30">
       <c r="A390" t="s">
         <v>298</v>
       </c>
@@ -14119,7 +14215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="391" spans="1:6" ht="29">
+    <row r="391" spans="1:6" ht="30">
       <c r="A391" t="s">
         <v>298</v>
       </c>
@@ -14239,7 +14335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="397" spans="1:6" ht="29">
+    <row r="397" spans="1:6" ht="30">
       <c r="A397" t="s">
         <v>298</v>
       </c>
@@ -14259,7 +14355,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="398" spans="1:6" ht="29">
+    <row r="398" spans="1:6" ht="30">
       <c r="A398" t="s">
         <v>298</v>
       </c>
@@ -14279,7 +14375,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="399" spans="1:6">
+    <row r="399" spans="1:6" ht="30">
       <c r="A399" t="s">
         <v>298</v>
       </c>
@@ -14299,7 +14395,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="400" spans="1:6" ht="29">
+    <row r="400" spans="1:6" ht="30">
       <c r="A400" t="s">
         <v>298</v>
       </c>
@@ -14319,7 +14415,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="401" spans="1:6" ht="29">
+    <row r="401" spans="1:6" ht="30">
       <c r="A401" t="s">
         <v>298</v>
       </c>
@@ -14339,7 +14435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="402" spans="1:6" ht="29">
+    <row r="402" spans="1:6" ht="30">
       <c r="A402" t="s">
         <v>298</v>
       </c>
@@ -14359,7 +14455,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="403" spans="1:6" ht="29">
+    <row r="403" spans="1:6" ht="30">
       <c r="A403" t="s">
         <v>298</v>
       </c>
@@ -14379,7 +14475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="404" spans="1:6" ht="29">
+    <row r="404" spans="1:6" ht="30">
       <c r="A404" t="s">
         <v>298</v>
       </c>
@@ -14399,7 +14495,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="405" spans="1:6" ht="29">
+    <row r="405" spans="1:6" ht="30">
       <c r="A405" t="s">
         <v>298</v>
       </c>
@@ -14419,7 +14515,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="406" spans="1:6" ht="29">
+    <row r="406" spans="1:6" ht="30">
       <c r="A406" t="s">
         <v>298</v>
       </c>
@@ -14439,7 +14535,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="407" spans="1:6" ht="29">
+    <row r="407" spans="1:6" ht="30">
       <c r="A407" t="s">
         <v>298</v>
       </c>
@@ -14459,7 +14555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="408" spans="1:6" ht="29">
+    <row r="408" spans="1:6" ht="45">
       <c r="A408" t="s">
         <v>298</v>
       </c>
@@ -14479,7 +14575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="409" spans="1:6" ht="29">
+    <row r="409" spans="1:6" ht="30">
       <c r="A409" t="s">
         <v>298</v>
       </c>
@@ -14499,7 +14595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="410" spans="1:6" ht="29">
+    <row r="410" spans="1:6" ht="30">
       <c r="A410" t="s">
         <v>298</v>
       </c>
@@ -14519,7 +14615,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="411" spans="1:6" ht="29">
+    <row r="411" spans="1:6" ht="30">
       <c r="A411" t="s">
         <v>298</v>
       </c>
@@ -14539,7 +14635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="412" spans="1:6" ht="29">
+    <row r="412" spans="1:6" ht="30">
       <c r="A412" t="s">
         <v>298</v>
       </c>
@@ -14559,7 +14655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="413" spans="1:6" ht="43.5">
+    <row r="413" spans="1:6" ht="45">
       <c r="A413" t="s">
         <v>298</v>
       </c>
@@ -14579,7 +14675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="414" spans="1:6" ht="29">
+    <row r="414" spans="1:6" ht="30">
       <c r="A414" t="s">
         <v>298</v>
       </c>
@@ -14599,7 +14695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="415" spans="1:6" ht="43.5">
+    <row r="415" spans="1:6" ht="45">
       <c r="A415" t="s">
         <v>298</v>
       </c>
@@ -14619,7 +14715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="416" spans="1:6" ht="29">
+    <row r="416" spans="1:6" ht="30">
       <c r="A416" t="s">
         <v>298</v>
       </c>
@@ -14639,7 +14735,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="417" spans="1:6" ht="29">
+    <row r="417" spans="1:6" ht="30">
       <c r="A417" t="s">
         <v>298</v>
       </c>
@@ -14659,7 +14755,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="418" spans="1:6" ht="29">
+    <row r="418" spans="1:6" ht="30">
       <c r="A418" t="s">
         <v>298</v>
       </c>
@@ -14679,7 +14775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="419" spans="1:6" ht="29">
+    <row r="419" spans="1:6" ht="30">
       <c r="A419" t="s">
         <v>298</v>
       </c>
@@ -14699,7 +14795,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="420" spans="1:6" ht="29">
+    <row r="420" spans="1:6" ht="30">
       <c r="A420" t="s">
         <v>298</v>
       </c>
@@ -14739,7 +14835,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="422" spans="1:6" ht="29">
+    <row r="422" spans="1:6" ht="30">
       <c r="A422" t="s">
         <v>298</v>
       </c>
@@ -14799,7 +14895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="425" spans="1:6">
+    <row r="425" spans="1:6" ht="30">
       <c r="A425" t="s">
         <v>298</v>
       </c>
@@ -14819,7 +14915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="426" spans="1:6" ht="29">
+    <row r="426" spans="1:6" ht="30">
       <c r="A426" t="s">
         <v>298</v>
       </c>
@@ -14919,7 +15015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="431" spans="1:6" ht="43.5">
+    <row r="431" spans="1:6" ht="45">
       <c r="A431" t="s">
         <v>298</v>
       </c>
@@ -14979,7 +15075,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="434" spans="1:6" ht="29">
+    <row r="434" spans="1:6" ht="45">
       <c r="A434" t="s">
         <v>298</v>
       </c>
@@ -14999,7 +15095,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="435" spans="1:6" ht="29">
+    <row r="435" spans="1:6" ht="30">
       <c r="A435" t="s">
         <v>298</v>
       </c>
@@ -15059,7 +15155,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="438" spans="1:6" ht="29">
+    <row r="438" spans="1:6" ht="30">
       <c r="A438" t="s">
         <v>298</v>
       </c>
@@ -15079,7 +15175,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="439" spans="1:6" ht="43.5">
+    <row r="439" spans="1:6" ht="45">
       <c r="A439" t="s">
         <v>298</v>
       </c>
@@ -15099,7 +15195,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="440" spans="1:6" ht="29">
+    <row r="440" spans="1:6" ht="30">
       <c r="A440" t="s">
         <v>298</v>
       </c>
@@ -15119,7 +15215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="441" spans="1:6" ht="43.5">
+    <row r="441" spans="1:6" ht="45">
       <c r="A441" t="s">
         <v>299</v>
       </c>
@@ -15139,7 +15235,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="442" spans="1:6" ht="43.5">
+    <row r="442" spans="1:6" ht="45">
       <c r="A442" t="s">
         <v>299</v>
       </c>
@@ -15159,7 +15255,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="443" spans="1:6" ht="43.5">
+    <row r="443" spans="1:6" ht="45">
       <c r="A443" t="s">
         <v>299</v>
       </c>
@@ -15179,7 +15275,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="444" spans="1:6" ht="43.5">
+    <row r="444" spans="1:6" ht="45">
       <c r="A444" t="s">
         <v>299</v>
       </c>
@@ -15199,7 +15295,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="445" spans="1:6" ht="29">
+    <row r="445" spans="1:6" ht="45">
       <c r="A445" t="s">
         <v>299</v>
       </c>
@@ -15219,7 +15315,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="446" spans="1:6" ht="29">
+    <row r="446" spans="1:6" ht="30">
       <c r="A446" t="s">
         <v>299</v>
       </c>
@@ -15239,7 +15335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="447" spans="1:6" ht="58">
+    <row r="447" spans="1:6" ht="60">
       <c r="A447" t="s">
         <v>299</v>
       </c>
@@ -15259,7 +15355,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="448" spans="1:6" ht="43.5">
+    <row r="448" spans="1:6" ht="45">
       <c r="A448" t="s">
         <v>299</v>
       </c>
@@ -15279,7 +15375,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="449" spans="1:6" ht="43.5">
+    <row r="449" spans="1:6" ht="45">
       <c r="A449" t="s">
         <v>299</v>
       </c>
@@ -15299,7 +15395,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="450" spans="1:6" ht="58">
+    <row r="450" spans="1:6" ht="60">
       <c r="A450" t="s">
         <v>299</v>
       </c>
@@ -15319,7 +15415,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="451" spans="1:6" ht="58">
+    <row r="451" spans="1:6" ht="60">
       <c r="A451" t="s">
         <v>299</v>
       </c>
@@ -15339,7 +15435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="452" spans="1:6" ht="58">
+    <row r="452" spans="1:6" ht="60">
       <c r="A452" t="s">
         <v>299</v>
       </c>
@@ -15359,7 +15455,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="453" spans="1:6" ht="58">
+    <row r="453" spans="1:6" ht="60">
       <c r="A453" t="s">
         <v>299</v>
       </c>
@@ -15379,7 +15475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="454" spans="1:6" ht="43.5">
+    <row r="454" spans="1:6" ht="45">
       <c r="A454" t="s">
         <v>299</v>
       </c>
@@ -15399,7 +15495,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="455" spans="1:6" ht="58">
+    <row r="455" spans="1:6" ht="75">
       <c r="A455" t="s">
         <v>299</v>
       </c>
@@ -15419,7 +15515,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="456" spans="1:6" ht="58">
+    <row r="456" spans="1:6" ht="75">
       <c r="A456" t="s">
         <v>299</v>
       </c>
@@ -15439,7 +15535,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="457" spans="1:6" ht="29">
+    <row r="457" spans="1:6" ht="30">
       <c r="A457" t="s">
         <v>299</v>
       </c>
@@ -15459,7 +15555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="458" spans="1:6" ht="72.5">
+    <row r="458" spans="1:6" ht="75">
       <c r="A458" t="s">
         <v>299</v>
       </c>
@@ -15479,7 +15575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="459" spans="1:6" ht="72.5">
+    <row r="459" spans="1:6" ht="75">
       <c r="A459" t="s">
         <v>299</v>
       </c>
@@ -15499,7 +15595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="460" spans="1:6" ht="58">
+    <row r="460" spans="1:6" ht="60">
       <c r="A460" t="s">
         <v>299</v>
       </c>
@@ -15519,7 +15615,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="461" spans="1:6" ht="43.5">
+    <row r="461" spans="1:6" ht="45">
       <c r="A461" t="s">
         <v>299</v>
       </c>
@@ -15539,7 +15635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="462" spans="1:6" ht="43.5">
+    <row r="462" spans="1:6" ht="45">
       <c r="A462" t="s">
         <v>299</v>
       </c>
@@ -15559,7 +15655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="463" spans="1:6" ht="43.5">
+    <row r="463" spans="1:6" ht="45">
       <c r="A463" t="s">
         <v>299</v>
       </c>
@@ -15579,7 +15675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="464" spans="1:6" ht="43.5">
+    <row r="464" spans="1:6" ht="45">
       <c r="A464" t="s">
         <v>299</v>
       </c>
@@ -15599,7 +15695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="465" spans="1:6" ht="29">
+    <row r="465" spans="1:6" ht="30">
       <c r="A465" t="s">
         <v>299</v>
       </c>
@@ -15619,7 +15715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="466" spans="1:6" ht="58">
+    <row r="466" spans="1:6" ht="60">
       <c r="A466" t="s">
         <v>299</v>
       </c>
@@ -15639,7 +15735,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="467" spans="1:6" ht="29">
+    <row r="467" spans="1:6" ht="30">
       <c r="A467" s="5" t="s">
         <v>299</v>
       </c>
@@ -15659,7 +15755,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="468" spans="1:6" ht="29">
+    <row r="468" spans="1:6" ht="30">
       <c r="A468" t="s">
         <v>299</v>
       </c>
@@ -15679,7 +15775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="469" spans="1:6" ht="43.5">
+    <row r="469" spans="1:6" ht="45">
       <c r="A469" t="s">
         <v>299</v>
       </c>
@@ -15699,7 +15795,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="470" spans="1:6" ht="43.5">
+    <row r="470" spans="1:6" ht="60">
       <c r="A470" t="s">
         <v>299</v>
       </c>
@@ -15719,7 +15815,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="471" spans="1:6" ht="58">
+    <row r="471" spans="1:6" ht="60">
       <c r="A471" t="s">
         <v>299</v>
       </c>
@@ -15799,7 +15895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="475" spans="1:6" ht="29">
+    <row r="475" spans="1:6" ht="45">
       <c r="A475" t="s">
         <v>299</v>
       </c>
@@ -15819,7 +15915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="476" spans="1:6" ht="29">
+    <row r="476" spans="1:6" ht="45">
       <c r="A476" t="s">
         <v>299</v>
       </c>
@@ -15839,7 +15935,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="477" spans="1:6" ht="29">
+    <row r="477" spans="1:6" ht="45">
       <c r="A477" t="s">
         <v>299</v>
       </c>
@@ -15859,7 +15955,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="478" spans="1:6" ht="43.5">
+    <row r="478" spans="1:6" ht="45">
       <c r="A478" t="s">
         <v>299</v>
       </c>
@@ -15879,7 +15975,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="479" spans="1:6" ht="43.5">
+    <row r="479" spans="1:6" ht="45">
       <c r="A479" t="s">
         <v>299</v>
       </c>
@@ -15899,7 +15995,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="480" spans="1:6" ht="29">
+    <row r="480" spans="1:6" ht="30">
       <c r="A480" t="s">
         <v>299</v>
       </c>
@@ -15919,7 +16015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="481" spans="1:6">
+    <row r="481" spans="1:6" ht="30">
       <c r="A481" t="s">
         <v>299</v>
       </c>
@@ -16019,7 +16115,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="486" spans="1:6" ht="43.5">
+    <row r="486" spans="1:6" ht="45">
       <c r="A486" t="s">
         <v>299</v>
       </c>
@@ -16059,7 +16155,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="488" spans="1:6" ht="29">
+    <row r="488" spans="1:6" ht="45">
       <c r="A488" t="s">
         <v>299</v>
       </c>
@@ -16079,7 +16175,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="489" spans="1:6" ht="58">
+    <row r="489" spans="1:6" ht="60">
       <c r="A489" t="s">
         <v>299</v>
       </c>
@@ -16099,7 +16195,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="490" spans="1:6" ht="43.5">
+    <row r="490" spans="1:6" ht="45">
       <c r="A490" t="s">
         <v>299</v>
       </c>
@@ -16119,7 +16215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="491" spans="1:6" ht="72.5">
+    <row r="491" spans="1:6" ht="75">
       <c r="A491" t="s">
         <v>299</v>
       </c>
@@ -16139,7 +16235,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="492" spans="1:6" ht="43.5">
+    <row r="492" spans="1:6" ht="60">
       <c r="A492" t="s">
         <v>299</v>
       </c>
@@ -16159,7 +16255,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="493" spans="1:6" ht="43.5">
+    <row r="493" spans="1:6" ht="60">
       <c r="A493" t="s">
         <v>299</v>
       </c>
@@ -16179,7 +16275,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="494" spans="1:6" ht="72.5">
+    <row r="494" spans="1:6" ht="75">
       <c r="A494" t="s">
         <v>299</v>
       </c>
@@ -16199,7 +16295,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="495" spans="1:6" ht="72.5">
+    <row r="495" spans="1:6" ht="90">
       <c r="A495" t="s">
         <v>299</v>
       </c>
@@ -16219,7 +16315,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="496" spans="1:6" ht="58">
+    <row r="496" spans="1:6" ht="75">
       <c r="A496" t="s">
         <v>299</v>
       </c>
@@ -16239,7 +16335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="497" spans="1:6" ht="72.5">
+    <row r="497" spans="1:6" ht="75">
       <c r="A497" t="s">
         <v>299</v>
       </c>
@@ -16259,7 +16355,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="498" spans="1:6" ht="58">
+    <row r="498" spans="1:6" ht="75">
       <c r="A498" t="s">
         <v>299</v>
       </c>
@@ -16279,7 +16375,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="499" spans="1:6" ht="72.5">
+    <row r="499" spans="1:6" ht="75">
       <c r="A499" t="s">
         <v>299</v>
       </c>
@@ -16299,7 +16395,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="500" spans="1:6" ht="58">
+    <row r="500" spans="1:6" ht="60">
       <c r="A500" t="s">
         <v>299</v>
       </c>
@@ -16319,7 +16415,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="501" spans="1:6" ht="72.5">
+    <row r="501" spans="1:6" ht="75">
       <c r="A501" t="s">
         <v>299</v>
       </c>
@@ -16339,7 +16435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="502" spans="1:6" ht="72.5">
+    <row r="502" spans="1:6" ht="75">
       <c r="A502" t="s">
         <v>299</v>
       </c>
@@ -16359,7 +16455,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="503" spans="1:6" ht="43.5">
+    <row r="503" spans="1:6" ht="60">
       <c r="A503" t="s">
         <v>299</v>
       </c>
@@ -16379,7 +16475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="504" spans="1:6" ht="87">
+    <row r="504" spans="1:6" ht="90">
       <c r="A504" t="s">
         <v>299</v>
       </c>
@@ -16399,7 +16495,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="505" spans="1:6" ht="43.5">
+    <row r="505" spans="1:6" ht="60">
       <c r="A505" t="s">
         <v>299</v>
       </c>
@@ -16419,7 +16515,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="506" spans="1:6" ht="58">
+    <row r="506" spans="1:6" ht="75">
       <c r="A506" t="s">
         <v>299</v>
       </c>
@@ -16439,7 +16535,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="507" spans="1:6" ht="58">
+    <row r="507" spans="1:6" ht="90">
       <c r="A507" t="s">
         <v>299</v>
       </c>
@@ -16459,7 +16555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="508" spans="1:6" ht="58">
+    <row r="508" spans="1:6" ht="90">
       <c r="A508" t="s">
         <v>299</v>
       </c>
@@ -16479,7 +16575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="509" spans="1:6" ht="43.5">
+    <row r="509" spans="1:6" ht="75">
       <c r="A509" t="s">
         <v>299</v>
       </c>
@@ -16499,7 +16595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="510" spans="1:6" ht="29">
+    <row r="510" spans="1:6" ht="30">
       <c r="A510" t="s">
         <v>299</v>
       </c>
@@ -16519,7 +16615,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="511" spans="1:6" ht="29">
+    <row r="511" spans="1:6" ht="30">
       <c r="A511" t="s">
         <v>299</v>
       </c>
@@ -16539,7 +16635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="512" spans="1:6" ht="29">
+    <row r="512" spans="1:6" ht="30">
       <c r="A512" t="s">
         <v>299</v>
       </c>
@@ -16559,7 +16655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="513" spans="1:6">
+    <row r="513" spans="1:6" ht="30">
       <c r="A513" t="s">
         <v>299</v>
       </c>
@@ -16579,7 +16675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="514" spans="1:6" ht="29">
+    <row r="514" spans="1:6" ht="30">
       <c r="A514" t="s">
         <v>299</v>
       </c>
@@ -16599,7 +16695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="515" spans="1:6" ht="29">
+    <row r="515" spans="1:6" ht="30">
       <c r="A515" t="s">
         <v>299</v>
       </c>
@@ -56196,6 +56292,486 @@
         <v>1391</v>
       </c>
       <c r="F2494" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2495" spans="1:6">
+      <c r="A2495" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2495" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2495" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D2495" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2495" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2495" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:6">
+      <c r="A2496" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2496" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2496" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D2496" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2496" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2496" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:6">
+      <c r="A2497" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2497" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2497" t="s">
+        <v>1409</v>
+      </c>
+      <c r="D2497" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2497" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2497" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:6">
+      <c r="A2498" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2498" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C2498" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D2498" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2498" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2498" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:6">
+      <c r="A2499" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2499" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C2499" t="s">
+        <v>1411</v>
+      </c>
+      <c r="D2499" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2499" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2499" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:6">
+      <c r="A2500" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2500" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C2500" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D2500" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2500" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2500" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2501" spans="1:6">
+      <c r="A2501" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2501" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C2501" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D2501" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2501" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2501" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2502" spans="1:6">
+      <c r="A2502" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2502" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C2502" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D2502" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2502" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2502" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2503" spans="1:6">
+      <c r="A2503" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2503" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C2503" t="s">
+        <v>1415</v>
+      </c>
+      <c r="D2503" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2503" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2503" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2504" spans="1:6">
+      <c r="A2504" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2504" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C2504" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D2504" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2504" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2504" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2505" spans="1:6">
+      <c r="A2505" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2505" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C2505" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D2505" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2505" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2505" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2506" spans="1:6">
+      <c r="A2506" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2506" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C2506" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D2506" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2506" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2506" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2507" spans="1:6">
+      <c r="A2507" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2507" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2507" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D2507" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2507" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2507" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2508" spans="1:6">
+      <c r="A2508" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2508" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2508" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D2508" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2508" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2508" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2509" spans="1:6">
+      <c r="A2509" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2509" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2509" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D2509" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2509" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2509" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2510" spans="1:6">
+      <c r="A2510" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2510" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C2510" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D2510" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2510" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2510" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2511" spans="1:6">
+      <c r="A2511" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2511" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C2511" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D2511" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2511" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2511" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2512" spans="1:6">
+      <c r="A2512" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2512" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C2512" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D2512" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2512" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2512" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2513" spans="1:6">
+      <c r="A2513" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2513" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C2513" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D2513" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2513" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2513" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2514" spans="1:6">
+      <c r="A2514" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2514" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C2514" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D2514" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2514" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2514" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:6">
+      <c r="A2515" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2515" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C2515" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D2515" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2515" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2515" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:6">
+      <c r="A2516" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2516" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C2516" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D2516" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2516" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2516" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:6">
+      <c r="A2517" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2517" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C2517" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D2517" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2517" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2517" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:6">
+      <c r="A2518" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2518" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C2518" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D2518" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2518" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2518" t="s">
         <v>1392</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MOSIP-40766: Added all new templates in release-1.3.x
Signed-off-by: Swetha K <swetha.k@technoforte.co.in>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FBD232-C82B-47AC-B317-F76556C5A17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A95166E-6361-4800-BC8F-6E5490572258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14964" uniqueCount="1399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15108" uniqueCount="1431">
   <si>
     <t>lang_code</t>
   </si>
@@ -5837,6 +5837,102 @@
   </si>
   <si>
     <t>Authentication positive summary</t>
+  </si>
+  <si>
+    <t>ROOT_CERT_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for root certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle d'expiration du certificat racine</t>
+  </si>
+  <si>
+    <t>نموذج لانتهاء صلاحية شهادة الجذر</t>
+  </si>
+  <si>
+    <t>INTERMEDIATE_CERT_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for intermediate certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle d'expiration de certificat intermédiaire</t>
+  </si>
+  <si>
+    <t>نموذج انتهاء صلاحية الشهادة المتوسطة</t>
+  </si>
+  <si>
+    <t>PARTNER_CERT_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for partner certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle d'expiration du certificat de partenaire</t>
+  </si>
+  <si>
+    <t>نموذج انتهاء صلاحية شهادة الشريك</t>
+  </si>
+  <si>
+    <t>WEEKLY_SUMMARY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for weekly summary notifications</t>
+  </si>
+  <si>
+    <t>Modèle pour les notifications récapitulatives hebdomadaires</t>
+  </si>
+  <si>
+    <t>نموذج لإشعارات الملخص الأسبوعية</t>
+  </si>
+  <si>
+    <t>ROOT_CERT_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for root certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du certificat racine</t>
+  </si>
+  <si>
+    <t>نموذج موضوعي لانتهاء صلاحية شهادة الجذر</t>
+  </si>
+  <si>
+    <t>INTERMEDIATE_CERT_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for intermediate certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du certificat intermédiaire</t>
+  </si>
+  <si>
+    <t>نموذج موضوعي لانتهاء صلاحية الشهادة المتوسطة</t>
+  </si>
+  <si>
+    <t>PARTNER_CERT_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for partner certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du certificat du partenaire</t>
+  </si>
+  <si>
+    <t>نموذج موضوعي لانتهاء صلاحية شهادة الشريك</t>
+  </si>
+  <si>
+    <t>WEEKLY_SUMMARY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for weekly summary notifications</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour les notifications récapitulatives hebdomadaires</t>
+  </si>
+  <si>
+    <t>قالب موضوعي لإشعارات الملخص الأسبوعي</t>
   </si>
 </sst>
 </file>
@@ -6305,17 +6401,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2494"/>
+  <dimension ref="A1:F2518"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2478" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2493" sqref="B2493"/>
+    <sheetView tabSelected="1" topLeftCell="A2502" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2495" sqref="B2495"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" customWidth="1"/>
-    <col min="2" max="2" width="40.453125" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="27" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6879,7 +6975,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28.5">
+    <row r="29" spans="1:6" ht="29.25">
       <c r="A29" t="s">
         <v>291</v>
       </c>
@@ -6919,7 +7015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" ht="29.25">
       <c r="A31" t="s">
         <v>291</v>
       </c>
@@ -6959,7 +7055,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.5">
+    <row r="33" spans="1:6" ht="29.25">
       <c r="A33" t="s">
         <v>291</v>
       </c>
@@ -7359,7 +7455,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.5">
+    <row r="53" spans="1:6" ht="29.25">
       <c r="A53" t="s">
         <v>291</v>
       </c>
@@ -7379,7 +7475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="28.5">
+    <row r="54" spans="1:6" ht="29.25">
       <c r="A54" t="s">
         <v>291</v>
       </c>
@@ -7419,7 +7515,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="28.5">
+    <row r="56" spans="1:6" ht="29.25">
       <c r="A56" t="s">
         <v>291</v>
       </c>
@@ -7439,7 +7535,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="29">
+    <row r="57" spans="1:6" ht="30">
       <c r="A57" t="s">
         <v>291</v>
       </c>
@@ -7479,7 +7575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="28.5">
+    <row r="59" spans="1:6" ht="29.25">
       <c r="A59" t="s">
         <v>291</v>
       </c>
@@ -7499,7 +7595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="28.5">
+    <row r="60" spans="1:6" ht="29.25">
       <c r="A60" t="s">
         <v>291</v>
       </c>
@@ -7799,7 +7895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" ht="29.25">
       <c r="A75" t="s">
         <v>291</v>
       </c>
@@ -7819,7 +7915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="28.5">
+    <row r="76" spans="1:6" ht="29.25">
       <c r="A76" t="s">
         <v>291</v>
       </c>
@@ -7839,7 +7935,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="28.5">
+    <row r="77" spans="1:6" ht="29.25">
       <c r="A77" t="s">
         <v>291</v>
       </c>
@@ -7939,7 +8035,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="28.5">
+    <row r="82" spans="1:6" ht="29.25">
       <c r="A82" t="s">
         <v>291</v>
       </c>
@@ -8119,7 +8215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="28.5">
+    <row r="91" spans="1:6" ht="29.25">
       <c r="A91" t="s">
         <v>291</v>
       </c>
@@ -8239,7 +8335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="29">
+    <row r="97" spans="1:6" ht="30">
       <c r="A97" t="s">
         <v>291</v>
       </c>
@@ -8479,7 +8575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="28.5">
+    <row r="109" spans="1:6" ht="29.25">
       <c r="A109" t="s">
         <v>291</v>
       </c>
@@ -8539,7 +8635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="28.5">
+    <row r="112" spans="1:6" ht="29.25">
       <c r="A112" t="s">
         <v>291</v>
       </c>
@@ -8719,7 +8815,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" ht="30">
       <c r="A121" t="s">
         <v>291</v>
       </c>
@@ -9199,7 +9295,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="29">
+    <row r="145" spans="1:6" ht="30">
       <c r="A145" t="s">
         <v>291</v>
       </c>
@@ -9259,7 +9355,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="28.5">
+    <row r="148" spans="1:6" ht="29.25">
       <c r="A148" t="s">
         <v>291</v>
       </c>
@@ -9319,7 +9415,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="29">
+    <row r="151" spans="1:6" ht="30">
       <c r="A151" t="s">
         <v>291</v>
       </c>
@@ -9379,7 +9475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="28.5">
+    <row r="154" spans="1:6" ht="29.25">
       <c r="A154" t="s">
         <v>291</v>
       </c>
@@ -9439,7 +9535,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="28.5">
+    <row r="157" spans="1:6" ht="29.25">
       <c r="A157" t="s">
         <v>291</v>
       </c>
@@ -9499,7 +9595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="28.5">
+    <row r="160" spans="1:6" ht="29.25">
       <c r="A160" t="s">
         <v>291</v>
       </c>
@@ -9559,7 +9655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="29">
+    <row r="163" spans="1:6" ht="30">
       <c r="A163" t="s">
         <v>291</v>
       </c>
@@ -9619,7 +9715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="28.5">
+    <row r="166" spans="1:6" ht="29.25">
       <c r="A166" t="s">
         <v>291</v>
       </c>
@@ -9679,7 +9775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="29">
+    <row r="169" spans="1:6" ht="30">
       <c r="A169" t="s">
         <v>291</v>
       </c>
@@ -9739,7 +9835,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="42.5">
+    <row r="172" spans="1:6" ht="43.5">
       <c r="A172" t="s">
         <v>291</v>
       </c>
@@ -9799,7 +9895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="29">
+    <row r="175" spans="1:6" ht="30">
       <c r="A175" t="s">
         <v>291</v>
       </c>
@@ -9859,7 +9955,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="28.5">
+    <row r="178" spans="1:6" ht="29.25">
       <c r="A178" t="s">
         <v>291</v>
       </c>
@@ -9919,7 +10015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="29">
+    <row r="181" spans="1:6" ht="30">
       <c r="A181" t="s">
         <v>291</v>
       </c>
@@ -9979,7 +10075,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="28.5">
+    <row r="184" spans="1:6" ht="29.25">
       <c r="A184" t="s">
         <v>291</v>
       </c>
@@ -10039,7 +10135,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="43">
+    <row r="187" spans="1:6" ht="44.25">
       <c r="A187" t="s">
         <v>291</v>
       </c>
@@ -10099,7 +10195,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="28.5">
+    <row r="190" spans="1:6" ht="29.25">
       <c r="A190" t="s">
         <v>291</v>
       </c>
@@ -10159,7 +10255,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="28.5">
+    <row r="193" spans="1:6" ht="29.25">
       <c r="A193" t="s">
         <v>291</v>
       </c>
@@ -10219,7 +10315,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="28.5">
+    <row r="196" spans="1:6" ht="29.25">
       <c r="A196" t="s">
         <v>291</v>
       </c>
@@ -10279,7 +10375,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="42.5">
+    <row r="199" spans="1:6" ht="43.5">
       <c r="A199" t="s">
         <v>291</v>
       </c>
@@ -10339,7 +10435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="42.5">
+    <row r="202" spans="1:6" ht="43.5">
       <c r="A202" t="s">
         <v>291</v>
       </c>
@@ -10399,7 +10495,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="28.5">
+    <row r="205" spans="1:6" ht="29.25">
       <c r="A205" t="s">
         <v>291</v>
       </c>
@@ -10459,7 +10555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="42.5">
+    <row r="208" spans="1:6" ht="43.5">
       <c r="A208" t="s">
         <v>291</v>
       </c>
@@ -10999,7 +11095,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="28.5">
+    <row r="235" spans="1:6" ht="29.25">
       <c r="A235" t="s">
         <v>291</v>
       </c>
@@ -11059,7 +11155,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="28.5">
+    <row r="238" spans="1:6" ht="29.25">
       <c r="A238" t="s">
         <v>291</v>
       </c>
@@ -11119,7 +11215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="28.5">
+    <row r="241" spans="1:6" ht="29.25">
       <c r="A241" t="s">
         <v>291</v>
       </c>
@@ -11179,7 +11275,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="244" spans="1:6">
+    <row r="244" spans="1:6" ht="29.25">
       <c r="A244" t="s">
         <v>291</v>
       </c>
@@ -11479,7 +11575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="28.5">
+    <row r="259" spans="1:6" ht="29.25">
       <c r="A259" t="s">
         <v>291</v>
       </c>
@@ -11559,7 +11655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="29">
+    <row r="263" spans="1:6" ht="30">
       <c r="A263" t="s">
         <v>297</v>
       </c>
@@ -11579,7 +11675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="29">
+    <row r="264" spans="1:6" ht="30">
       <c r="A264" t="s">
         <v>297</v>
       </c>
@@ -11599,7 +11695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="265" spans="1:6" ht="29">
+    <row r="265" spans="1:6" ht="30">
       <c r="A265" t="s">
         <v>297</v>
       </c>
@@ -11619,7 +11715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="266" spans="1:6" ht="29">
+    <row r="266" spans="1:6" ht="30">
       <c r="A266" t="s">
         <v>297</v>
       </c>
@@ -11639,7 +11735,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="267" spans="1:6" ht="29">
+    <row r="267" spans="1:6" ht="30">
       <c r="A267" t="s">
         <v>297</v>
       </c>
@@ -11659,7 +11755,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="268" spans="1:6" ht="29">
+    <row r="268" spans="1:6" ht="30">
       <c r="A268" t="s">
         <v>297</v>
       </c>
@@ -11679,7 +11775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="269" spans="1:6" ht="29">
+    <row r="269" spans="1:6" ht="30">
       <c r="A269" t="s">
         <v>297</v>
       </c>
@@ -11699,7 +11795,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="270" spans="1:6" ht="29">
+    <row r="270" spans="1:6" ht="30">
       <c r="A270" t="s">
         <v>297</v>
       </c>
@@ -11719,7 +11815,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="271" spans="1:6" ht="29">
+    <row r="271" spans="1:6" ht="30">
       <c r="A271" t="s">
         <v>297</v>
       </c>
@@ -11739,7 +11835,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="272" spans="1:6" ht="29">
+    <row r="272" spans="1:6" ht="45">
       <c r="A272" t="s">
         <v>297</v>
       </c>
@@ -11759,7 +11855,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="273" spans="1:6" ht="29">
+    <row r="273" spans="1:6" ht="45">
       <c r="A273" t="s">
         <v>297</v>
       </c>
@@ -11779,7 +11875,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="274" spans="1:6" ht="43.5">
+    <row r="274" spans="1:6" ht="45">
       <c r="A274" t="s">
         <v>297</v>
       </c>
@@ -11799,7 +11895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="275" spans="1:6" ht="43.5">
+    <row r="275" spans="1:6" ht="45">
       <c r="A275" t="s">
         <v>297</v>
       </c>
@@ -11819,7 +11915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="276" spans="1:6" ht="29">
+    <row r="276" spans="1:6" ht="30">
       <c r="A276" t="s">
         <v>297</v>
       </c>
@@ -11839,7 +11935,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="277" spans="1:6" ht="29">
+    <row r="277" spans="1:6" ht="30">
       <c r="A277" t="s">
         <v>297</v>
       </c>
@@ -11859,7 +11955,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="278" spans="1:6" ht="29">
+    <row r="278" spans="1:6" ht="30">
       <c r="A278" t="s">
         <v>297</v>
       </c>
@@ -11899,7 +11995,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="280" spans="1:6" ht="43.5">
+    <row r="280" spans="1:6" ht="60">
       <c r="A280" t="s">
         <v>297</v>
       </c>
@@ -11919,7 +12015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="281" spans="1:6" ht="43.5">
+    <row r="281" spans="1:6" ht="60">
       <c r="A281" t="s">
         <v>297</v>
       </c>
@@ -11939,7 +12035,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="282" spans="1:6" ht="43.5">
+    <row r="282" spans="1:6" ht="45">
       <c r="A282" t="s">
         <v>297</v>
       </c>
@@ -11959,7 +12055,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="283" spans="1:6" ht="29">
+    <row r="283" spans="1:6" ht="30">
       <c r="A283" t="s">
         <v>297</v>
       </c>
@@ -11979,7 +12075,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="284" spans="1:6" ht="29">
+    <row r="284" spans="1:6" ht="30">
       <c r="A284" t="s">
         <v>297</v>
       </c>
@@ -11999,7 +12095,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="285" spans="1:6" ht="29">
+    <row r="285" spans="1:6" ht="30">
       <c r="A285" t="s">
         <v>297</v>
       </c>
@@ -12019,7 +12115,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="286" spans="1:6" ht="29">
+    <row r="286" spans="1:6" ht="30">
       <c r="A286" t="s">
         <v>297</v>
       </c>
@@ -12059,7 +12155,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="288" spans="1:6" ht="29">
+    <row r="288" spans="1:6" ht="30">
       <c r="A288" t="s">
         <v>297</v>
       </c>
@@ -12079,7 +12175,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="289" spans="1:6" ht="29">
+    <row r="289" spans="1:6" ht="30">
       <c r="A289" t="s">
         <v>297</v>
       </c>
@@ -12099,7 +12195,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="15">
+    <row r="290" spans="1:6">
       <c r="A290" s="5" t="s">
         <v>297</v>
       </c>
@@ -12119,7 +12215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="291" spans="1:6" ht="29">
+    <row r="291" spans="1:6" ht="45">
       <c r="A291" t="s">
         <v>297</v>
       </c>
@@ -12139,7 +12235,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="29">
+    <row r="292" spans="1:6" ht="30">
       <c r="A292" t="s">
         <v>297</v>
       </c>
@@ -12159,7 +12255,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="293" spans="1:6" ht="29">
+    <row r="293" spans="1:6" ht="45">
       <c r="A293" t="s">
         <v>297</v>
       </c>
@@ -12179,7 +12275,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="294" spans="1:6" ht="43.5">
+    <row r="294" spans="1:6" ht="45">
       <c r="A294" t="s">
         <v>297</v>
       </c>
@@ -12239,7 +12335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="297" spans="1:6" ht="29">
+    <row r="297" spans="1:6" ht="30">
       <c r="A297" t="s">
         <v>297</v>
       </c>
@@ -12259,7 +12355,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="298" spans="1:6" ht="29">
+    <row r="298" spans="1:6" ht="30">
       <c r="A298" t="s">
         <v>297</v>
       </c>
@@ -12279,7 +12375,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="299" spans="1:6" ht="29">
+    <row r="299" spans="1:6" ht="30">
       <c r="A299" t="s">
         <v>297</v>
       </c>
@@ -12299,7 +12395,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="29">
+    <row r="300" spans="1:6" ht="30">
       <c r="A300" t="s">
         <v>297</v>
       </c>
@@ -12319,7 +12415,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="29">
+    <row r="301" spans="1:6" ht="30">
       <c r="A301" t="s">
         <v>297</v>
       </c>
@@ -12339,7 +12435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="302" spans="1:6" ht="29">
+    <row r="302" spans="1:6" ht="30">
       <c r="A302" t="s">
         <v>297</v>
       </c>
@@ -12459,7 +12555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="29">
+    <row r="308" spans="1:6" ht="45">
       <c r="A308" t="s">
         <v>297</v>
       </c>
@@ -12479,7 +12575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="29">
+    <row r="309" spans="1:6" ht="30">
       <c r="A309" t="s">
         <v>297</v>
       </c>
@@ -12499,7 +12595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="310" spans="1:6" ht="29">
+    <row r="310" spans="1:6" ht="30">
       <c r="A310" t="s">
         <v>297</v>
       </c>
@@ -12519,7 +12615,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="311" spans="1:6" ht="43.5">
+    <row r="311" spans="1:6" ht="45">
       <c r="A311" t="s">
         <v>297</v>
       </c>
@@ -12539,7 +12635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="312" spans="1:6" ht="43.5">
+    <row r="312" spans="1:6" ht="45">
       <c r="A312" t="s">
         <v>297</v>
       </c>
@@ -12559,7 +12655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="313" spans="1:6" ht="43.5">
+    <row r="313" spans="1:6" ht="60">
       <c r="A313" t="s">
         <v>297</v>
       </c>
@@ -12579,7 +12675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="43.5">
+    <row r="314" spans="1:6" ht="60">
       <c r="A314" t="s">
         <v>297</v>
       </c>
@@ -12599,7 +12695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="315" spans="1:6" ht="43.5">
+    <row r="315" spans="1:6" ht="45">
       <c r="A315" t="s">
         <v>297</v>
       </c>
@@ -12619,7 +12715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="316" spans="1:6" ht="43.5">
+    <row r="316" spans="1:6" ht="45">
       <c r="A316" t="s">
         <v>297</v>
       </c>
@@ -12639,7 +12735,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="317" spans="1:6" ht="43.5">
+    <row r="317" spans="1:6" ht="60">
       <c r="A317" t="s">
         <v>297</v>
       </c>
@@ -12659,7 +12755,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="318" spans="1:6" ht="43.5">
+    <row r="318" spans="1:6" ht="45">
       <c r="A318" t="s">
         <v>297</v>
       </c>
@@ -12679,7 +12775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="319" spans="1:6" ht="43.5">
+    <row r="319" spans="1:6" ht="60">
       <c r="A319" t="s">
         <v>297</v>
       </c>
@@ -12719,7 +12815,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="321" spans="1:6" ht="43.5">
+    <row r="321" spans="1:6" ht="60">
       <c r="A321" t="s">
         <v>297</v>
       </c>
@@ -12739,7 +12835,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="322" spans="1:6" ht="43.5">
+    <row r="322" spans="1:6" ht="60">
       <c r="A322" t="s">
         <v>297</v>
       </c>
@@ -12759,7 +12855,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="323" spans="1:6" ht="43.5">
+    <row r="323" spans="1:6" ht="60">
       <c r="A323" t="s">
         <v>297</v>
       </c>
@@ -12779,7 +12875,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="324" spans="1:6" ht="43.5">
+    <row r="324" spans="1:6" ht="45">
       <c r="A324" t="s">
         <v>297</v>
       </c>
@@ -12799,7 +12895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="325" spans="1:6" ht="43.5">
+    <row r="325" spans="1:6" ht="45">
       <c r="A325" t="s">
         <v>297</v>
       </c>
@@ -12819,7 +12915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="326" spans="1:6" ht="43.5">
+    <row r="326" spans="1:6" ht="60">
       <c r="A326" t="s">
         <v>297</v>
       </c>
@@ -12839,7 +12935,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="43.5">
+    <row r="327" spans="1:6" ht="45">
       <c r="A327" t="s">
         <v>297</v>
       </c>
@@ -12859,7 +12955,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="43.5">
+    <row r="328" spans="1:6" ht="60">
       <c r="A328" t="s">
         <v>297</v>
       </c>
@@ -12879,7 +12975,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="329" spans="1:6" ht="43.5">
+    <row r="329" spans="1:6" ht="60">
       <c r="A329" t="s">
         <v>297</v>
       </c>
@@ -12899,7 +12995,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="330" spans="1:6" ht="43.5">
+    <row r="330" spans="1:6" ht="60">
       <c r="A330" t="s">
         <v>297</v>
       </c>
@@ -12919,7 +13015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="331" spans="1:6" ht="43.5">
+    <row r="331" spans="1:6" ht="45">
       <c r="A331" t="s">
         <v>297</v>
       </c>
@@ -12939,7 +13035,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="332" spans="1:6" ht="29">
+    <row r="332" spans="1:6" ht="30">
       <c r="A332" t="s">
         <v>297</v>
       </c>
@@ -12959,7 +13055,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="333" spans="1:6" ht="29">
+    <row r="333" spans="1:6" ht="45">
       <c r="A333" t="s">
         <v>297</v>
       </c>
@@ -12979,7 +13075,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="334" spans="1:6" ht="29">
+    <row r="334" spans="1:6" ht="30">
       <c r="A334" t="s">
         <v>297</v>
       </c>
@@ -12999,7 +13095,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="335" spans="1:6" ht="29">
+    <row r="335" spans="1:6" ht="30">
       <c r="A335" t="s">
         <v>297</v>
       </c>
@@ -13019,7 +13115,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="336" spans="1:6" ht="29">
+    <row r="336" spans="1:6" ht="30">
       <c r="A336" t="s">
         <v>297</v>
       </c>
@@ -13039,7 +13135,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="337" spans="1:6" ht="29">
+    <row r="337" spans="1:6" ht="30">
       <c r="A337" t="s">
         <v>297</v>
       </c>
@@ -13239,7 +13335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="347" spans="1:6" ht="29">
+    <row r="347" spans="1:6" ht="30">
       <c r="A347" t="s">
         <v>297</v>
       </c>
@@ -13339,7 +13435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="352" spans="1:6" ht="29">
+    <row r="352" spans="1:6" ht="30">
       <c r="A352" t="s">
         <v>298</v>
       </c>
@@ -13359,7 +13455,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="353" spans="1:6" ht="29">
+    <row r="353" spans="1:6" ht="30">
       <c r="A353" t="s">
         <v>298</v>
       </c>
@@ -13379,7 +13475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="354" spans="1:6" ht="29">
+    <row r="354" spans="1:6" ht="30">
       <c r="A354" t="s">
         <v>298</v>
       </c>
@@ -13399,7 +13495,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="355" spans="1:6" ht="29">
+    <row r="355" spans="1:6" ht="30">
       <c r="A355" t="s">
         <v>298</v>
       </c>
@@ -13419,7 +13515,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="356" spans="1:6" ht="29">
+    <row r="356" spans="1:6" ht="30">
       <c r="A356" t="s">
         <v>298</v>
       </c>
@@ -13459,7 +13555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="358" spans="1:6" ht="29">
+    <row r="358" spans="1:6" ht="30">
       <c r="A358" t="s">
         <v>298</v>
       </c>
@@ -13479,7 +13575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="359" spans="1:6" ht="29">
+    <row r="359" spans="1:6" ht="30">
       <c r="A359" t="s">
         <v>298</v>
       </c>
@@ -13499,7 +13595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="360" spans="1:6" ht="29">
+    <row r="360" spans="1:6" ht="30">
       <c r="A360" t="s">
         <v>298</v>
       </c>
@@ -13519,7 +13615,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="361" spans="1:6" ht="29">
+    <row r="361" spans="1:6" ht="30">
       <c r="A361" t="s">
         <v>298</v>
       </c>
@@ -13539,7 +13635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="362" spans="1:6" ht="29">
+    <row r="362" spans="1:6" ht="30">
       <c r="A362" t="s">
         <v>298</v>
       </c>
@@ -13559,7 +13655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="363" spans="1:6" ht="29">
+    <row r="363" spans="1:6" ht="30">
       <c r="A363" t="s">
         <v>298</v>
       </c>
@@ -13579,7 +13675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="364" spans="1:6" ht="29">
+    <row r="364" spans="1:6" ht="30">
       <c r="A364" t="s">
         <v>298</v>
       </c>
@@ -13599,7 +13695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="365" spans="1:6" ht="29">
+    <row r="365" spans="1:6" ht="30">
       <c r="A365" t="s">
         <v>298</v>
       </c>
@@ -13619,7 +13715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="366" spans="1:6" ht="29">
+    <row r="366" spans="1:6" ht="30">
       <c r="A366" t="s">
         <v>298</v>
       </c>
@@ -13639,7 +13735,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="367" spans="1:6" ht="29">
+    <row r="367" spans="1:6" ht="30">
       <c r="A367" t="s">
         <v>298</v>
       </c>
@@ -13659,7 +13755,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="368" spans="1:6" ht="29">
+    <row r="368" spans="1:6" ht="30">
       <c r="A368" t="s">
         <v>298</v>
       </c>
@@ -13679,7 +13775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="369" spans="1:6" ht="29">
+    <row r="369" spans="1:6" ht="30">
       <c r="A369" t="s">
         <v>298</v>
       </c>
@@ -13699,7 +13795,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="370" spans="1:6" ht="29">
+    <row r="370" spans="1:6" ht="30">
       <c r="A370" t="s">
         <v>298</v>
       </c>
@@ -13719,7 +13815,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="371" spans="1:6" ht="29">
+    <row r="371" spans="1:6" ht="30">
       <c r="A371" t="s">
         <v>298</v>
       </c>
@@ -13739,7 +13835,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="372" spans="1:6">
+    <row r="372" spans="1:6" ht="30">
       <c r="A372" t="s">
         <v>298</v>
       </c>
@@ -13759,7 +13855,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="29">
+    <row r="373" spans="1:6" ht="30">
       <c r="A373" t="s">
         <v>298</v>
       </c>
@@ -13779,7 +13875,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="374" spans="1:6" ht="29">
+    <row r="374" spans="1:6" ht="30">
       <c r="A374" t="s">
         <v>298</v>
       </c>
@@ -13799,7 +13895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="375" spans="1:6" ht="29">
+    <row r="375" spans="1:6" ht="30">
       <c r="A375" t="s">
         <v>298</v>
       </c>
@@ -13819,7 +13915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="376" spans="1:6" ht="29">
+    <row r="376" spans="1:6" ht="30">
       <c r="A376" t="s">
         <v>298</v>
       </c>
@@ -13839,7 +13935,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="377" spans="1:6" ht="29">
+    <row r="377" spans="1:6" ht="30">
       <c r="A377" t="s">
         <v>298</v>
       </c>
@@ -13859,7 +13955,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="378" spans="1:6" ht="29">
+    <row r="378" spans="1:6" ht="30">
       <c r="A378" t="s">
         <v>298</v>
       </c>
@@ -13899,7 +13995,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="380" spans="1:6" ht="29">
+    <row r="380" spans="1:6" ht="30">
       <c r="A380" t="s">
         <v>298</v>
       </c>
@@ -13919,7 +14015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="381" spans="1:6" ht="29">
+    <row r="381" spans="1:6" ht="30">
       <c r="A381" t="s">
         <v>298</v>
       </c>
@@ -13939,7 +14035,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="382" spans="1:6" ht="29">
+    <row r="382" spans="1:6" ht="30">
       <c r="A382" t="s">
         <v>298</v>
       </c>
@@ -13959,7 +14055,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="383" spans="1:6" ht="29">
+    <row r="383" spans="1:6" ht="30">
       <c r="A383" t="s">
         <v>298</v>
       </c>
@@ -14039,7 +14135,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="387" spans="1:6" ht="29">
+    <row r="387" spans="1:6" ht="30">
       <c r="A387" t="s">
         <v>298</v>
       </c>
@@ -14059,7 +14155,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="388" spans="1:6" ht="29">
+    <row r="388" spans="1:6" ht="30">
       <c r="A388" t="s">
         <v>298</v>
       </c>
@@ -14079,7 +14175,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="389" spans="1:6">
+    <row r="389" spans="1:6" ht="30">
       <c r="A389" t="s">
         <v>298</v>
       </c>
@@ -14099,7 +14195,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="390" spans="1:6">
+    <row r="390" spans="1:6" ht="30">
       <c r="A390" t="s">
         <v>298</v>
       </c>
@@ -14119,7 +14215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="391" spans="1:6" ht="29">
+    <row r="391" spans="1:6" ht="30">
       <c r="A391" t="s">
         <v>298</v>
       </c>
@@ -14239,7 +14335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="397" spans="1:6" ht="29">
+    <row r="397" spans="1:6" ht="30">
       <c r="A397" t="s">
         <v>298</v>
       </c>
@@ -14259,7 +14355,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="398" spans="1:6" ht="29">
+    <row r="398" spans="1:6" ht="30">
       <c r="A398" t="s">
         <v>298</v>
       </c>
@@ -14279,7 +14375,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="399" spans="1:6">
+    <row r="399" spans="1:6" ht="30">
       <c r="A399" t="s">
         <v>298</v>
       </c>
@@ -14299,7 +14395,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="400" spans="1:6" ht="29">
+    <row r="400" spans="1:6" ht="30">
       <c r="A400" t="s">
         <v>298</v>
       </c>
@@ -14319,7 +14415,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="401" spans="1:6" ht="29">
+    <row r="401" spans="1:6" ht="30">
       <c r="A401" t="s">
         <v>298</v>
       </c>
@@ -14339,7 +14435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="402" spans="1:6" ht="29">
+    <row r="402" spans="1:6" ht="30">
       <c r="A402" t="s">
         <v>298</v>
       </c>
@@ -14359,7 +14455,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="403" spans="1:6" ht="29">
+    <row r="403" spans="1:6" ht="30">
       <c r="A403" t="s">
         <v>298</v>
       </c>
@@ -14379,7 +14475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="404" spans="1:6" ht="29">
+    <row r="404" spans="1:6" ht="30">
       <c r="A404" t="s">
         <v>298</v>
       </c>
@@ -14399,7 +14495,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="405" spans="1:6" ht="29">
+    <row r="405" spans="1:6" ht="30">
       <c r="A405" t="s">
         <v>298</v>
       </c>
@@ -14419,7 +14515,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="406" spans="1:6" ht="29">
+    <row r="406" spans="1:6" ht="30">
       <c r="A406" t="s">
         <v>298</v>
       </c>
@@ -14439,7 +14535,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="407" spans="1:6" ht="29">
+    <row r="407" spans="1:6" ht="30">
       <c r="A407" t="s">
         <v>298</v>
       </c>
@@ -14459,7 +14555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="408" spans="1:6" ht="29">
+    <row r="408" spans="1:6" ht="45">
       <c r="A408" t="s">
         <v>298</v>
       </c>
@@ -14479,7 +14575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="409" spans="1:6" ht="29">
+    <row r="409" spans="1:6" ht="30">
       <c r="A409" t="s">
         <v>298</v>
       </c>
@@ -14499,7 +14595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="410" spans="1:6" ht="29">
+    <row r="410" spans="1:6" ht="30">
       <c r="A410" t="s">
         <v>298</v>
       </c>
@@ -14519,7 +14615,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="411" spans="1:6" ht="29">
+    <row r="411" spans="1:6" ht="30">
       <c r="A411" t="s">
         <v>298</v>
       </c>
@@ -14539,7 +14635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="412" spans="1:6" ht="29">
+    <row r="412" spans="1:6" ht="30">
       <c r="A412" t="s">
         <v>298</v>
       </c>
@@ -14559,7 +14655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="413" spans="1:6" ht="43.5">
+    <row r="413" spans="1:6" ht="45">
       <c r="A413" t="s">
         <v>298</v>
       </c>
@@ -14579,7 +14675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="414" spans="1:6" ht="29">
+    <row r="414" spans="1:6" ht="30">
       <c r="A414" t="s">
         <v>298</v>
       </c>
@@ -14599,7 +14695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="415" spans="1:6" ht="43.5">
+    <row r="415" spans="1:6" ht="45">
       <c r="A415" t="s">
         <v>298</v>
       </c>
@@ -14619,7 +14715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="416" spans="1:6" ht="29">
+    <row r="416" spans="1:6" ht="30">
       <c r="A416" t="s">
         <v>298</v>
       </c>
@@ -14639,7 +14735,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="417" spans="1:6" ht="29">
+    <row r="417" spans="1:6" ht="30">
       <c r="A417" t="s">
         <v>298</v>
       </c>
@@ -14659,7 +14755,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="418" spans="1:6" ht="29">
+    <row r="418" spans="1:6" ht="30">
       <c r="A418" t="s">
         <v>298</v>
       </c>
@@ -14679,7 +14775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="419" spans="1:6" ht="29">
+    <row r="419" spans="1:6" ht="30">
       <c r="A419" t="s">
         <v>298</v>
       </c>
@@ -14699,7 +14795,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="420" spans="1:6" ht="29">
+    <row r="420" spans="1:6" ht="30">
       <c r="A420" t="s">
         <v>298</v>
       </c>
@@ -14739,7 +14835,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="422" spans="1:6" ht="29">
+    <row r="422" spans="1:6" ht="30">
       <c r="A422" t="s">
         <v>298</v>
       </c>
@@ -14799,7 +14895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="425" spans="1:6">
+    <row r="425" spans="1:6" ht="30">
       <c r="A425" t="s">
         <v>298</v>
       </c>
@@ -14819,7 +14915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="426" spans="1:6" ht="29">
+    <row r="426" spans="1:6" ht="30">
       <c r="A426" t="s">
         <v>298</v>
       </c>
@@ -14919,7 +15015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="431" spans="1:6" ht="43.5">
+    <row r="431" spans="1:6" ht="45">
       <c r="A431" t="s">
         <v>298</v>
       </c>
@@ -14979,7 +15075,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="434" spans="1:6" ht="29">
+    <row r="434" spans="1:6" ht="45">
       <c r="A434" t="s">
         <v>298</v>
       </c>
@@ -14999,7 +15095,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="435" spans="1:6" ht="29">
+    <row r="435" spans="1:6" ht="30">
       <c r="A435" t="s">
         <v>298</v>
       </c>
@@ -15059,7 +15155,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="438" spans="1:6" ht="29">
+    <row r="438" spans="1:6" ht="30">
       <c r="A438" t="s">
         <v>298</v>
       </c>
@@ -15079,7 +15175,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="439" spans="1:6" ht="43.5">
+    <row r="439" spans="1:6" ht="45">
       <c r="A439" t="s">
         <v>298</v>
       </c>
@@ -15099,7 +15195,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="440" spans="1:6" ht="29">
+    <row r="440" spans="1:6" ht="30">
       <c r="A440" t="s">
         <v>298</v>
       </c>
@@ -15119,7 +15215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="441" spans="1:6" ht="43.5">
+    <row r="441" spans="1:6" ht="45">
       <c r="A441" t="s">
         <v>299</v>
       </c>
@@ -15139,7 +15235,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="442" spans="1:6" ht="43.5">
+    <row r="442" spans="1:6" ht="45">
       <c r="A442" t="s">
         <v>299</v>
       </c>
@@ -15159,7 +15255,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="443" spans="1:6" ht="43.5">
+    <row r="443" spans="1:6" ht="45">
       <c r="A443" t="s">
         <v>299</v>
       </c>
@@ -15179,7 +15275,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="444" spans="1:6" ht="43.5">
+    <row r="444" spans="1:6" ht="45">
       <c r="A444" t="s">
         <v>299</v>
       </c>
@@ -15199,7 +15295,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="445" spans="1:6" ht="29">
+    <row r="445" spans="1:6" ht="45">
       <c r="A445" t="s">
         <v>299</v>
       </c>
@@ -15219,7 +15315,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="446" spans="1:6" ht="29">
+    <row r="446" spans="1:6" ht="30">
       <c r="A446" t="s">
         <v>299</v>
       </c>
@@ -15239,7 +15335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="447" spans="1:6" ht="58">
+    <row r="447" spans="1:6" ht="60">
       <c r="A447" t="s">
         <v>299</v>
       </c>
@@ -15259,7 +15355,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="448" spans="1:6" ht="43.5">
+    <row r="448" spans="1:6" ht="45">
       <c r="A448" t="s">
         <v>299</v>
       </c>
@@ -15279,7 +15375,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="449" spans="1:6" ht="43.5">
+    <row r="449" spans="1:6" ht="45">
       <c r="A449" t="s">
         <v>299</v>
       </c>
@@ -15299,7 +15395,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="450" spans="1:6" ht="58">
+    <row r="450" spans="1:6" ht="60">
       <c r="A450" t="s">
         <v>299</v>
       </c>
@@ -15319,7 +15415,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="451" spans="1:6" ht="58">
+    <row r="451" spans="1:6" ht="60">
       <c r="A451" t="s">
         <v>299</v>
       </c>
@@ -15339,7 +15435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="452" spans="1:6" ht="58">
+    <row r="452" spans="1:6" ht="60">
       <c r="A452" t="s">
         <v>299</v>
       </c>
@@ -15359,7 +15455,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="453" spans="1:6" ht="58">
+    <row r="453" spans="1:6" ht="60">
       <c r="A453" t="s">
         <v>299</v>
       </c>
@@ -15379,7 +15475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="454" spans="1:6" ht="43.5">
+    <row r="454" spans="1:6" ht="45">
       <c r="A454" t="s">
         <v>299</v>
       </c>
@@ -15399,7 +15495,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="455" spans="1:6" ht="58">
+    <row r="455" spans="1:6" ht="75">
       <c r="A455" t="s">
         <v>299</v>
       </c>
@@ -15419,7 +15515,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="456" spans="1:6" ht="58">
+    <row r="456" spans="1:6" ht="75">
       <c r="A456" t="s">
         <v>299</v>
       </c>
@@ -15439,7 +15535,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="457" spans="1:6" ht="29">
+    <row r="457" spans="1:6" ht="30">
       <c r="A457" t="s">
         <v>299</v>
       </c>
@@ -15459,7 +15555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="458" spans="1:6" ht="72.5">
+    <row r="458" spans="1:6" ht="75">
       <c r="A458" t="s">
         <v>299</v>
       </c>
@@ -15479,7 +15575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="459" spans="1:6" ht="72.5">
+    <row r="459" spans="1:6" ht="75">
       <c r="A459" t="s">
         <v>299</v>
       </c>
@@ -15499,7 +15595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="460" spans="1:6" ht="58">
+    <row r="460" spans="1:6" ht="60">
       <c r="A460" t="s">
         <v>299</v>
       </c>
@@ -15519,7 +15615,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="461" spans="1:6" ht="43.5">
+    <row r="461" spans="1:6" ht="45">
       <c r="A461" t="s">
         <v>299</v>
       </c>
@@ -15539,7 +15635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="462" spans="1:6" ht="43.5">
+    <row r="462" spans="1:6" ht="45">
       <c r="A462" t="s">
         <v>299</v>
       </c>
@@ -15559,7 +15655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="463" spans="1:6" ht="43.5">
+    <row r="463" spans="1:6" ht="45">
       <c r="A463" t="s">
         <v>299</v>
       </c>
@@ -15579,7 +15675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="464" spans="1:6" ht="43.5">
+    <row r="464" spans="1:6" ht="45">
       <c r="A464" t="s">
         <v>299</v>
       </c>
@@ -15599,7 +15695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="465" spans="1:6" ht="29">
+    <row r="465" spans="1:6" ht="30">
       <c r="A465" t="s">
         <v>299</v>
       </c>
@@ -15619,7 +15715,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="466" spans="1:6" ht="58">
+    <row r="466" spans="1:6" ht="60">
       <c r="A466" t="s">
         <v>299</v>
       </c>
@@ -15639,7 +15735,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="467" spans="1:6" ht="29">
+    <row r="467" spans="1:6" ht="30">
       <c r="A467" s="5" t="s">
         <v>299</v>
       </c>
@@ -15659,7 +15755,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="468" spans="1:6" ht="29">
+    <row r="468" spans="1:6" ht="30">
       <c r="A468" t="s">
         <v>299</v>
       </c>
@@ -15679,7 +15775,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="469" spans="1:6" ht="43.5">
+    <row r="469" spans="1:6" ht="45">
       <c r="A469" t="s">
         <v>299</v>
       </c>
@@ -15699,7 +15795,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="470" spans="1:6" ht="43.5">
+    <row r="470" spans="1:6" ht="60">
       <c r="A470" t="s">
         <v>299</v>
       </c>
@@ -15719,7 +15815,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="471" spans="1:6" ht="58">
+    <row r="471" spans="1:6" ht="60">
       <c r="A471" t="s">
         <v>299</v>
       </c>
@@ -15799,7 +15895,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="475" spans="1:6" ht="29">
+    <row r="475" spans="1:6" ht="45">
       <c r="A475" t="s">
         <v>299</v>
       </c>
@@ -15819,7 +15915,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="476" spans="1:6" ht="29">
+    <row r="476" spans="1:6" ht="45">
       <c r="A476" t="s">
         <v>299</v>
       </c>
@@ -15839,7 +15935,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="477" spans="1:6" ht="29">
+    <row r="477" spans="1:6" ht="45">
       <c r="A477" t="s">
         <v>299</v>
       </c>
@@ -15859,7 +15955,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="478" spans="1:6" ht="43.5">
+    <row r="478" spans="1:6" ht="45">
       <c r="A478" t="s">
         <v>299</v>
       </c>
@@ -15879,7 +15975,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="479" spans="1:6" ht="43.5">
+    <row r="479" spans="1:6" ht="45">
       <c r="A479" t="s">
         <v>299</v>
       </c>
@@ -15899,7 +15995,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="480" spans="1:6" ht="29">
+    <row r="480" spans="1:6" ht="30">
       <c r="A480" t="s">
         <v>299</v>
       </c>
@@ -15919,7 +16015,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="481" spans="1:6">
+    <row r="481" spans="1:6" ht="30">
       <c r="A481" t="s">
         <v>299</v>
       </c>
@@ -16019,7 +16115,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="486" spans="1:6" ht="43.5">
+    <row r="486" spans="1:6" ht="45">
       <c r="A486" t="s">
         <v>299</v>
       </c>
@@ -16059,7 +16155,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="488" spans="1:6" ht="29">
+    <row r="488" spans="1:6" ht="45">
       <c r="A488" t="s">
         <v>299</v>
       </c>
@@ -16079,7 +16175,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="489" spans="1:6" ht="58">
+    <row r="489" spans="1:6" ht="60">
       <c r="A489" t="s">
         <v>299</v>
       </c>
@@ -16099,7 +16195,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="490" spans="1:6" ht="43.5">
+    <row r="490" spans="1:6" ht="45">
       <c r="A490" t="s">
         <v>299</v>
       </c>
@@ -16119,7 +16215,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="491" spans="1:6" ht="72.5">
+    <row r="491" spans="1:6" ht="75">
       <c r="A491" t="s">
         <v>299</v>
       </c>
@@ -16139,7 +16235,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="492" spans="1:6" ht="43.5">
+    <row r="492" spans="1:6" ht="60">
       <c r="A492" t="s">
         <v>299</v>
       </c>
@@ -16159,7 +16255,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="493" spans="1:6" ht="43.5">
+    <row r="493" spans="1:6" ht="60">
       <c r="A493" t="s">
         <v>299</v>
       </c>
@@ -16179,7 +16275,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="494" spans="1:6" ht="72.5">
+    <row r="494" spans="1:6" ht="75">
       <c r="A494" t="s">
         <v>299</v>
       </c>
@@ -16199,7 +16295,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="495" spans="1:6" ht="72.5">
+    <row r="495" spans="1:6" ht="90">
       <c r="A495" t="s">
         <v>299</v>
       </c>
@@ -16219,7 +16315,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="496" spans="1:6" ht="58">
+    <row r="496" spans="1:6" ht="75">
       <c r="A496" t="s">
         <v>299</v>
       </c>
@@ -16239,7 +16335,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="497" spans="1:6" ht="72.5">
+    <row r="497" spans="1:6" ht="75">
       <c r="A497" t="s">
         <v>299</v>
       </c>
@@ -16259,7 +16355,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="498" spans="1:6" ht="58">
+    <row r="498" spans="1:6" ht="75">
       <c r="A498" t="s">
         <v>299</v>
       </c>
@@ -16279,7 +16375,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="499" spans="1:6" ht="72.5">
+    <row r="499" spans="1:6" ht="75">
       <c r="A499" t="s">
         <v>299</v>
       </c>
@@ -16299,7 +16395,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="500" spans="1:6" ht="58">
+    <row r="500" spans="1:6" ht="60">
       <c r="A500" t="s">
         <v>299</v>
       </c>
@@ -16319,7 +16415,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="501" spans="1:6" ht="72.5">
+    <row r="501" spans="1:6" ht="75">
       <c r="A501" t="s">
         <v>299</v>
       </c>
@@ -16339,7 +16435,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="502" spans="1:6" ht="72.5">
+    <row r="502" spans="1:6" ht="75">
       <c r="A502" t="s">
         <v>299</v>
       </c>
@@ -16359,7 +16455,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="503" spans="1:6" ht="43.5">
+    <row r="503" spans="1:6" ht="60">
       <c r="A503" t="s">
         <v>299</v>
       </c>
@@ -16379,7 +16475,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="504" spans="1:6" ht="87">
+    <row r="504" spans="1:6" ht="90">
       <c r="A504" t="s">
         <v>299</v>
       </c>
@@ -16399,7 +16495,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="505" spans="1:6" ht="43.5">
+    <row r="505" spans="1:6" ht="60">
       <c r="A505" t="s">
         <v>299</v>
       </c>
@@ -16419,7 +16515,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="506" spans="1:6" ht="58">
+    <row r="506" spans="1:6" ht="75">
       <c r="A506" t="s">
         <v>299</v>
       </c>
@@ -16439,7 +16535,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="507" spans="1:6" ht="58">
+    <row r="507" spans="1:6" ht="90">
       <c r="A507" t="s">
         <v>299</v>
       </c>
@@ -16459,7 +16555,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="508" spans="1:6" ht="58">
+    <row r="508" spans="1:6" ht="90">
       <c r="A508" t="s">
         <v>299</v>
       </c>
@@ -16479,7 +16575,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="509" spans="1:6" ht="43.5">
+    <row r="509" spans="1:6" ht="75">
       <c r="A509" t="s">
         <v>299</v>
       </c>
@@ -16499,7 +16595,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="510" spans="1:6" ht="29">
+    <row r="510" spans="1:6" ht="30">
       <c r="A510" t="s">
         <v>299</v>
       </c>
@@ -16519,7 +16615,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="511" spans="1:6" ht="29">
+    <row r="511" spans="1:6" ht="30">
       <c r="A511" t="s">
         <v>299</v>
       </c>
@@ -16539,7 +16635,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="512" spans="1:6" ht="29">
+    <row r="512" spans="1:6" ht="30">
       <c r="A512" t="s">
         <v>299</v>
       </c>
@@ -16559,7 +16655,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="513" spans="1:6">
+    <row r="513" spans="1:6" ht="30">
       <c r="A513" t="s">
         <v>299</v>
       </c>
@@ -16579,7 +16675,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="514" spans="1:6" ht="29">
+    <row r="514" spans="1:6" ht="30">
       <c r="A514" t="s">
         <v>299</v>
       </c>
@@ -16599,7 +16695,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="515" spans="1:6" ht="29">
+    <row r="515" spans="1:6" ht="30">
       <c r="A515" t="s">
         <v>299</v>
       </c>
@@ -56196,6 +56292,486 @@
         <v>1391</v>
       </c>
       <c r="F2494" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2495" spans="1:6">
+      <c r="A2495" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2495" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2495" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D2495" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2495" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2495" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:6">
+      <c r="A2496" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2496" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2496" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D2496" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2496" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2496" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:6">
+      <c r="A2497" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2497" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2497" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D2497" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2497" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2497" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:6">
+      <c r="A2498" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2498" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2498" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D2498" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2498" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2498" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:6">
+      <c r="A2499" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2499" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2499" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D2499" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2499" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2499" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:6">
+      <c r="A2500" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2500" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2500" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D2500" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2500" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2500" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2501" spans="1:6">
+      <c r="A2501" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2501" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C2501" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D2501" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2501" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2501" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2502" spans="1:6">
+      <c r="A2502" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2502" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C2502" t="s">
+        <v>1409</v>
+      </c>
+      <c r="D2502" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2502" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2502" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2503" spans="1:6">
+      <c r="A2503" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2503" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C2503" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D2503" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2503" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2503" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2504" spans="1:6">
+      <c r="A2504" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2504" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2504" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D2504" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2504" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2504" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2505" spans="1:6">
+      <c r="A2505" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2505" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2505" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D2505" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2505" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2505" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2506" spans="1:6">
+      <c r="A2506" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2506" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2506" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D2506" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2506" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2506" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2507" spans="1:6">
+      <c r="A2507" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2507" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C2507" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D2507" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2507" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2507" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2508" spans="1:6">
+      <c r="A2508" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2508" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C2508" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D2508" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2508" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2508" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2509" spans="1:6">
+      <c r="A2509" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2509" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C2509" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D2509" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2509" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2509" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2510" spans="1:6">
+      <c r="A2510" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2510" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C2510" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D2510" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2510" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2510" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2511" spans="1:6">
+      <c r="A2511" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2511" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C2511" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D2511" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2511" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2511" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2512" spans="1:6">
+      <c r="A2512" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2512" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C2512" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D2512" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2512" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2512" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2513" spans="1:6">
+      <c r="A2513" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2513" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C2513" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D2513" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2513" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2513" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2514" spans="1:6">
+      <c r="A2514" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2514" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C2514" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D2514" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2514" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2514" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:6">
+      <c r="A2515" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2515" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C2515" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D2515" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2515" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2515" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:6">
+      <c r="A2516" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2516" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C2516" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D2516" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2516" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2516" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:6">
+      <c r="A2517" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2517" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C2517" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D2517" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2517" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2517" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:6">
+      <c r="A2518" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2518" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C2518" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D2518" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2518" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2518" t="s">
         <v>1392</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MOSIP-40766: removed pms-revamp templates
Signed-off-by: Swetha K <swetha.k@technoforte.co.in>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2569C69-C9F3-4645-BAB1-9AE72E65D57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF45C81-6880-4123-B7BE-9F6CE6B1ADA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15108" uniqueCount="1431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14964" uniqueCount="1399">
   <si>
     <t>lang_code</t>
   </si>
@@ -5837,102 +5837,6 @@
   </si>
   <si>
     <t>Authentication positive summary</t>
-  </si>
-  <si>
-    <t>ROOT_CERT_EXPIRY_TEMPLATE</t>
-  </si>
-  <si>
-    <t>INTERMEDIATE_CERT_EXPIRY_TEMPLATE</t>
-  </si>
-  <si>
-    <t>PARTNER_CERT_EXPIRY_TEMPLATE</t>
-  </si>
-  <si>
-    <t>WEEKLY_SUMMARY_TEMPLATE</t>
-  </si>
-  <si>
-    <t>ROOT_CERT_EXPIRY_SUBJECT</t>
-  </si>
-  <si>
-    <t>INTERMEDIATE_CERT_EXPIRY_SUBJECT</t>
-  </si>
-  <si>
-    <t>PARTNER_CERT_EXPIRY_SUBJECT</t>
-  </si>
-  <si>
-    <t>WEEKLY_SUMMARY_SUBJECT</t>
-  </si>
-  <si>
-    <t>Template for root certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle d'expiration du certificat racine</t>
-  </si>
-  <si>
-    <t>نموذج لانتهاء صلاحية شهادة الجذر</t>
-  </si>
-  <si>
-    <t>Template for intermediate certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle d'expiration de certificat intermédiaire</t>
-  </si>
-  <si>
-    <t>نموذج انتهاء صلاحية الشهادة المتوسطة</t>
-  </si>
-  <si>
-    <t>Template for partner certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle d'expiration du certificat de partenaire</t>
-  </si>
-  <si>
-    <t>نموذج انتهاء صلاحية شهادة الشريك</t>
-  </si>
-  <si>
-    <t>Template for weekly summary notifications</t>
-  </si>
-  <si>
-    <t>Modèle pour les notifications récapitulatives hebdomadaires</t>
-  </si>
-  <si>
-    <t>نموذج لإشعارات الملخص الأسبوعية</t>
-  </si>
-  <si>
-    <t>Subject template for root certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle de sujet pour l'expiration du certificat racine</t>
-  </si>
-  <si>
-    <t>نموذج موضوعي لانتهاء صلاحية شهادة الجذر</t>
-  </si>
-  <si>
-    <t>Subject template for intermediate certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle de sujet pour l'expiration du certificat intermédiaire</t>
-  </si>
-  <si>
-    <t>نموذج موضوعي لانتهاء صلاحية الشهادة المتوسطة</t>
-  </si>
-  <si>
-    <t>Subject template for partner certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle de sujet pour l'expiration du certificat du partenaire</t>
-  </si>
-  <si>
-    <t>نموذج موضوعي لانتهاء صلاحية شهادة الشريك</t>
-  </si>
-  <si>
-    <t>Subject template for weekly summary notifications</t>
-  </si>
-  <si>
-    <t>Modèle de sujet pour les notifications récapitulatives hebdomadaires</t>
-  </si>
-  <si>
-    <t>قالب موضوعي لإشعارات الملخص الأسبوعي</t>
   </si>
 </sst>
 </file>
@@ -6401,10 +6305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2518"/>
+  <dimension ref="A1:F2494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2510" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2518" sqref="D2518"/>
+    <sheetView tabSelected="1" topLeftCell="A2486" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2494" sqref="A2494"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -56295,486 +56199,6 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="2495" spans="1:6">
-      <c r="A2495" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2495" t="s">
-        <v>1399</v>
-      </c>
-      <c r="C2495" t="s">
-        <v>1407</v>
-      </c>
-      <c r="D2495" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2495" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2495" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2496" spans="1:6">
-      <c r="A2496" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2496" t="s">
-        <v>1399</v>
-      </c>
-      <c r="C2496" t="s">
-        <v>1408</v>
-      </c>
-      <c r="D2496" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2496" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2496" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2497" spans="1:6">
-      <c r="A2497" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2497" t="s">
-        <v>1399</v>
-      </c>
-      <c r="C2497" t="s">
-        <v>1409</v>
-      </c>
-      <c r="D2497" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2497" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2497" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2498" spans="1:6">
-      <c r="A2498" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2498" t="s">
-        <v>1400</v>
-      </c>
-      <c r="C2498" t="s">
-        <v>1410</v>
-      </c>
-      <c r="D2498" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2498" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2498" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2499" spans="1:6">
-      <c r="A2499" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2499" t="s">
-        <v>1400</v>
-      </c>
-      <c r="C2499" t="s">
-        <v>1411</v>
-      </c>
-      <c r="D2499" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2499" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2499" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2500" spans="1:6">
-      <c r="A2500" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2500" t="s">
-        <v>1400</v>
-      </c>
-      <c r="C2500" t="s">
-        <v>1412</v>
-      </c>
-      <c r="D2500" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2500" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2500" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2501" spans="1:6">
-      <c r="A2501" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2501" t="s">
-        <v>1401</v>
-      </c>
-      <c r="C2501" t="s">
-        <v>1413</v>
-      </c>
-      <c r="D2501" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2501" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2501" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2502" spans="1:6">
-      <c r="A2502" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2502" t="s">
-        <v>1401</v>
-      </c>
-      <c r="C2502" t="s">
-        <v>1414</v>
-      </c>
-      <c r="D2502" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2502" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2502" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2503" spans="1:6">
-      <c r="A2503" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2503" t="s">
-        <v>1401</v>
-      </c>
-      <c r="C2503" t="s">
-        <v>1415</v>
-      </c>
-      <c r="D2503" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2503" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2503" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2504" spans="1:6">
-      <c r="A2504" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2504" t="s">
-        <v>1402</v>
-      </c>
-      <c r="C2504" t="s">
-        <v>1416</v>
-      </c>
-      <c r="D2504" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2504" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2504" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2505" spans="1:6">
-      <c r="A2505" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2505" t="s">
-        <v>1402</v>
-      </c>
-      <c r="C2505" t="s">
-        <v>1417</v>
-      </c>
-      <c r="D2505" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2505" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2505" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2506" spans="1:6">
-      <c r="A2506" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2506" t="s">
-        <v>1402</v>
-      </c>
-      <c r="C2506" t="s">
-        <v>1418</v>
-      </c>
-      <c r="D2506" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2506" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2506" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2507" spans="1:6">
-      <c r="A2507" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2507" t="s">
-        <v>1403</v>
-      </c>
-      <c r="C2507" t="s">
-        <v>1419</v>
-      </c>
-      <c r="D2507" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2507" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2507" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2508" spans="1:6">
-      <c r="A2508" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2508" t="s">
-        <v>1403</v>
-      </c>
-      <c r="C2508" t="s">
-        <v>1420</v>
-      </c>
-      <c r="D2508" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2508" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2508" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2509" spans="1:6">
-      <c r="A2509" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2509" t="s">
-        <v>1403</v>
-      </c>
-      <c r="C2509" t="s">
-        <v>1421</v>
-      </c>
-      <c r="D2509" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2509" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2509" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2510" spans="1:6">
-      <c r="A2510" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2510" t="s">
-        <v>1404</v>
-      </c>
-      <c r="C2510" t="s">
-        <v>1422</v>
-      </c>
-      <c r="D2510" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2510" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2510" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2511" spans="1:6">
-      <c r="A2511" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2511" t="s">
-        <v>1404</v>
-      </c>
-      <c r="C2511" t="s">
-        <v>1423</v>
-      </c>
-      <c r="D2511" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2511" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2511" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2512" spans="1:6">
-      <c r="A2512" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2512" t="s">
-        <v>1404</v>
-      </c>
-      <c r="C2512" t="s">
-        <v>1424</v>
-      </c>
-      <c r="D2512" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2512" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2512" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2513" spans="1:6">
-      <c r="A2513" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2513" t="s">
-        <v>1405</v>
-      </c>
-      <c r="C2513" t="s">
-        <v>1425</v>
-      </c>
-      <c r="D2513" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2513" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2513" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2514" spans="1:6">
-      <c r="A2514" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2514" t="s">
-        <v>1405</v>
-      </c>
-      <c r="C2514" t="s">
-        <v>1426</v>
-      </c>
-      <c r="D2514" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2514" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2514" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2515" spans="1:6">
-      <c r="A2515" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2515" t="s">
-        <v>1405</v>
-      </c>
-      <c r="C2515" t="s">
-        <v>1427</v>
-      </c>
-      <c r="D2515" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2515" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2515" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2516" spans="1:6">
-      <c r="A2516" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2516" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C2516" t="s">
-        <v>1428</v>
-      </c>
-      <c r="D2516" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2516" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2516" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2517" spans="1:6">
-      <c r="A2517" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2517" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C2517" t="s">
-        <v>1429</v>
-      </c>
-      <c r="D2517" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2517" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2517" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2518" spans="1:6">
-      <c r="A2518" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2518" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C2518" t="s">
-        <v>1430</v>
-      </c>
-      <c r="D2518" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2518" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2518" t="s">
-        <v>1392</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:D365" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
MOSIP-40766: removed pms-revamp templates (#340)
* MOSIP-40766: removed pms-revamp templates

Signed-off-by: Swetha K <swetha.k@technoforte.co.in>

* Added converted CSV files

Signed-off-by: SwethaKrish4 <swetha.k@technoforte.co.in>

---------

Signed-off-by: Swetha K <swetha.k@technoforte.co.in>
Signed-off-by: SwethaKrish4 <swetha.k@technoforte.co.in>
Co-authored-by: Swetha K <swetha.k@technoforte.co.in>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2569C69-C9F3-4645-BAB1-9AE72E65D57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF45C81-6880-4123-B7BE-9F6CE6B1ADA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15108" uniqueCount="1431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14964" uniqueCount="1399">
   <si>
     <t>lang_code</t>
   </si>
@@ -5837,102 +5837,6 @@
   </si>
   <si>
     <t>Authentication positive summary</t>
-  </si>
-  <si>
-    <t>ROOT_CERT_EXPIRY_TEMPLATE</t>
-  </si>
-  <si>
-    <t>INTERMEDIATE_CERT_EXPIRY_TEMPLATE</t>
-  </si>
-  <si>
-    <t>PARTNER_CERT_EXPIRY_TEMPLATE</t>
-  </si>
-  <si>
-    <t>WEEKLY_SUMMARY_TEMPLATE</t>
-  </si>
-  <si>
-    <t>ROOT_CERT_EXPIRY_SUBJECT</t>
-  </si>
-  <si>
-    <t>INTERMEDIATE_CERT_EXPIRY_SUBJECT</t>
-  </si>
-  <si>
-    <t>PARTNER_CERT_EXPIRY_SUBJECT</t>
-  </si>
-  <si>
-    <t>WEEKLY_SUMMARY_SUBJECT</t>
-  </si>
-  <si>
-    <t>Template for root certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle d'expiration du certificat racine</t>
-  </si>
-  <si>
-    <t>نموذج لانتهاء صلاحية شهادة الجذر</t>
-  </si>
-  <si>
-    <t>Template for intermediate certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle d'expiration de certificat intermédiaire</t>
-  </si>
-  <si>
-    <t>نموذج انتهاء صلاحية الشهادة المتوسطة</t>
-  </si>
-  <si>
-    <t>Template for partner certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle d'expiration du certificat de partenaire</t>
-  </si>
-  <si>
-    <t>نموذج انتهاء صلاحية شهادة الشريك</t>
-  </si>
-  <si>
-    <t>Template for weekly summary notifications</t>
-  </si>
-  <si>
-    <t>Modèle pour les notifications récapitulatives hebdomadaires</t>
-  </si>
-  <si>
-    <t>نموذج لإشعارات الملخص الأسبوعية</t>
-  </si>
-  <si>
-    <t>Subject template for root certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle de sujet pour l'expiration du certificat racine</t>
-  </si>
-  <si>
-    <t>نموذج موضوعي لانتهاء صلاحية شهادة الجذر</t>
-  </si>
-  <si>
-    <t>Subject template for intermediate certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle de sujet pour l'expiration du certificat intermédiaire</t>
-  </si>
-  <si>
-    <t>نموذج موضوعي لانتهاء صلاحية الشهادة المتوسطة</t>
-  </si>
-  <si>
-    <t>Subject template for partner certificate expiry</t>
-  </si>
-  <si>
-    <t>Modèle de sujet pour l'expiration du certificat du partenaire</t>
-  </si>
-  <si>
-    <t>نموذج موضوعي لانتهاء صلاحية شهادة الشريك</t>
-  </si>
-  <si>
-    <t>Subject template for weekly summary notifications</t>
-  </si>
-  <si>
-    <t>Modèle de sujet pour les notifications récapitulatives hebdomadaires</t>
-  </si>
-  <si>
-    <t>قالب موضوعي لإشعارات الملخص الأسبوعي</t>
   </si>
 </sst>
 </file>
@@ -6401,10 +6305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2518"/>
+  <dimension ref="A1:F2494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2510" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2518" sqref="D2518"/>
+    <sheetView tabSelected="1" topLeftCell="A2486" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2494" sqref="A2494"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -56295,486 +56199,6 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="2495" spans="1:6">
-      <c r="A2495" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2495" t="s">
-        <v>1399</v>
-      </c>
-      <c r="C2495" t="s">
-        <v>1407</v>
-      </c>
-      <c r="D2495" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2495" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2495" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2496" spans="1:6">
-      <c r="A2496" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2496" t="s">
-        <v>1399</v>
-      </c>
-      <c r="C2496" t="s">
-        <v>1408</v>
-      </c>
-      <c r="D2496" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2496" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2496" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2497" spans="1:6">
-      <c r="A2497" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2497" t="s">
-        <v>1399</v>
-      </c>
-      <c r="C2497" t="s">
-        <v>1409</v>
-      </c>
-      <c r="D2497" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2497" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2497" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2498" spans="1:6">
-      <c r="A2498" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2498" t="s">
-        <v>1400</v>
-      </c>
-      <c r="C2498" t="s">
-        <v>1410</v>
-      </c>
-      <c r="D2498" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2498" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2498" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2499" spans="1:6">
-      <c r="A2499" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2499" t="s">
-        <v>1400</v>
-      </c>
-      <c r="C2499" t="s">
-        <v>1411</v>
-      </c>
-      <c r="D2499" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2499" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2499" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2500" spans="1:6">
-      <c r="A2500" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2500" t="s">
-        <v>1400</v>
-      </c>
-      <c r="C2500" t="s">
-        <v>1412</v>
-      </c>
-      <c r="D2500" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2500" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2500" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2501" spans="1:6">
-      <c r="A2501" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2501" t="s">
-        <v>1401</v>
-      </c>
-      <c r="C2501" t="s">
-        <v>1413</v>
-      </c>
-      <c r="D2501" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2501" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2501" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2502" spans="1:6">
-      <c r="A2502" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2502" t="s">
-        <v>1401</v>
-      </c>
-      <c r="C2502" t="s">
-        <v>1414</v>
-      </c>
-      <c r="D2502" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2502" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2502" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2503" spans="1:6">
-      <c r="A2503" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2503" t="s">
-        <v>1401</v>
-      </c>
-      <c r="C2503" t="s">
-        <v>1415</v>
-      </c>
-      <c r="D2503" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2503" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2503" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2504" spans="1:6">
-      <c r="A2504" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2504" t="s">
-        <v>1402</v>
-      </c>
-      <c r="C2504" t="s">
-        <v>1416</v>
-      </c>
-      <c r="D2504" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2504" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2504" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2505" spans="1:6">
-      <c r="A2505" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2505" t="s">
-        <v>1402</v>
-      </c>
-      <c r="C2505" t="s">
-        <v>1417</v>
-      </c>
-      <c r="D2505" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2505" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2505" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2506" spans="1:6">
-      <c r="A2506" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2506" t="s">
-        <v>1402</v>
-      </c>
-      <c r="C2506" t="s">
-        <v>1418</v>
-      </c>
-      <c r="D2506" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2506" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2506" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2507" spans="1:6">
-      <c r="A2507" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2507" t="s">
-        <v>1403</v>
-      </c>
-      <c r="C2507" t="s">
-        <v>1419</v>
-      </c>
-      <c r="D2507" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2507" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2507" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2508" spans="1:6">
-      <c r="A2508" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2508" t="s">
-        <v>1403</v>
-      </c>
-      <c r="C2508" t="s">
-        <v>1420</v>
-      </c>
-      <c r="D2508" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2508" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2508" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2509" spans="1:6">
-      <c r="A2509" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2509" t="s">
-        <v>1403</v>
-      </c>
-      <c r="C2509" t="s">
-        <v>1421</v>
-      </c>
-      <c r="D2509" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2509" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2509" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2510" spans="1:6">
-      <c r="A2510" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2510" t="s">
-        <v>1404</v>
-      </c>
-      <c r="C2510" t="s">
-        <v>1422</v>
-      </c>
-      <c r="D2510" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2510" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2510" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2511" spans="1:6">
-      <c r="A2511" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2511" t="s">
-        <v>1404</v>
-      </c>
-      <c r="C2511" t="s">
-        <v>1423</v>
-      </c>
-      <c r="D2511" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2511" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2511" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2512" spans="1:6">
-      <c r="A2512" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2512" t="s">
-        <v>1404</v>
-      </c>
-      <c r="C2512" t="s">
-        <v>1424</v>
-      </c>
-      <c r="D2512" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2512" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2512" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2513" spans="1:6">
-      <c r="A2513" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2513" t="s">
-        <v>1405</v>
-      </c>
-      <c r="C2513" t="s">
-        <v>1425</v>
-      </c>
-      <c r="D2513" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2513" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2513" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2514" spans="1:6">
-      <c r="A2514" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2514" t="s">
-        <v>1405</v>
-      </c>
-      <c r="C2514" t="s">
-        <v>1426</v>
-      </c>
-      <c r="D2514" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2514" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2514" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2515" spans="1:6">
-      <c r="A2515" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2515" t="s">
-        <v>1405</v>
-      </c>
-      <c r="C2515" t="s">
-        <v>1427</v>
-      </c>
-      <c r="D2515" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2515" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2515" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2516" spans="1:6">
-      <c r="A2516" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2516" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C2516" t="s">
-        <v>1428</v>
-      </c>
-      <c r="D2516" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2516" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2516" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2517" spans="1:6">
-      <c r="A2517" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2517" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C2517" t="s">
-        <v>1429</v>
-      </c>
-      <c r="D2517" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2517" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2517" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="2518" spans="1:6">
-      <c r="A2518" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2518" t="s">
-        <v>1406</v>
-      </c>
-      <c r="C2518" t="s">
-        <v>1430</v>
-      </c>
-      <c r="D2518" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2518" t="s">
-        <v>1391</v>
-      </c>
-      <c r="F2518" t="s">
-        <v>1392</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:D365" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
MOSIP-40766: Added all new pms-revamp templates
Signed-off-by: Swetha K <swetha.k@technoforte.co.in>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF45C81-6880-4123-B7BE-9F6CE6B1ADA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2A89C4-95B5-421B-9706-6D277F1A82C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14964" uniqueCount="1399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15252" uniqueCount="1455">
   <si>
     <t>lang_code</t>
   </si>
@@ -5837,6 +5837,174 @@
   </si>
   <si>
     <t>Authentication positive summary</t>
+  </si>
+  <si>
+    <t>ROOT_CERT_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for root certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle d'expiration du certificat racine</t>
+  </si>
+  <si>
+    <t>نموذج لانتهاء صلاحية شهادة الجذر</t>
+  </si>
+  <si>
+    <t>INTERMEDIATE_CERT_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for intermediate certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle d'expiration de certificat intermédiaire</t>
+  </si>
+  <si>
+    <t>نموذج انتهاء صلاحية الشهادة المتوسطة</t>
+  </si>
+  <si>
+    <t>PARTNER_CERT_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for partner certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle d'expiration du certificat de partenaire</t>
+  </si>
+  <si>
+    <t>نموذج انتهاء صلاحية شهادة الشريك</t>
+  </si>
+  <si>
+    <t>WEEKLY_SUMMARY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for weekly summary notifications</t>
+  </si>
+  <si>
+    <t>Modèle pour les notifications récapitulatives hebdomadaires</t>
+  </si>
+  <si>
+    <t>نموذج لإشعارات الملخص الأسبوعية</t>
+  </si>
+  <si>
+    <t>ROOT_CERT_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for root certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du certificat racine</t>
+  </si>
+  <si>
+    <t>نموذج موضوعي لانتهاء صلاحية شهادة الجذر</t>
+  </si>
+  <si>
+    <t>INTERMEDIATE_CERT_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for intermediate certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du certificat intermédiaire</t>
+  </si>
+  <si>
+    <t>نموذج موضوعي لانتهاء صلاحية الشهادة المتوسطة</t>
+  </si>
+  <si>
+    <t>PARTNER_CERT_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for partner certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du certificat du partenaire</t>
+  </si>
+  <si>
+    <t>نموذج موضوعي لانتهاء صلاحية شهادة الشريك</t>
+  </si>
+  <si>
+    <t>WEEKLY_SUMMARY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for weekly summary notifications</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour les notifications récapitulatives hebdomadaires</t>
+  </si>
+  <si>
+    <t>قالب موضوعي لإشعارات الملخص الأسبوعي</t>
+  </si>
+  <si>
+    <t>ரூட் சான்றிதழ் காலாவதிக்கான டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>रूट प्रमाणपत्र समाप्ति के लिए टेम्पलेट</t>
+  </si>
+  <si>
+    <t>ಮೂಲ ಪ್ರಮಾಣಪತ್ರದ ಮುಕ್ತಾಯ ದಿನಾಂಕದ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>ಮಧ್ಯಂತರ ಪ್ರಮಾಣಪತ್ರ ಮುಕ್ತಾಯಕ್ಕಾಗಿ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>मध्यवर्ती प्रमाणपत्र समाप्ति के लिए टेम्पलेट</t>
+  </si>
+  <si>
+    <t>இடைநிலை சான்றிதழ் காலாவதிக்கான டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>கூட்டாளர் சான்றிதழ் காலாவதிக்கான டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>ಪಾಲುದಾರ ಪ್ರಮಾಣಪತ್ರದ ಮುಕ್ತಾಯ ದಿನಾಂಕದ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>भागीदार प्रमाणपत्र समाप्ति के लिए टेम्पलेट</t>
+  </si>
+  <si>
+    <t>साप्ताहिक सारांश अधिसूचनाओं के लिए टेम्पलेट</t>
+  </si>
+  <si>
+    <t>ವಾರದ ಸಾರಾಂಶ ಅಧಿಸೂಚನೆಗಳಿಗಾಗಿ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>வாராந்திர சுருக்க அறிவிப்புகளுக்கான டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>மூலச் சான்றிதழ் காலாவதிக்கான பொருள் டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>रूट प्रमाणपत्र समाप्ति के लिए विषय टेम्पलेट</t>
+  </si>
+  <si>
+    <t>ಮೂಲ ಪ್ರಮಾಣಪತ್ರದ ಮುಕ್ತಾಯ ದಿನಾಂಕದ ವಿಷಯ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>ಮಧ್ಯಂತರ ಪ್ರಮಾಣಪತ್ರ ಮುಕ್ತಾಯಕ್ಕಾಗಿ ವಿಷಯ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>इंटरमीडिएट प्रमाणपत्र समाप्ति के लिए विषय टेम्पलेट</t>
+  </si>
+  <si>
+    <t>இடைநிலை சான்றிதழ் காலாவதிக்கான பொருள் வார்ப்புரு</t>
+  </si>
+  <si>
+    <t>கூட்டாளர் சான்றிதழ் காலாவதிக்கான பொருள் டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>ಪಾಲುದಾರ ಪ್ರಮಾಣಪತ್ರದ ಮುಕ್ತಾಯದ ವಿಷಯ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>भागीदार प्रमाणपत्र समाप्ति के लिए विषय टेम्पलेट</t>
+  </si>
+  <si>
+    <t>साप्ताहिक सारांश अधिसूचनाओं के लिए विषय टेम्पलेट</t>
+  </si>
+  <si>
+    <t>ವಾರದ ಸಾರಾಂಶ ಅಧಿಸೂಚನೆಗಳಿಗಾಗಿ ವಿಷಯ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>வாராந்திர சுருக்க அறிவிப்புகளுக்கான தலைப்பு டெம்ப்ளேட்</t>
   </si>
 </sst>
 </file>
@@ -6305,17 +6473,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2494"/>
+  <dimension ref="A1:F2542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2486" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2494" sqref="A2494"/>
+    <sheetView tabSelected="1" topLeftCell="A2489" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2541" sqref="B2541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="40.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="66.7109375" customWidth="1"/>
     <col min="4" max="4" width="27" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -56199,6 +56367,966 @@
         <v>1392</v>
       </c>
     </row>
+    <row r="2495" spans="1:6">
+      <c r="A2495" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2495" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2495" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D2495" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2495" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2495" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:6">
+      <c r="A2496" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2496" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2496" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D2496" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2496" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2496" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:6">
+      <c r="A2497" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2497" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2497" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D2497" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2497" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2497" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:6">
+      <c r="A2498" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2498" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2498" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D2498" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2498" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2498" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:6">
+      <c r="A2499" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2499" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2499" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D2499" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2499" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2499" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:6">
+      <c r="A2500" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2500" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C2500" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D2500" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2500" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2500" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2501" spans="1:6">
+      <c r="A2501" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2501" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2501" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D2501" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2501" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2501" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2502" spans="1:6">
+      <c r="A2502" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2502" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2502" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D2502" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2502" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2502" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2503" spans="1:6">
+      <c r="A2503" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2503" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2503" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D2503" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2503" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2503" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2504" spans="1:6">
+      <c r="A2504" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2504" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2504" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D2504" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2504" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2504" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2505" spans="1:6">
+      <c r="A2505" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2505" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2505" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D2505" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2505" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2505" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2506" spans="1:6">
+      <c r="A2506" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2506" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C2506" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D2506" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2506" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2506" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2507" spans="1:6">
+      <c r="A2507" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2507" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C2507" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D2507" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2507" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2507" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2508" spans="1:6">
+      <c r="A2508" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2508" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C2508" t="s">
+        <v>1409</v>
+      </c>
+      <c r="D2508" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2508" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2508" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2509" spans="1:6">
+      <c r="A2509" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2509" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C2509" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D2509" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2509" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2509" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2510" spans="1:6">
+      <c r="A2510" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2510" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C2510" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D2510" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2510" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2510" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2511" spans="1:6">
+      <c r="A2511" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2511" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C2511" t="s">
+        <v>1438</v>
+      </c>
+      <c r="D2511" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2511" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2511" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2512" spans="1:6">
+      <c r="A2512" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2512" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C2512" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D2512" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2512" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2512" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2513" spans="1:6">
+      <c r="A2513" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2513" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2513" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D2513" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2513" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2513" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2514" spans="1:6">
+      <c r="A2514" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2514" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2514" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D2514" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2514" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2514" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:6">
+      <c r="A2515" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2515" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2515" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D2515" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2515" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2515" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:6">
+      <c r="A2516" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2516" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2516" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D2516" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2516" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2516" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:6">
+      <c r="A2517" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2517" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2517" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D2517" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2517" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2517" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:6">
+      <c r="A2518" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2518" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2518" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D2518" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2518" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2518" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2519" spans="1:6">
+      <c r="A2519" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2519" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C2519" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D2519" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2519" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2519" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2520" spans="1:6">
+      <c r="A2520" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2520" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C2520" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D2520" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2520" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2520" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2521" spans="1:6">
+      <c r="A2521" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2521" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C2521" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D2521" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2521" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2521" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2522" spans="1:6">
+      <c r="A2522" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2522" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C2522" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D2522" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2522" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2522" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2523" spans="1:6">
+      <c r="A2523" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2523" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C2523" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D2523" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2523" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2523" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2524" spans="1:6">
+      <c r="A2524" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2524" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C2524" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D2524" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2524" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2524" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2525" spans="1:6">
+      <c r="A2525" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2525" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C2525" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D2525" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2525" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2525" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2526" spans="1:6">
+      <c r="A2526" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2526" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C2526" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D2526" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2526" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2526" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2527" spans="1:6">
+      <c r="A2527" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2527" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C2527" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D2527" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2527" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2527" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2528" spans="1:6">
+      <c r="A2528" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2528" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C2528" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D2528" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2528" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2528" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2529" spans="1:6">
+      <c r="A2529" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2529" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C2529" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D2529" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2529" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2529" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2530" spans="1:6">
+      <c r="A2530" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2530" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C2530" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D2530" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2530" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2530" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2531" spans="1:6">
+      <c r="A2531" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2531" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C2531" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D2531" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2531" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2531" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2532" spans="1:6">
+      <c r="A2532" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2532" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C2532" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D2532" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2532" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2532" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2533" spans="1:6">
+      <c r="A2533" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2533" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C2533" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D2533" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2533" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2533" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2534" spans="1:6">
+      <c r="A2534" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2534" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C2534" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D2534" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2534" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2534" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2535" spans="1:6">
+      <c r="A2535" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2535" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C2535" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D2535" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2535" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2535" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2536" spans="1:6">
+      <c r="A2536" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2536" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C2536" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D2536" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2536" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2536" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2537" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A2537" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2537" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C2537" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D2537" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2537" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2537" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2538" spans="1:6">
+      <c r="A2538" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2538" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C2538" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D2538" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2538" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2538" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2539" spans="1:6">
+      <c r="A2539" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2539" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C2539" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D2539" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2539" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2539" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2540" spans="1:6">
+      <c r="A2540" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2540" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C2540" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D2540" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2540" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2540" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2541" spans="1:6">
+      <c r="A2541" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2541" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C2541" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D2541" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2541" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2541" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:6">
+      <c r="A2542" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2542" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C2542" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D2542" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2542" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2542" t="s">
+        <v>1392</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D365" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
MOSIP-42622: Added new FTM, APIKEY, SBI and Weekly summary templates
Signed-off-by: Swetha K <swetha.k@technoforte.co.in>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/template_type.xlsx
+++ b/mosip_master/xlsx/template_type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2A89C4-95B5-421B-9706-6D277F1A82C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D493FBBA-311F-4FC6-980D-93205FF0EC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15252" uniqueCount="1455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15468" uniqueCount="1497">
   <si>
     <t>lang_code</t>
   </si>
@@ -6005,6 +6005,132 @@
   </si>
   <si>
     <t>வாராந்திர சுருக்க அறிவிப்புகளுக்கான தலைப்பு டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>FTM_CHIP_CERT_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for FTM chip certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle d'expiration du certificat de puce FTM</t>
+  </si>
+  <si>
+    <t>نموذج لانتهاء صلاحية شهادة شريحة FTM</t>
+  </si>
+  <si>
+    <t>FTM चिप प्रमाणपत्र समाप्ति के लिए टेम्पलेट</t>
+  </si>
+  <si>
+    <t>FTM ಚಿಪ್ ಪ್ರಮಾಣಪತ್ರದ ಮುಕ್ತಾಯದ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>FTM சிப் சான்றிதழ் காலாவதிக்கான டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>API_KEY_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for API key expiry</t>
+  </si>
+  <si>
+    <t>Modèle pour l'expiration de la clé API</t>
+  </si>
+  <si>
+    <t>قالب لانتهاء صلاحية مفتاح API</t>
+  </si>
+  <si>
+    <t>API कुंजी समाप्ति के लिए टेम्पलेट</t>
+  </si>
+  <si>
+    <t>API ಕೀ ಅವಧಿ ಮುಗಿಯುವ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>API விசை காலாவதிக்கான டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>SBI_EXPIRY_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Template for SBI expiry</t>
+  </si>
+  <si>
+    <t>Modèle pour l'expiration du SBI</t>
+  </si>
+  <si>
+    <t>نموذج لانتهاء صلاحية SBI</t>
+  </si>
+  <si>
+    <t>एसबीआई समाप्ति के लिए टेम्पलेट</t>
+  </si>
+  <si>
+    <t>ಎಸ್‌ಬಿಐ ಅವಧಿ ಮುಗಿಯುವ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>எஸ்பிஐ காலாவதிக்கான டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>FTM_CHIP_CERT_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for FTM chip certificate expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du certificat de puce FTM</t>
+  </si>
+  <si>
+    <t>نموذج موضوعي لانتهاء صلاحية شهادة شريحة FTM</t>
+  </si>
+  <si>
+    <t>एफटीएम चिप प्रमाणपत्र समाप्ति के लिए विषय टेम्पलेट</t>
+  </si>
+  <si>
+    <t>FTM ಚಿಪ್ ಪ್ರಮಾಣಪತ್ರದ ಮುಕ್ತಾಯದ ವಿಷಯ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>FTM சிப் சான்றிதழ் காலாவதிக்கான பொருள் டெம்ப்ளேட்.</t>
+  </si>
+  <si>
+    <t>API_KEY_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for API key expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration de la clé API</t>
+  </si>
+  <si>
+    <t>قالب موضوع لانتهاء صلاحية مفتاح API</t>
+  </si>
+  <si>
+    <t>API कुंजी समाप्ति के लिए विषय टेम्पलेट</t>
+  </si>
+  <si>
+    <t>API ಕೀ ಅವಧಿ ಮುಗಿಯುವ ವಿಷಯ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>API விசை காலாவதிக்கான பொருள் டெம்ப்ளேட்</t>
+  </si>
+  <si>
+    <t>SBI_EXPIRY_SUBJECT</t>
+  </si>
+  <si>
+    <t>Subject template for SBI expiry</t>
+  </si>
+  <si>
+    <t>Modèle de sujet pour l'expiration du SBI</t>
+  </si>
+  <si>
+    <t>نموذج موضوع لانتهاء صلاحية بنك SBI</t>
+  </si>
+  <si>
+    <t>एसबीआई समाप्ति के लिए विषय टेम्पलेट</t>
+  </si>
+  <si>
+    <t>SBI ಅವಧಿ ಮುಗಿಯುವ ವಿಷಯದ ಟೆಂಪ್ಲೇಟ್</t>
+  </si>
+  <si>
+    <t>எஸ்பிஐ காலாவதிக்கான பாட வார்ப்புரு</t>
   </si>
 </sst>
 </file>
@@ -6473,10 +6599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2542"/>
+  <dimension ref="A1:F2578"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2489" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2541" sqref="B2541"/>
+    <sheetView tabSelected="1" topLeftCell="A2539" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2572" sqref="F2572:F2578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15"/>
@@ -7047,7 +7173,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="29.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>291</v>
       </c>
@@ -7087,7 +7213,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="29.25">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>291</v>
       </c>
@@ -7127,7 +7253,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="29.25">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>291</v>
       </c>
@@ -7527,7 +7653,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="29.25">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>291</v>
       </c>
@@ -7547,7 +7673,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="29.25">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>291</v>
       </c>
@@ -7587,7 +7713,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="29.25">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>291</v>
       </c>
@@ -7607,7 +7733,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="30">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>291</v>
       </c>
@@ -7647,7 +7773,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="29.25">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>291</v>
       </c>
@@ -7667,7 +7793,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="29.25">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>291</v>
       </c>
@@ -7967,7 +8093,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="29.25">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>291</v>
       </c>
@@ -7987,7 +8113,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="29.25">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>291</v>
       </c>
@@ -8007,7 +8133,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="29.25">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>291</v>
       </c>
@@ -8107,7 +8233,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="29.25">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>291</v>
       </c>
@@ -8287,7 +8413,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="29.25">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>291</v>
       </c>
@@ -8407,7 +8533,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="30">
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>291</v>
       </c>
@@ -8647,7 +8773,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="29.25">
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>291</v>
       </c>
@@ -8707,7 +8833,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="29.25">
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>291</v>
       </c>
@@ -8887,7 +9013,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="30">
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>291</v>
       </c>
@@ -9367,7 +9493,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="30">
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
         <v>291</v>
       </c>
@@ -9427,7 +9553,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="29.25">
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
         <v>291</v>
       </c>
@@ -9487,7 +9613,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="30">
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>291</v>
       </c>
@@ -9547,7 +9673,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="29.25">
+    <row r="154" spans="1:6">
       <c r="A154" t="s">
         <v>291</v>
       </c>
@@ -9607,7 +9733,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="29.25">
+    <row r="157" spans="1:6">
       <c r="A157" t="s">
         <v>291</v>
       </c>
@@ -9667,7 +9793,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="29.25">
+    <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>291</v>
       </c>
@@ -9727,7 +9853,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="30">
+    <row r="163" spans="1:6">
       <c r="A163" t="s">
         <v>291</v>
       </c>
@@ -9787,7 +9913,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="29.25">
+    <row r="166" spans="1:6">
       <c r="A166" t="s">
         <v>291</v>
       </c>
@@ -9847,7 +9973,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="30">
+    <row r="169" spans="1:6">
       <c r="A169" t="s">
         <v>291</v>
       </c>
@@ -9907,7 +10033,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="43.5">
+    <row r="172" spans="1:6">
       <c r="A172" t="s">
         <v>291</v>
       </c>
@@ -9967,7 +10093,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="30">
+    <row r="175" spans="1:6">
       <c r="A175" t="s">
         <v>291</v>
       </c>
@@ -10027,7 +10153,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="29.25">
+    <row r="178" spans="1:6">
       <c r="A178" t="s">
         <v>291</v>
       </c>
@@ -10087,7 +10213,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="30">
+    <row r="181" spans="1:6">
       <c r="A181" t="s">
         <v>291</v>
       </c>
@@ -10147,7 +10273,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="29.25">
+    <row r="184" spans="1:6">
       <c r="A184" t="s">
         <v>291</v>
       </c>
@@ -10207,7 +10333,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="44.25">
+    <row r="187" spans="1:6">
       <c r="A187" t="s">
         <v>291</v>
       </c>
@@ -10267,7 +10393,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="29.25">
+    <row r="190" spans="1:6">
       <c r="A190" t="s">
         <v>291</v>
       </c>
@@ -10327,7 +10453,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="29.25">
+    <row r="193" spans="1:6">
       <c r="A193" t="s">
         <v>291</v>
       </c>
@@ -10387,7 +10513,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="29.25">
+    <row r="196" spans="1:6">
       <c r="A196" t="s">
         <v>291</v>
       </c>
@@ -10447,7 +10573,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="43.5">
+    <row r="199" spans="1:6">
       <c r="A199" t="s">
         <v>291</v>
       </c>
@@ -10507,7 +10633,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="43.5">
+    <row r="202" spans="1:6">
       <c r="A202" t="s">
         <v>291</v>
       </c>
@@ -10567,7 +10693,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="29.25">
+    <row r="205" spans="1:6">
       <c r="A205" t="s">
         <v>291</v>
       </c>
@@ -10627,7 +10753,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="43.5">
+    <row r="208" spans="1:6">
       <c r="A208" t="s">
         <v>291</v>
       </c>
@@ -11167,7 +11293,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="29.25">
+    <row r="235" spans="1:6">
       <c r="A235" t="s">
         <v>291</v>
       </c>
@@ -11227,7 +11353,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="29.25">
+    <row r="238" spans="1:6">
       <c r="A238" t="s">
         <v>291</v>
       </c>
@@ -11287,7 +11413,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="29.25">
+    <row r="241" spans="1:6">
       <c r="A241" t="s">
         <v>291</v>
       </c>
@@ -11347,7 +11473,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="29.25">
+    <row r="244" spans="1:6">
       <c r="A244" t="s">
         <v>291</v>
       </c>
@@ -11647,7 +11773,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="29.25">
+    <row r="259" spans="1:6">
       <c r="A259" t="s">
         <v>291</v>
       </c>
@@ -11727,7 +11853,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="30">
+    <row r="263" spans="1:6">
       <c r="A263" t="s">
         <v>297</v>
       </c>
@@ -11747,7 +11873,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="30">
+    <row r="264" spans="1:6">
       <c r="A264" t="s">
         <v>297</v>
       </c>
@@ -11767,7 +11893,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="265" spans="1:6" ht="30">
+    <row r="265" spans="1:6">
       <c r="A265" t="s">
         <v>297</v>
       </c>
@@ -11787,7 +11913,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="266" spans="1:6" ht="30">
+    <row r="266" spans="1:6">
       <c r="A266" t="s">
         <v>297</v>
       </c>
@@ -11807,7 +11933,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="267" spans="1:6" ht="30">
+    <row r="267" spans="1:6">
       <c r="A267" t="s">
         <v>297</v>
       </c>
@@ -11827,7 +11953,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="268" spans="1:6" ht="30">
+    <row r="268" spans="1:6">
       <c r="A268" t="s">
         <v>297</v>
       </c>
@@ -11847,7 +11973,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="269" spans="1:6" ht="30">
+    <row r="269" spans="1:6">
       <c r="A269" t="s">
         <v>297</v>
       </c>
@@ -11867,7 +11993,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="270" spans="1:6" ht="30">
+    <row r="270" spans="1:6">
       <c r="A270" t="s">
         <v>297</v>
       </c>
@@ -11887,7 +12013,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="271" spans="1:6" ht="30">
+    <row r="271" spans="1:6">
       <c r="A271" t="s">
         <v>297</v>
       </c>
@@ -11907,7 +12033,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="272" spans="1:6" ht="45">
+    <row r="272" spans="1:6">
       <c r="A272" t="s">
         <v>297</v>
       </c>
@@ -11927,7 +12053,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="273" spans="1:6" ht="45">
+    <row r="273" spans="1:6">
       <c r="A273" t="s">
         <v>297</v>
       </c>
@@ -11947,7 +12073,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="274" spans="1:6" ht="45">
+    <row r="274" spans="1:6">
       <c r="A274" t="s">
         <v>297</v>
       </c>
@@ -11967,7 +12093,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="275" spans="1:6" ht="45">
+    <row r="275" spans="1:6">
       <c r="A275" t="s">
         <v>297</v>
       </c>
@@ -11987,7 +12113,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="276" spans="1:6" ht="30">
+    <row r="276" spans="1:6">
       <c r="A276" t="s">
         <v>297</v>
       </c>
@@ -12007,7 +12133,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="277" spans="1:6" ht="30">
+    <row r="277" spans="1:6">
       <c r="A277" t="s">
         <v>297</v>
       </c>
@@ -12027,7 +12153,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="278" spans="1:6" ht="30">
+    <row r="278" spans="1:6">
       <c r="A278" t="s">
         <v>297</v>
       </c>
@@ -12067,7 +12193,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="280" spans="1:6" ht="60">
+    <row r="280" spans="1:6">
       <c r="A280" t="s">
         <v>297</v>
       </c>
@@ -12087,7 +12213,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="281" spans="1:6" ht="60">
+    <row r="281" spans="1:6">
       <c r="A281" t="s">
         <v>297</v>
       </c>
@@ -12107,7 +12233,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="282" spans="1:6" ht="45">
+    <row r="282" spans="1:6">
       <c r="A282" t="s">
         <v>297</v>
       </c>
@@ -12127,7 +12253,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="283" spans="1:6" ht="30">
+    <row r="283" spans="1:6">
       <c r="A283" t="s">
         <v>297</v>
       </c>
@@ -12147,7 +12273,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="284" spans="1:6" ht="30">
+    <row r="284" spans="1:6">
       <c r="A284" t="s">
         <v>297</v>
       </c>
@@ -12167,7 +12293,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="285" spans="1:6" ht="30">
+    <row r="285" spans="1:6">
       <c r="A285" t="s">
         <v>297</v>
       </c>
@@ -12187,7 +12313,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="286" spans="1:6" ht="30">
+    <row r="286" spans="1:6">
       <c r="A286" t="s">
         <v>297</v>
       </c>
@@ -12227,7 +12353,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="288" spans="1:6" ht="30">
+    <row r="288" spans="1:6">
       <c r="A288" t="s">
         <v>297</v>
       </c>
@@ -12247,7 +12373,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="289" spans="1:6" ht="30">
+    <row r="289" spans="1:6">
       <c r="A289" t="s">
         <v>297</v>
       </c>
@@ -12287,7 +12413,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="291" spans="1:6" ht="45">
+    <row r="291" spans="1:6">
       <c r="A291" t="s">
         <v>297</v>
       </c>
@@ -12307,7 +12433,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="292" spans="1:6" ht="30">
+    <row r="292" spans="1:6">
       <c r="A292" t="s">
         <v>297</v>
       </c>
@@ -12327,7 +12453,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="293" spans="1:6" ht="45">
+    <row r="293" spans="1:6">
       <c r="A293" t="s">
         <v>297</v>
       </c>
@@ -12347,7 +12473,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="294" spans="1:6" ht="45">
+    <row r="294" spans="1:6">
       <c r="A294" t="s">
         <v>297</v>
       </c>
@@ -12407,7 +12533,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="297" spans="1:6" ht="30">
+    <row r="297" spans="1:6">
       <c r="A297" t="s">
         <v>297</v>
       </c>
@@ -12427,7 +12553,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="298" spans="1:6" ht="30">
+    <row r="298" spans="1:6">
       <c r="A298" t="s">
         <v>297</v>
       </c>
@@ -12447,7 +12573,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="299" spans="1:6" ht="30">
+    <row r="299" spans="1:6">
       <c r="A299" t="s">
         <v>297</v>
       </c>
@@ -12467,7 +12593,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="300" spans="1:6" ht="30">
+    <row r="300" spans="1:6">
       <c r="A300" t="s">
         <v>297</v>
       </c>
@@ -12487,7 +12613,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="301" spans="1:6" ht="30">
+    <row r="301" spans="1:6">
       <c r="A301" t="s">
         <v>297</v>
       </c>
@@ -12507,7 +12633,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="302" spans="1:6" ht="30">
+    <row r="302" spans="1:6">
       <c r="A302" t="s">
         <v>297</v>
       </c>
@@ -12627,7 +12753,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="308" spans="1:6" ht="45">
+    <row r="308" spans="1:6">
       <c r="A308" t="s">
         <v>297</v>
       </c>
@@ -12647,7 +12773,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="309" spans="1:6" ht="30">
+    <row r="309" spans="1:6">
       <c r="A309" t="s">
         <v>297</v>
       </c>
@@ -12667,7 +12793,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="310" spans="1:6" ht="30">
+    <row r="310" spans="1:6">
       <c r="A310" t="s">
         <v>297</v>
       </c>
@@ -12687,7 +12813,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="311" spans="1:6" ht="45">
+    <row r="311" spans="1:6">
       <c r="A311" t="s">
         <v>297</v>
       </c>
@@ -12707,7 +12833,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="312" spans="1:6" ht="45">
+    <row r="312" spans="1:6">
       <c r="A312" t="s">
         <v>297</v>
       </c>
@@ -12727,7 +12853,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="313" spans="1:6" ht="60">
+    <row r="313" spans="1:6">
       <c r="A313" t="s">
         <v>297</v>
       </c>
@@ -12747,7 +12873,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="314" spans="1:6" ht="60">
+    <row r="314" spans="1:6">
       <c r="A314" t="s">
         <v>297</v>
       </c>
@@ -12767,7 +12893,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="315" spans="1:6" ht="45">
+    <row r="315" spans="1:6">
       <c r="A315" t="s">
         <v>297</v>
       </c>
@@ -12787,7 +12913,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="316" spans="1:6" ht="45">
+    <row r="316" spans="1:6">
       <c r="A316" t="s">
         <v>297</v>
       </c>
@@ -12807,7 +12933,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="317" spans="1:6" ht="60">
+    <row r="317" spans="1:6">
       <c r="A317" t="s">
         <v>297</v>
       </c>
@@ -12827,7 +12953,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="318" spans="1:6" ht="45">
+    <row r="318" spans="1:6">
       <c r="A318" t="s">
         <v>297</v>
       </c>
@@ -12847,7 +12973,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="319" spans="1:6" ht="60">
+    <row r="319" spans="1:6">
       <c r="A319" t="s">
         <v>297</v>
       </c>
@@ -12887,7 +13013,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="321" spans="1:6" ht="60">
+    <row r="321" spans="1:6">
       <c r="A321" t="s">
         <v>297</v>
       </c>
@@ -12907,7 +13033,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="322" spans="1:6" ht="60">
+    <row r="322" spans="1:6">
       <c r="A322" t="s">
         <v>297</v>
       </c>
@@ -12927,7 +13053,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="323" spans="1:6" ht="60">
+    <row r="323" spans="1:6">
       <c r="A323" t="s">
         <v>297</v>
       </c>
@@ -12947,7 +13073,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="324" spans="1:6" ht="45">
+    <row r="324" spans="1:6">
       <c r="A324" t="s">
         <v>297</v>
       </c>
@@ -12967,7 +13093,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="325" spans="1:6" ht="45">
+    <row r="325" spans="1:6">
       <c r="A325" t="s">
         <v>297</v>
       </c>
@@ -12987,7 +13113,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="326" spans="1:6" ht="60">
+    <row r="326" spans="1:6">
       <c r="A326" t="s">
         <v>297</v>
       </c>
@@ -13007,7 +13133,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="327" spans="1:6" ht="45">
+    <row r="327" spans="1:6">
       <c r="A327" t="s">
         <v>297</v>
       </c>
@@ -13027,7 +13153,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="60">
+    <row r="328" spans="1:6" ht="30">
       <c r="A328" t="s">
         <v>297</v>
       </c>
@@ -13047,7 +13173,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="329" spans="1:6" ht="60">
+    <row r="329" spans="1:6">
       <c r="A329" t="s">
         <v>297</v>
       </c>
@@ -13067,7 +13193,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="330" spans="1:6" ht="60">
+    <row r="330" spans="1:6">
       <c r="A330" t="s">
         <v>297</v>
       </c>
@@ -13087,7 +13213,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="331" spans="1:6" ht="45">
+    <row r="331" spans="1:6">
       <c r="A331" t="s">
         <v>297</v>
       </c>
@@ -13107,7 +13233,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="332" spans="1:6" ht="30">
+    <row r="332" spans="1:6">
       <c r="A332" t="s">
         <v>297</v>
       </c>
@@ -13127,7 +13253,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="333" spans="1:6" ht="45">
+    <row r="333" spans="1:6">
       <c r="A333" t="s">
         <v>297</v>
       </c>
@@ -13147,7 +13273,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="334" spans="1:6" ht="30">
+    <row r="334" spans="1:6">
       <c r="A334" t="s">
         <v>297</v>
       </c>
@@ -13167,7 +13293,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="335" spans="1:6" ht="30">
+    <row r="335" spans="1:6">
       <c r="A335" t="s">
         <v>297</v>
       </c>
@@ -13187,7 +13313,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="336" spans="1:6" ht="30">
+    <row r="336" spans="1:6">
       <c r="A336" t="s">
         <v>297</v>
       </c>
@@ -13207,7 +13333,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="337" spans="1:6" ht="30">
+    <row r="337" spans="1:6">
       <c r="A337" t="s">
         <v>297</v>
       </c>
@@ -13407,7 +13533,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="347" spans="1:6" ht="30">
+    <row r="347" spans="1:6">
       <c r="A347" t="s">
         <v>297</v>
       </c>
@@ -13507,7 +13633,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="352" spans="1:6" ht="30">
+    <row r="352" spans="1:6">
       <c r="A352" t="s">
         <v>298</v>
       </c>
@@ -13527,7 +13653,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="353" spans="1:6" ht="30">
+    <row r="353" spans="1:6">
       <c r="A353" t="s">
         <v>298</v>
       </c>
@@ -13547,7 +13673,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="354" spans="1:6" ht="30">
+    <row r="354" spans="1:6">
       <c r="A354" t="s">
         <v>298</v>
       </c>
@@ -13567,7 +13693,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="355" spans="1:6" ht="30">
+    <row r="355" spans="1:6">
       <c r="A355" t="s">
         <v>298</v>
       </c>
@@ -13587,7 +13713,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="356" spans="1:6" ht="30">
+    <row r="356" spans="1:6">
       <c r="A356" t="s">
         <v>298</v>
       </c>
@@ -13627,7 +13753,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="358" spans="1:6" ht="30">
+    <row r="358" spans="1:6">
       <c r="A358" t="s">
         <v>298</v>
       </c>
@@ -13647,7 +13773,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="359" spans="1:6" ht="30">
+    <row r="359" spans="1:6">
       <c r="A359" t="s">
         <v>298</v>
       </c>
@@ -13667,7 +13793,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="360" spans="1:6" ht="30">
+    <row r="360" spans="1:6">
       <c r="A360" t="s">
         <v>298</v>
       </c>
@@ -13687,7 +13813,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="361" spans="1:6" ht="30">
+    <row r="361" spans="1:6">
       <c r="A361" t="s">
         <v>298</v>
       </c>
@@ -13707,7 +13833,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="362" spans="1:6" ht="30">
+    <row r="362" spans="1:6">
       <c r="A362" t="s">
         <v>298</v>
       </c>
@@ -13727,7 +13853,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="363" spans="1:6" ht="30">
+    <row r="363" spans="1:6">
       <c r="A363" t="s">
         <v>298</v>
       </c>
@@ -13747,7 +13873,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="364" spans="1:6" ht="30">
+    <row r="364" spans="1:6">
       <c r="A364" t="s">
         <v>298</v>
       </c>
@@ -13767,7 +13893,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="365" spans="1:6" ht="30">
+    <row r="365" spans="1:6">
       <c r="A365" t="s">
         <v>298</v>
       </c>
@@ -13787,7 +13913,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="366" spans="1:6" ht="30">
+    <row r="366" spans="1:6">
       <c r="A366" t="s">
         <v>298</v>
       </c>
@@ -13807,7 +13933,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="367" spans="1:6" ht="30">
+    <row r="367" spans="1:6">
       <c r="A367" t="s">
         <v>298</v>
       </c>
@@ -13827,7 +13953,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="368" spans="1:6" ht="30">
+    <row r="368" spans="1:6">
       <c r="A368" t="s">
         <v>298</v>
       </c>
@@ -13847,7 +13973,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="369" spans="1:6" ht="30">
+    <row r="369" spans="1:6">
       <c r="A369" t="s">
         <v>298</v>
       </c>
@@ -13867,7 +13993,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="370" spans="1:6" ht="30">
+    <row r="370" spans="1:6">
       <c r="A370" t="s">
         <v>298</v>
       </c>
@@ -13887,7 +14013,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="371" spans="1:6" ht="30">
+    <row r="371" spans="1:6">
       <c r="A371" t="s">
         <v>298</v>
       </c>
@@ -13907,7 +14033,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="372" spans="1:6" ht="30">
+    <row r="372" spans="1:6">
       <c r="A372" t="s">
         <v>298</v>
       </c>
@@ -13927,7 +14053,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="373" spans="1:6" ht="30">
+    <row r="373" spans="1:6">
       <c r="A373" t="s">
         <v>298</v>
       </c>
@@ -13947,7 +14073,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="374" spans="1:6" ht="30">
+    <row r="374" spans="1:6">
       <c r="A374" t="s">
         <v>298</v>
       </c>
@@ -13967,7 +14093,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="375" spans="1:6" ht="30">
+    <row r="375" spans="1:6">
       <c r="A375" t="s">
         <v>298</v>
       </c>
@@ -13987,7 +14113,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="376" spans="1:6" ht="30">
+    <row r="376" spans="1:6">
       <c r="A376" t="s">
         <v>298</v>
       </c>
@@ -14007,7 +14133,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="377" spans="1:6" ht="30">
+    <row r="377" spans="1:6">
       <c r="A377" t="s">
         <v>298</v>
       </c>
@@ -14027,7 +14153,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="378" spans="1:6" ht="30">
+    <row r="378" spans="1:6">
       <c r="A378" t="s">
         <v>298</v>
       </c>
@@ -14067,7 +14193,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="380" spans="1:6" ht="30">
+    <row r="380" spans="1:6">
       <c r="A380" t="s">
         <v>298</v>
       </c>
@@ -14087,7 +14213,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="381" spans="1:6" ht="30">
+    <row r="381" spans="1:6">
       <c r="A381" t="s">
         <v>298</v>
       </c>
@@ -14107,7 +14233,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="382" spans="1:6" ht="30">
+    <row r="382" spans="1:6">
       <c r="A382" t="s">
         <v>298</v>
       </c>
@@ -14127,7 +14253,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="383" spans="1:6" ht="30">
+    <row r="383" spans="1:6">
       <c r="A383" t="s">
         <v>298</v>
       </c>
@@ -14207,7 +14333,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="387" spans="1:6" ht="30">
+    <row r="387" spans="1:6">
       <c r="A387" t="s">
         <v>298</v>
       </c>
@@ -14227,7 +14353,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="388" spans="1:6" ht="30">
+    <row r="388" spans="1:6">
       <c r="A388" t="s">
         <v>298</v>
       </c>
@@ -14247,7 +14373,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="389" spans="1:6" ht="30">
+    <row r="389" spans="1:6">
       <c r="A389" t="s">
         <v>298</v>
       </c>
@@ -14267,7 +14393,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="390" spans="1:6" ht="30">
+    <row r="390" spans="1:6">
       <c r="A390" t="s">
         <v>298</v>
       </c>
@@ -14287,7 +14413,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="391" spans="1:6" ht="30">
+    <row r="391" spans="1:6">
       <c r="A391" t="s">
         <v>298</v>
       </c>
@@ -14407,7 +14533,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="397" spans="1:6" ht="30">
+    <row r="397" spans="1:6">
       <c r="A397" t="s">
         <v>298</v>
       </c>
@@ -14427,7 +14553,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="398" spans="1:6" ht="30">
+    <row r="398" spans="1:6">
       <c r="A398" t="s">
         <v>298</v>
       </c>
@@ -14447,7 +14573,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="399" spans="1:6" ht="30">
+    <row r="399" spans="1:6">
       <c r="A399" t="s">
         <v>298</v>
       </c>
@@ -14467,7 +14593,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="400" spans="1:6" ht="30">
+    <row r="400" spans="1:6">
       <c r="A400" t="s">
         <v>298</v>
       </c>
@@ -14487,7 +14613,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="401" spans="1:6" ht="30">
+    <row r="401" spans="1:6">
       <c r="A401" t="s">
         <v>298</v>
       </c>
@@ -14507,7 +14633,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="402" spans="1:6" ht="30">
+    <row r="402" spans="1:6">
       <c r="A402" t="s">
         <v>298</v>
       </c>
@@ -14527,7 +14653,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="403" spans="1:6" ht="30">
+    <row r="403" spans="1:6">
       <c r="A403" t="s">
         <v>298</v>
       </c>
@@ -14547,7 +14673,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="404" spans="1:6" ht="30">
+    <row r="404" spans="1:6">
       <c r="A404" t="s">
         <v>298</v>
       </c>
@@ -14567,7 +14693,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="405" spans="1:6" ht="30">
+    <row r="405" spans="1:6">
       <c r="A405" t="s">
         <v>298</v>
       </c>
@@ -14587,7 +14713,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="406" spans="1:6" ht="30">
+    <row r="406" spans="1:6">
       <c r="A406" t="s">
         <v>298</v>
       </c>
@@ -14607,7 +14733,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="407" spans="1:6" ht="30">
+    <row r="407" spans="1:6">
       <c r="A407" t="s">
         <v>298</v>
       </c>
@@ -14627,7 +14753,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="408" spans="1:6" ht="45">
+    <row r="408" spans="1:6">
       <c r="A408" t="s">
         <v>298</v>
       </c>
@@ -14647,7 +14773,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="409" spans="1:6" ht="30">
+    <row r="409" spans="1:6">
       <c r="A409" t="s">
         <v>298</v>
       </c>
@@ -14667,7 +14793,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="410" spans="1:6" ht="30">
+    <row r="410" spans="1:6">
       <c r="A410" t="s">
         <v>298</v>
       </c>
@@ -14687,7 +14813,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="411" spans="1:6" ht="30">
+    <row r="411" spans="1:6">
       <c r="A411" t="s">
         <v>298</v>
       </c>
@@ -14707,7 +14833,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="412" spans="1:6" ht="30">
+    <row r="412" spans="1:6">
       <c r="A412" t="s">
         <v>298</v>
       </c>
@@ -14727,7 +14853,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="413" spans="1:6" ht="45">
+    <row r="413" spans="1:6">
       <c r="A413" t="s">
         <v>298</v>
       </c>
@@ -14747,7 +14873,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="414" spans="1:6" ht="30">
+    <row r="414" spans="1:6">
       <c r="A414" t="s">
         <v>298</v>
       </c>
@@ -14767,7 +14893,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="415" spans="1:6" ht="45">
+    <row r="415" spans="1:6">
       <c r="A415" t="s">
         <v>298</v>
       </c>
@@ -14787,7 +14913,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="416" spans="1:6" ht="30">
+    <row r="416" spans="1:6">
       <c r="A416" t="s">
         <v>298</v>
       </c>
@@ -14807,7 +14933,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="417" spans="1:6" ht="30">
+    <row r="417" spans="1:6">
       <c r="A417" t="s">
         <v>298</v>
       </c>
@@ -14827,7 +14953,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="418" spans="1:6" ht="30">
+    <row r="418" spans="1:6">
       <c r="A418" t="s">
         <v>298</v>
       </c>
@@ -14847,7 +14973,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="419" spans="1:6" ht="30">
+    <row r="419" spans="1:6">
       <c r="A419" t="s">
         <v>298</v>
       </c>
@@ -14867,7 +14993,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="420" spans="1:6" ht="30">
+    <row r="420" spans="1:6">
       <c r="A420" t="s">
         <v>298</v>
       </c>
@@ -14907,7 +15033,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="422" spans="1:6" ht="30">
+    <row r="422" spans="1:6">
       <c r="A422" t="s">
         <v>298</v>
       </c>
@@ -14967,7 +15093,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="425" spans="1:6" ht="30">
+    <row r="425" spans="1:6">
       <c r="A425" t="s">
         <v>298</v>
       </c>
@@ -14987,7 +15113,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="426" spans="1:6" ht="30">
+    <row r="426" spans="1:6">
       <c r="A426" t="s">
         <v>298</v>
       </c>
@@ -15087,7 +15213,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="431" spans="1:6" ht="45">
+    <row r="431" spans="1:6">
       <c r="A431" t="s">
         <v>298</v>
       </c>
@@ -15147,7 +15273,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="434" spans="1:6" ht="45">
+    <row r="434" spans="1:6">
       <c r="A434" t="s">
         <v>298</v>
       </c>
@@ -15167,7 +15293,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="435" spans="1:6" ht="30">
+    <row r="435" spans="1:6">
       <c r="A435" t="s">
         <v>298</v>
       </c>
@@ -15227,7 +15353,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="438" spans="1:6" ht="30">
+    <row r="438" spans="1:6">
       <c r="A438" t="s">
         <v>298</v>
       </c>
@@ -15247,7 +15373,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="439" spans="1:6" ht="45">
+    <row r="439" spans="1:6">
       <c r="A439" t="s">
         <v>298</v>
       </c>
@@ -15267,7 +15393,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="440" spans="1:6" ht="30">
+    <row r="440" spans="1:6">
       <c r="A440" t="s">
         <v>298</v>
       </c>
@@ -15287,7 +15413,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="441" spans="1:6" ht="45">
+    <row r="441" spans="1:6">
       <c r="A441" t="s">
         <v>299</v>
       </c>
@@ -15307,7 +15433,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="442" spans="1:6" ht="45">
+    <row r="442" spans="1:6">
       <c r="A442" t="s">
         <v>299</v>
       </c>
@@ -15327,7 +15453,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="443" spans="1:6" ht="45">
+    <row r="443" spans="1:6">
       <c r="A443" t="s">
         <v>299</v>
       </c>
@@ -15347,7 +15473,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="444" spans="1:6" ht="45">
+    <row r="444" spans="1:6">
       <c r="A444" t="s">
         <v>299</v>
       </c>
@@ -15367,7 +15493,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="445" spans="1:6" ht="45">
+    <row r="445" spans="1:6">
       <c r="A445" t="s">
         <v>299</v>
       </c>
@@ -15387,7 +15513,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="446" spans="1:6" ht="30">
+    <row r="446" spans="1:6">
       <c r="A446" t="s">
         <v>299</v>
       </c>
@@ -15407,7 +15533,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="447" spans="1:6" ht="60">
+    <row r="447" spans="1:6" ht="30">
       <c r="A447" t="s">
         <v>299</v>
       </c>
@@ -15427,7 +15553,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="448" spans="1:6" ht="45">
+    <row r="448" spans="1:6">
       <c r="A448" t="s">
         <v>299</v>
       </c>
@@ -15447,7 +15573,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="449" spans="1:6" ht="45">
+    <row r="449" spans="1:6">
       <c r="A449" t="s">
         <v>299</v>
       </c>
@@ -15467,7 +15593,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="450" spans="1:6" ht="60">
+    <row r="450" spans="1:6">
       <c r="A450" t="s">
         <v>299</v>
       </c>
@@ -15487,7 +15613,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="451" spans="1:6" ht="60">
+    <row r="451" spans="1:6">
       <c r="A451" t="s">
         <v>299</v>
       </c>
@@ -15507,7 +15633,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="452" spans="1:6" ht="60">
+    <row r="452" spans="1:6" ht="30">
       <c r="A452" t="s">
         <v>299</v>
       </c>
@@ -15527,7 +15653,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="453" spans="1:6" ht="60">
+    <row r="453" spans="1:6" ht="30">
       <c r="A453" t="s">
         <v>299</v>
       </c>
@@ -15547,7 +15673,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="454" spans="1:6" ht="45">
+    <row r="454" spans="1:6">
       <c r="A454" t="s">
         <v>299</v>
       </c>
@@ -15567,7 +15693,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="455" spans="1:6" ht="75">
+    <row r="455" spans="1:6" ht="30">
       <c r="A455" t="s">
         <v>299</v>
       </c>
@@ -15587,7 +15713,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="456" spans="1:6" ht="75">
+    <row r="456" spans="1:6" ht="30">
       <c r="A456" t="s">
         <v>299</v>
       </c>
@@ -15607,7 +15733,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="457" spans="1:6" ht="30">
+    <row r="457" spans="1:6">
       <c r="A457" t="s">
         <v>299</v>
       </c>
@@ -15627,7 +15753,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="458" spans="1:6" ht="75">
+    <row r="458" spans="1:6" ht="30">
       <c r="A458" t="s">
         <v>299</v>
       </c>
@@ -15647,7 +15773,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="459" spans="1:6" ht="75">
+    <row r="459" spans="1:6" ht="30">
       <c r="A459" t="s">
         <v>299</v>
       </c>
@@ -15667,7 +15793,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="460" spans="1:6" ht="60">
+    <row r="460" spans="1:6">
       <c r="A460" t="s">
         <v>299</v>
       </c>
@@ -15687,7 +15813,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="461" spans="1:6" ht="45">
+    <row r="461" spans="1:6">
       <c r="A461" t="s">
         <v>299</v>
       </c>
@@ -15707,7 +15833,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="462" spans="1:6" ht="45">
+    <row r="462" spans="1:6">
       <c r="A462" t="s">
         <v>299</v>
       </c>
@@ -15727,7 +15853,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="463" spans="1:6" ht="45">
+    <row r="463" spans="1:6">
       <c r="A463" t="s">
         <v>299</v>
       </c>
@@ -15747,7 +15873,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="464" spans="1:6" ht="45">
+    <row r="464" spans="1:6">
       <c r="A464" t="s">
         <v>299</v>
       </c>
@@ -15767,7 +15893,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="465" spans="1:6" ht="30">
+    <row r="465" spans="1:6">
       <c r="A465" t="s">
         <v>299</v>
       </c>
@@ -15787,7 +15913,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="466" spans="1:6" ht="60">
+    <row r="466" spans="1:6" ht="30">
       <c r="A466" t="s">
         <v>299</v>
       </c>
@@ -15807,7 +15933,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="467" spans="1:6" ht="30">
+    <row r="467" spans="1:6">
       <c r="A467" s="5" t="s">
         <v>299</v>
       </c>
@@ -15827,7 +15953,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="468" spans="1:6" ht="30">
+    <row r="468" spans="1:6">
       <c r="A468" t="s">
         <v>299</v>
       </c>
@@ -15847,7 +15973,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="469" spans="1:6" ht="45">
+    <row r="469" spans="1:6">
       <c r="A469" t="s">
         <v>299</v>
       </c>
@@ -15867,7 +15993,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="470" spans="1:6" ht="60">
+    <row r="470" spans="1:6">
       <c r="A470" t="s">
         <v>299</v>
       </c>
@@ -15887,7 +16013,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="471" spans="1:6" ht="60">
+    <row r="471" spans="1:6" ht="30">
       <c r="A471" t="s">
         <v>299</v>
       </c>
@@ -15967,7 +16093,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="475" spans="1:6" ht="45">
+    <row r="475" spans="1:6">
       <c r="A475" t="s">
         <v>299</v>
       </c>
@@ -15987,7 +16113,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="476" spans="1:6" ht="45">
+    <row r="476" spans="1:6">
       <c r="A476" t="s">
         <v>299</v>
       </c>
@@ -16007,7 +16133,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="477" spans="1:6" ht="45">
+    <row r="477" spans="1:6">
       <c r="A477" t="s">
         <v>299</v>
       </c>
@@ -16027,7 +16153,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="478" spans="1:6" ht="45">
+    <row r="478" spans="1:6">
       <c r="A478" t="s">
         <v>299</v>
       </c>
@@ -16047,7 +16173,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="479" spans="1:6" ht="45">
+    <row r="479" spans="1:6">
       <c r="A479" t="s">
         <v>299</v>
       </c>
@@ -16067,7 +16193,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="480" spans="1:6" ht="30">
+    <row r="480" spans="1:6">
       <c r="A480" t="s">
         <v>299</v>
       </c>
@@ -16087,7 +16213,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="481" spans="1:6" ht="30">
+    <row r="481" spans="1:6">
       <c r="A481" t="s">
         <v>299</v>
       </c>
@@ -16187,7 +16313,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="486" spans="1:6" ht="45">
+    <row r="486" spans="1:6">
       <c r="A486" t="s">
         <v>299</v>
       </c>
@@ -16227,7 +16353,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="488" spans="1:6" ht="45">
+    <row r="488" spans="1:6">
       <c r="A488" t="s">
         <v>299</v>
       </c>
@@ -16247,7 +16373,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="489" spans="1:6" ht="60">
+    <row r="489" spans="1:6">
       <c r="A489" t="s">
         <v>299</v>
       </c>
@@ -16267,7 +16393,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="490" spans="1:6" ht="45">
+    <row r="490" spans="1:6">
       <c r="A490" t="s">
         <v>299</v>
       </c>
@@ -16287,7 +16413,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="491" spans="1:6" ht="75">
+    <row r="491" spans="1:6" ht="30">
       <c r="A491" t="s">
         <v>299</v>
       </c>
@@ -16307,7 +16433,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="492" spans="1:6" ht="60">
+    <row r="492" spans="1:6">
       <c r="A492" t="s">
         <v>299</v>
       </c>
@@ -16327,7 +16453,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="493" spans="1:6" ht="60">
+    <row r="493" spans="1:6">
       <c r="A493" t="s">
         <v>299</v>
       </c>
@@ -16347,7 +16473,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="494" spans="1:6" ht="75">
+    <row r="494" spans="1:6" ht="30">
       <c r="A494" t="s">
         <v>299</v>
       </c>
@@ -16367,7 +16493,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="495" spans="1:6" ht="90">
+    <row r="495" spans="1:6" ht="30">
       <c r="A495" t="s">
         <v>299</v>
       </c>
@@ -16387,7 +16513,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="496" spans="1:6" ht="75">
+    <row r="496" spans="1:6" ht="30">
       <c r="A496" t="s">
         <v>299</v>
       </c>
@@ -16407,7 +16533,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="497" spans="1:6" ht="75">
+    <row r="497" spans="1:6" ht="30">
       <c r="A497" t="s">
         <v>299</v>
       </c>
@@ -16427,7 +16553,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="498" spans="1:6" ht="75">
+    <row r="498" spans="1:6" ht="30">
       <c r="A498" t="s">
         <v>299</v>
       </c>
@@ -16447,7 +16573,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="499" spans="1:6" ht="75">
+    <row r="499" spans="1:6" ht="30">
       <c r="A499" t="s">
         <v>299</v>
       </c>
@@ -16467,7 +16593,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="500" spans="1:6" ht="60">
+    <row r="500" spans="1:6" ht="30">
       <c r="A500" t="s">
         <v>299</v>
       </c>
@@ -16487,7 +16613,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="501" spans="1:6" ht="75">
+    <row r="501" spans="1:6" ht="30">
       <c r="A501" t="s">
         <v>299</v>
       </c>
@@ -16507,7 +16633,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="502" spans="1:6" ht="75">
+    <row r="502" spans="1:6" ht="30">
       <c r="A502" t="s">
         <v>299</v>
       </c>
@@ -16527,7 +16653,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="503" spans="1:6" ht="60">
+    <row r="503" spans="1:6">
       <c r="A503" t="s">
         <v>299</v>
       </c>
@@ -16547,7 +16673,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="504" spans="1:6" ht="90">
+    <row r="504" spans="1:6" ht="30">
       <c r="A504" t="s">
         <v>299</v>
       </c>
@@ -16567,7 +16693,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="505" spans="1:6" ht="60">
+    <row r="505" spans="1:6" ht="30">
       <c r="A505" t="s">
         <v>299</v>
       </c>
@@ -16587,7 +16713,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="506" spans="1:6" ht="75">
+    <row r="506" spans="1:6" ht="30">
       <c r="A506" t="s">
         <v>299</v>
       </c>
@@ -16607,7 +16733,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="507" spans="1:6" ht="90">
+    <row r="507" spans="1:6" ht="30">
       <c r="A507" t="s">
         <v>299</v>
       </c>
@@ -16627,7 +16753,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="508" spans="1:6" ht="90">
+    <row r="508" spans="1:6" ht="30">
       <c r="A508" t="s">
         <v>299</v>
       </c>
@@ -16647,7 +16773,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="509" spans="1:6" ht="75">
+    <row r="509" spans="1:6" ht="30">
       <c r="A509" t="s">
         <v>299</v>
       </c>
@@ -16667,7 +16793,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="510" spans="1:6" ht="30">
+    <row r="510" spans="1:6">
       <c r="A510" t="s">
         <v>299</v>
       </c>
@@ -16687,7 +16813,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="511" spans="1:6" ht="30">
+    <row r="511" spans="1:6">
       <c r="A511" t="s">
         <v>299</v>
       </c>
@@ -16707,7 +16833,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="512" spans="1:6" ht="30">
+    <row r="512" spans="1:6">
       <c r="A512" t="s">
         <v>299</v>
       </c>
@@ -16727,7 +16853,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="513" spans="1:6" ht="30">
+    <row r="513" spans="1:6">
       <c r="A513" t="s">
         <v>299</v>
       </c>
@@ -16747,7 +16873,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="514" spans="1:6" ht="30">
+    <row r="514" spans="1:6">
       <c r="A514" t="s">
         <v>299</v>
       </c>
@@ -16767,7 +16893,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="515" spans="1:6" ht="30">
+    <row r="515" spans="1:6">
       <c r="A515" t="s">
         <v>299</v>
       </c>
@@ -57324,6 +57450,726 @@
         <v>1391</v>
       </c>
       <c r="F2542" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:6">
+      <c r="A2543" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2543" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C2543" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D2543" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2543" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2543" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:6">
+      <c r="A2544" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2544" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C2544" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D2544" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2544" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2544" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2545" spans="1:6">
+      <c r="A2545" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2545" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C2545" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D2545" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2545" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2545" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:6">
+      <c r="A2546" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2546" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C2546" t="s">
+        <v>1459</v>
+      </c>
+      <c r="D2546" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2546" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2546" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:6">
+      <c r="A2547" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2547" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C2547" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D2547" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2547" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2547" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2548" spans="1:6">
+      <c r="A2548" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2548" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C2548" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D2548" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2548" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2548" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2549" spans="1:6">
+      <c r="A2549" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2549" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C2549" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D2549" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2549" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2549" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2550" spans="1:6">
+      <c r="A2550" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2550" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C2550" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D2550" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2550" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2550" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2551" spans="1:6">
+      <c r="A2551" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2551" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C2551" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D2551" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2551" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2551" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2552" spans="1:6">
+      <c r="A2552" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2552" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C2552" t="s">
+        <v>1466</v>
+      </c>
+      <c r="D2552" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2552" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2552" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2553" spans="1:6">
+      <c r="A2553" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2553" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C2553" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D2553" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2553" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2553" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2554" spans="1:6">
+      <c r="A2554" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2554" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C2554" t="s">
+        <v>1468</v>
+      </c>
+      <c r="D2554" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2554" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2554" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2555" spans="1:6">
+      <c r="A2555" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2555" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C2555" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D2555" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2555" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2555" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2556" spans="1:6">
+      <c r="A2556" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2556" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C2556" t="s">
+        <v>1471</v>
+      </c>
+      <c r="D2556" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2556" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2556" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:6">
+      <c r="A2557" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2557" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C2557" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D2557" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2557" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2557" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2558" spans="1:6">
+      <c r="A2558" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2558" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C2558" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D2558" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2558" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2558" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:6">
+      <c r="A2559" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2559" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C2559" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D2559" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2559" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2559" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:6">
+      <c r="A2560" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2560" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C2560" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D2560" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2560" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2560" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:6">
+      <c r="A2561" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2561" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C2561" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D2561" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2561" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2561" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:6">
+      <c r="A2562" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2562" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C2562" t="s">
+        <v>1478</v>
+      </c>
+      <c r="D2562" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2562" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2562" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:6">
+      <c r="A2563" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2563" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C2563" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D2563" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2563" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2563" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:6">
+      <c r="A2564" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2564" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C2564" t="s">
+        <v>1480</v>
+      </c>
+      <c r="D2564" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2564" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2564" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:6">
+      <c r="A2565" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2565" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C2565" t="s">
+        <v>1481</v>
+      </c>
+      <c r="D2565" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2565" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2565" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:6">
+      <c r="A2566" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2566" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C2566" t="s">
+        <v>1482</v>
+      </c>
+      <c r="D2566" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2566" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2566" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:6">
+      <c r="A2567" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2567" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C2567" t="s">
+        <v>1484</v>
+      </c>
+      <c r="D2567" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2567" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2567" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:6">
+      <c r="A2568" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2568" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C2568" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D2568" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2568" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2568" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2569" spans="1:6">
+      <c r="A2569" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2569" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C2569" t="s">
+        <v>1486</v>
+      </c>
+      <c r="D2569" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2569" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2569" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:6">
+      <c r="A2570" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2570" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C2570" t="s">
+        <v>1487</v>
+      </c>
+      <c r="D2570" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2570" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2570" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:6">
+      <c r="A2571" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2571" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C2571" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D2571" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2571" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2571" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:6">
+      <c r="A2572" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2572" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C2572" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D2572" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2572" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2572" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2573" spans="1:6">
+      <c r="A2573" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2573" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C2573" t="s">
+        <v>1491</v>
+      </c>
+      <c r="D2573" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2573" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2573" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:6">
+      <c r="A2574" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2574" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C2574" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D2574" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2574" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2574" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:6">
+      <c r="A2575" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2575" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C2575" t="s">
+        <v>1493</v>
+      </c>
+      <c r="D2575" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2575" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2575" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:6">
+      <c r="A2576" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2576" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C2576" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D2576" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2576" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2576" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:6">
+      <c r="A2577" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2577" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C2577" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D2577" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2577" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2577" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:6">
+      <c r="A2578" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2578" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C2578" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D2578" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2578" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F2578" t="s">
         <v>1392</v>
       </c>
     </row>

</xml_diff>